<commit_message>
Produce r-squared statistic giving the good of the fit.
</commit_message>
<xml_diff>
--- a/DATA/collate_cultivar_data/data/binned_kcp_data.xlsx
+++ b/DATA/collate_cultivar_data/data/binned_kcp_data.xlsx
@@ -440,7 +440,7 @@
         <v>182</v>
       </c>
       <c r="D2">
-        <v>0.4354402229893334</v>
+        <v>0.4997836293541847</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -454,7 +454,7 @@
         <v>183</v>
       </c>
       <c r="D3">
-        <v>0.4381425784996799</v>
+        <v>0.4997847696149227</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -468,7 +468,7 @@
         <v>184</v>
       </c>
       <c r="D4">
-        <v>0.4408264777897513</v>
+        <v>0.4998128481427201</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -482,7 +482,7 @@
         <v>185</v>
       </c>
       <c r="D5">
-        <v>0.4434919208595477</v>
+        <v>0.4998675690634674</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -496,7 +496,7 @@
         <v>186</v>
       </c>
       <c r="D6">
-        <v>0.4461389077090691</v>
+        <v>0.499948636503055</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -510,7 +510,7 @@
         <v>187</v>
       </c>
       <c r="D7">
-        <v>0.4487674383383154</v>
+        <v>0.5000557545873736</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -524,7 +524,7 @@
         <v>188</v>
       </c>
       <c r="D8">
-        <v>0.4513775127472868</v>
+        <v>0.5001886274423136</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -538,7 +538,7 @@
         <v>189</v>
       </c>
       <c r="D9">
-        <v>0.4539691309359831</v>
+        <v>0.5003469591937658</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -552,7 +552,7 @@
         <v>190</v>
       </c>
       <c r="D10">
-        <v>0.4565422929044043</v>
+        <v>0.5005304539676205</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -566,7 +566,7 @@
         <v>191</v>
       </c>
       <c r="D11">
-        <v>0.4590969986525506</v>
+        <v>0.5007388158897683</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -580,7 +580,7 @@
         <v>192</v>
       </c>
       <c r="D12">
-        <v>0.4616332481804218</v>
+        <v>0.5009717490860999</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -594,7 +594,7 @@
         <v>193</v>
       </c>
       <c r="D13">
-        <v>0.4641510414880181</v>
+        <v>0.5012289576825055</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -608,7 +608,7 @@
         <v>194</v>
       </c>
       <c r="D14">
-        <v>0.4666503785753393</v>
+        <v>0.5015101458048761</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -622,7 +622,7 @@
         <v>195</v>
       </c>
       <c r="D15">
-        <v>0.4691312594423854</v>
+        <v>0.5018150175791019</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -636,7 +636,7 @@
         <v>196</v>
       </c>
       <c r="D16">
-        <v>0.4715936840891565</v>
+        <v>0.5021432771310734</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -650,7 +650,7 @@
         <v>197</v>
       </c>
       <c r="D17">
-        <v>0.4740376525156527</v>
+        <v>0.5024946285866814</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -664,7 +664,7 @@
         <v>198</v>
       </c>
       <c r="D18">
-        <v>0.4764631647218737</v>
+        <v>0.5028687760718162</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -678,7 +678,7 @@
         <v>199</v>
       </c>
       <c r="D19">
-        <v>0.4788702207078198</v>
+        <v>0.5032654237123686</v>
       </c>
     </row>
     <row r="20" spans="1:4">
@@ -692,7 +692,7 @@
         <v>200</v>
       </c>
       <c r="D20">
-        <v>0.4812588204734908</v>
+        <v>0.5036842756342289</v>
       </c>
     </row>
     <row r="21" spans="1:4">
@@ -706,7 +706,7 @@
         <v>201</v>
       </c>
       <c r="D21">
-        <v>0.4836289640188868</v>
+        <v>0.5041250359632878</v>
       </c>
     </row>
     <row r="22" spans="1:4">
@@ -720,7 +720,7 @@
         <v>202</v>
       </c>
       <c r="D22">
-        <v>0.4859806513440078</v>
+        <v>0.5045874088254358</v>
       </c>
     </row>
     <row r="23" spans="1:4">
@@ -734,7 +734,7 @@
         <v>203</v>
       </c>
       <c r="D23">
-        <v>0.4883138824488538</v>
+        <v>0.5050710983465634</v>
       </c>
     </row>
     <row r="24" spans="1:4">
@@ -748,7 +748,7 @@
         <v>204</v>
       </c>
       <c r="D24">
-        <v>0.4906286573334247</v>
+        <v>0.5055758086525611</v>
       </c>
     </row>
     <row r="25" spans="1:4">
@@ -762,7 +762,7 @@
         <v>205</v>
       </c>
       <c r="D25">
-        <v>0.4929249759977206</v>
+        <v>0.5061012438693197</v>
       </c>
     </row>
     <row r="26" spans="1:4">
@@ -776,7 +776,7 @@
         <v>206</v>
       </c>
       <c r="D26">
-        <v>0.4952028384417415</v>
+        <v>0.5066471081227294</v>
       </c>
     </row>
     <row r="27" spans="1:4">
@@ -790,7 +790,7 @@
         <v>207</v>
       </c>
       <c r="D27">
-        <v>0.4974622446654874</v>
+        <v>0.5072131055386809</v>
       </c>
     </row>
     <row r="28" spans="1:4">
@@ -804,7 +804,7 @@
         <v>208</v>
       </c>
       <c r="D28">
-        <v>0.4997031946689582</v>
+        <v>0.5077989402430648</v>
       </c>
     </row>
     <row r="29" spans="1:4">
@@ -818,7 +818,7 @@
         <v>209</v>
       </c>
       <c r="D29">
-        <v>0.501925688452154</v>
+        <v>0.5084043163617715</v>
       </c>
     </row>
     <row r="30" spans="1:4">
@@ -832,7 +832,7 @@
         <v>210</v>
       </c>
       <c r="D30">
-        <v>0.5041297260150748</v>
+        <v>0.5090289380206917</v>
       </c>
     </row>
     <row r="31" spans="1:4">
@@ -846,7 +846,7 @@
         <v>211</v>
       </c>
       <c r="D31">
-        <v>0.5063153073577206</v>
+        <v>0.5096725093457158</v>
       </c>
     </row>
     <row r="32" spans="1:4">
@@ -860,7 +860,7 @@
         <v>212</v>
       </c>
       <c r="D32">
-        <v>0.5084824324800913</v>
+        <v>0.5103347344627345</v>
       </c>
     </row>
     <row r="33" spans="1:4">
@@ -874,7 +874,7 @@
         <v>213</v>
       </c>
       <c r="D33">
-        <v>0.510631101382187</v>
+        <v>0.5110153174976381</v>
       </c>
     </row>
     <row r="34" spans="1:4">
@@ -888,7 +888,7 @@
         <v>214</v>
       </c>
       <c r="D34">
-        <v>0.5127613140640077</v>
+        <v>0.5117139625763174</v>
       </c>
     </row>
     <row r="35" spans="1:4">
@@ -902,7 +902,7 @@
         <v>215</v>
       </c>
       <c r="D35">
-        <v>0.5148730705255533</v>
+        <v>0.5124303738246627</v>
       </c>
     </row>
     <row r="36" spans="1:4">
@@ -916,7 +916,7 @@
         <v>216</v>
       </c>
       <c r="D36">
-        <v>0.5169663707668241</v>
+        <v>0.5131642553685648</v>
       </c>
     </row>
     <row r="37" spans="1:4">
@@ -930,7 +930,7 @@
         <v>217</v>
       </c>
       <c r="D37">
-        <v>0.5190412147878196</v>
+        <v>0.5139153113339141</v>
       </c>
     </row>
     <row r="38" spans="1:4">
@@ -944,7 +944,7 @@
         <v>218</v>
       </c>
       <c r="D38">
-        <v>0.5210976025885402</v>
+        <v>0.5146832458466011</v>
       </c>
     </row>
     <row r="39" spans="1:4">
@@ -958,7 +958,7 @@
         <v>219</v>
       </c>
       <c r="D39">
-        <v>0.5231355341689858</v>
+        <v>0.5154677630325164</v>
       </c>
     </row>
     <row r="40" spans="1:4">
@@ -972,7 +972,7 @@
         <v>220</v>
       </c>
       <c r="D40">
-        <v>0.5251550095291563</v>
+        <v>0.5162685670175505</v>
       </c>
     </row>
     <row r="41" spans="1:4">
@@ -986,7 +986,7 @@
         <v>221</v>
       </c>
       <c r="D41">
-        <v>0.5271560286690519</v>
+        <v>0.5170853619275941</v>
       </c>
     </row>
     <row r="42" spans="1:4">
@@ -1000,7 +1000,7 @@
         <v>222</v>
       </c>
       <c r="D42">
-        <v>0.5291385915886724</v>
+        <v>0.5179178518885376</v>
       </c>
     </row>
     <row r="43" spans="1:4">
@@ -1014,7 +1014,7 @@
         <v>223</v>
       </c>
       <c r="D43">
-        <v>0.5311026982880178</v>
+        <v>0.5187657410262715</v>
       </c>
     </row>
     <row r="44" spans="1:4">
@@ -1028,7 +1028,7 @@
         <v>224</v>
       </c>
       <c r="D44">
-        <v>0.5330483487670883</v>
+        <v>0.5196287334666865</v>
       </c>
     </row>
     <row r="45" spans="1:4">
@@ -1042,7 +1042,7 @@
         <v>225</v>
       </c>
       <c r="D45">
-        <v>0.5349755430258837</v>
+        <v>0.5205065333356729</v>
       </c>
     </row>
     <row r="46" spans="1:4">
@@ -1056,7 +1056,7 @@
         <v>226</v>
       </c>
       <c r="D46">
-        <v>0.5368842810644041</v>
+        <v>0.5213988447591215</v>
       </c>
     </row>
     <row r="47" spans="1:4">
@@ -1070,7 +1070,7 @@
         <v>227</v>
       </c>
       <c r="D47">
-        <v>0.5387745628826495</v>
+        <v>0.5223053718629227</v>
       </c>
     </row>
     <row r="48" spans="1:4">
@@ -1084,7 +1084,7 @@
         <v>228</v>
       </c>
       <c r="D48">
-        <v>0.5406463884806197</v>
+        <v>0.523225818772967</v>
       </c>
     </row>
     <row r="49" spans="1:4">
@@ -1098,7 +1098,7 @@
         <v>229</v>
       </c>
       <c r="D49">
-        <v>0.5424997578583151</v>
+        <v>0.5241598896151451</v>
       </c>
     </row>
     <row r="50" spans="1:4">
@@ -1112,7 +1112,7 @@
         <v>230</v>
       </c>
       <c r="D50">
-        <v>0.5443346710157354</v>
+        <v>0.5251072885153475</v>
       </c>
     </row>
     <row r="51" spans="1:4">
@@ -1126,7 +1126,7 @@
         <v>231</v>
       </c>
       <c r="D51">
-        <v>0.5461511279528807</v>
+        <v>0.5260677195994646</v>
       </c>
     </row>
     <row r="52" spans="1:4">
@@ -1140,7 +1140,7 @@
         <v>232</v>
       </c>
       <c r="D52">
-        <v>0.5479491286697509</v>
+        <v>0.5270408869933871</v>
       </c>
     </row>
     <row r="53" spans="1:4">
@@ -1154,7 +1154,7 @@
         <v>233</v>
       </c>
       <c r="D53">
-        <v>0.5497286731663461</v>
+        <v>0.5280264948230055</v>
       </c>
     </row>
     <row r="54" spans="1:4">
@@ -1168,7 +1168,7 @@
         <v>234</v>
       </c>
       <c r="D54">
-        <v>0.5514897614426664</v>
+        <v>0.5290242472142103</v>
       </c>
     </row>
     <row r="55" spans="1:4">
@@ -1182,7 +1182,7 @@
         <v>235</v>
       </c>
       <c r="D55">
-        <v>0.5532323934987116</v>
+        <v>0.530033848292892</v>
       </c>
     </row>
     <row r="56" spans="1:4">
@@ -1196,7 +1196,7 @@
         <v>236</v>
       </c>
       <c r="D56">
-        <v>0.5549565693344817</v>
+        <v>0.5310550021849413</v>
       </c>
     </row>
     <row r="57" spans="1:4">
@@ -1210,7 +1210,7 @@
         <v>237</v>
       </c>
       <c r="D57">
-        <v>0.5566622889499768</v>
+        <v>0.5320874130162485</v>
       </c>
     </row>
     <row r="58" spans="1:4">
@@ -1224,7 +1224,7 @@
         <v>238</v>
       </c>
       <c r="D58">
-        <v>0.5583495523451969</v>
+        <v>0.5331307849127045</v>
       </c>
     </row>
     <row r="59" spans="1:4">
@@ -1238,7 +1238,7 @@
         <v>239</v>
       </c>
       <c r="D59">
-        <v>0.560018359520142</v>
+        <v>0.5341848220001995</v>
       </c>
     </row>
     <row r="60" spans="1:4">
@@ -1252,7 +1252,7 @@
         <v>240</v>
       </c>
       <c r="D60">
-        <v>0.561668710474812</v>
+        <v>0.5352492284046242</v>
       </c>
     </row>
     <row r="61" spans="1:4">
@@ -1266,7 +1266,7 @@
         <v>241</v>
       </c>
       <c r="D61">
-        <v>0.5633006052092071</v>
+        <v>0.5363237082518691</v>
       </c>
     </row>
     <row r="62" spans="1:4">
@@ -1280,7 +1280,7 @@
         <v>242</v>
       </c>
       <c r="D62">
-        <v>0.5649140437233271</v>
+        <v>0.5374079656678248</v>
       </c>
     </row>
     <row r="63" spans="1:4">
@@ -1294,7 +1294,7 @@
         <v>243</v>
       </c>
       <c r="D63">
-        <v>0.566509026017172</v>
+        <v>0.5385017047783818</v>
       </c>
     </row>
     <row r="64" spans="1:4">
@@ -1308,7 +1308,7 @@
         <v>244</v>
       </c>
       <c r="D64">
-        <v>0.568085552090742</v>
+        <v>0.5396046297094307</v>
       </c>
     </row>
     <row r="65" spans="1:4">
@@ -1322,7 +1322,7 @@
         <v>245</v>
       </c>
       <c r="D65">
-        <v>0.5696436219440368</v>
+        <v>0.5407164445868619</v>
       </c>
     </row>
     <row r="66" spans="1:4">
@@ -1336,7 +1336,7 @@
         <v>246</v>
       </c>
       <c r="D66">
-        <v>0.5711832355770567</v>
+        <v>0.541836853536566</v>
       </c>
     </row>
     <row r="67" spans="1:4">
@@ -1350,7 +1350,7 @@
         <v>247</v>
       </c>
       <c r="D67">
-        <v>0.5727043929898017</v>
+        <v>0.5429655606844336</v>
       </c>
     </row>
     <row r="68" spans="1:4">
@@ -1364,7 +1364,7 @@
         <v>248</v>
       </c>
       <c r="D68">
-        <v>0.5742070941822716</v>
+        <v>0.5441022701563553</v>
       </c>
     </row>
     <row r="69" spans="1:4">
@@ -1378,7 +1378,7 @@
         <v>249</v>
       </c>
       <c r="D69">
-        <v>0.5756913391544664</v>
+        <v>0.5452466860782214</v>
       </c>
     </row>
     <row r="70" spans="1:4">
@@ -1392,7 +1392,7 @@
         <v>250</v>
       </c>
       <c r="D70">
-        <v>0.5771571279063862</v>
+        <v>0.5463985125759226</v>
       </c>
     </row>
     <row r="71" spans="1:4">
@@ -1406,7 +1406,7 @@
         <v>251</v>
       </c>
       <c r="D71">
-        <v>0.5786044604380309</v>
+        <v>0.5475574537753496</v>
       </c>
     </row>
     <row r="72" spans="1:4">
@@ -1420,7 +1420,7 @@
         <v>252</v>
       </c>
       <c r="D72">
-        <v>0.5800333367494007</v>
+        <v>0.5487232138023926</v>
       </c>
     </row>
     <row r="73" spans="1:4">
@@ -1434,7 +1434,7 @@
         <v>253</v>
       </c>
       <c r="D73">
-        <v>0.5814437568404954</v>
+        <v>0.5498954967829425</v>
       </c>
     </row>
     <row r="74" spans="1:4">
@@ -1448,7 +1448,7 @@
         <v>254</v>
       </c>
       <c r="D74">
-        <v>0.5828357207113152</v>
+        <v>0.5510740068428895</v>
       </c>
     </row>
     <row r="75" spans="1:4">
@@ -1462,7 +1462,7 @@
         <v>255</v>
       </c>
       <c r="D75">
-        <v>0.5842092283618598</v>
+        <v>0.5522584481081244</v>
       </c>
     </row>
     <row r="76" spans="1:4">
@@ -1476,7 +1476,7 @@
         <v>256</v>
       </c>
       <c r="D76">
-        <v>0.5855642797921294</v>
+        <v>0.5534485247045375</v>
       </c>
     </row>
     <row r="77" spans="1:4">
@@ -1490,7 +1490,7 @@
         <v>257</v>
       </c>
       <c r="D77">
-        <v>0.5869008750021241</v>
+        <v>0.5546439407580197</v>
       </c>
     </row>
     <row r="78" spans="1:4">
@@ -1504,7 +1504,7 @@
         <v>258</v>
       </c>
       <c r="D78">
-        <v>0.5882190139918437</v>
+        <v>0.5558444003944611</v>
       </c>
     </row>
     <row r="79" spans="1:4">
@@ -1518,7 +1518,7 @@
         <v>259</v>
       </c>
       <c r="D79">
-        <v>0.5895186967612883</v>
+        <v>0.5570496077397527</v>
       </c>
     </row>
     <row r="80" spans="1:4">
@@ -1532,7 +1532,7 @@
         <v>260</v>
       </c>
       <c r="D80">
-        <v>0.5907999233104578</v>
+        <v>0.5582592669197847</v>
       </c>
     </row>
     <row r="81" spans="1:4">
@@ -1546,7 +1546,7 @@
         <v>261</v>
       </c>
       <c r="D81">
-        <v>0.5920626936393524</v>
+        <v>0.5594730820604478</v>
       </c>
     </row>
     <row r="82" spans="1:4">
@@ -1560,7 +1560,7 @@
         <v>262</v>
       </c>
       <c r="D82">
-        <v>0.5933070077479718</v>
+        <v>0.5606907572876324</v>
       </c>
     </row>
     <row r="83" spans="1:4">
@@ -1574,7 +1574,7 @@
         <v>263</v>
       </c>
       <c r="D83">
-        <v>0.5945328656363164</v>
+        <v>0.5619119967272291</v>
       </c>
     </row>
     <row r="84" spans="1:4">
@@ -1588,7 +1588,7 @@
         <v>264</v>
       </c>
       <c r="D84">
-        <v>0.5957402673043859</v>
+        <v>0.5631365045051286</v>
       </c>
     </row>
     <row r="85" spans="1:4">
@@ -1602,7 +1602,7 @@
         <v>265</v>
       </c>
       <c r="D85">
-        <v>0.5969292127521802</v>
+        <v>0.5643639847472213</v>
       </c>
     </row>
     <row r="86" spans="1:4">
@@ -1616,7 +1616,7 @@
         <v>266</v>
       </c>
       <c r="D86">
-        <v>0.5980997019796996</v>
+        <v>0.5655941415793978</v>
       </c>
     </row>
     <row r="87" spans="1:4">
@@ -1630,7 +1630,7 @@
         <v>267</v>
       </c>
       <c r="D87">
-        <v>0.5992517349869441</v>
+        <v>0.5668266791275485</v>
       </c>
     </row>
     <row r="88" spans="1:4">
@@ -1644,7 +1644,7 @@
         <v>268</v>
       </c>
       <c r="D88">
-        <v>0.6003853117739134</v>
+        <v>0.5680613015175642</v>
       </c>
     </row>
     <row r="89" spans="1:4">
@@ -1658,7 +1658,7 @@
         <v>269</v>
       </c>
       <c r="D89">
-        <v>0.6015004323406078</v>
+        <v>0.5692977128753351</v>
       </c>
     </row>
     <row r="90" spans="1:4">
@@ -1672,7 +1672,7 @@
         <v>270</v>
       </c>
       <c r="D90">
-        <v>0.6025970966870271</v>
+        <v>0.5705356173267521</v>
       </c>
     </row>
     <row r="91" spans="1:4">
@@ -1686,7 +1686,7 @@
         <v>271</v>
       </c>
       <c r="D91">
-        <v>0.6036753048131713</v>
+        <v>0.5717747189977055</v>
       </c>
     </row>
     <row r="92" spans="1:4">
@@ -1700,7 +1700,7 @@
         <v>272</v>
       </c>
       <c r="D92">
-        <v>0.6047350567190406</v>
+        <v>0.5730147220140859</v>
       </c>
     </row>
     <row r="93" spans="1:4">
@@ -1714,7 +1714,7 @@
         <v>273</v>
       </c>
       <c r="D93">
-        <v>0.6057763524046349</v>
+        <v>0.5742553305017838</v>
       </c>
     </row>
     <row r="94" spans="1:4">
@@ -1728,7 +1728,7 @@
         <v>274</v>
       </c>
       <c r="D94">
-        <v>0.6067991918699541</v>
+        <v>0.5754962485866899</v>
       </c>
     </row>
     <row r="95" spans="1:4">
@@ -1742,7 +1742,7 @@
         <v>275</v>
       </c>
       <c r="D95">
-        <v>0.6078035751149983</v>
+        <v>0.5767371803946946</v>
       </c>
     </row>
     <row r="96" spans="1:4">
@@ -1756,7 +1756,7 @@
         <v>276</v>
       </c>
       <c r="D96">
-        <v>0.6087895021397675</v>
+        <v>0.5779778300516885</v>
       </c>
     </row>
     <row r="97" spans="1:4">
@@ -1770,7 +1770,7 @@
         <v>277</v>
       </c>
       <c r="D97">
-        <v>0.6097569729442616</v>
+        <v>0.5792179016835621</v>
       </c>
     </row>
     <row r="98" spans="1:4">
@@ -1784,7 +1784,7 @@
         <v>278</v>
       </c>
       <c r="D98">
-        <v>0.6107059875284807</v>
+        <v>0.5804570994162059</v>
       </c>
     </row>
     <row r="99" spans="1:4">
@@ -1798,7 +1798,7 @@
         <v>279</v>
       </c>
       <c r="D99">
-        <v>0.6116365458924248</v>
+        <v>0.5816951273755107</v>
       </c>
     </row>
     <row r="100" spans="1:4">
@@ -1812,7 +1812,7 @@
         <v>280</v>
       </c>
       <c r="D100">
-        <v>0.6125486480360939</v>
+        <v>0.5829316896873666</v>
       </c>
     </row>
     <row r="101" spans="1:4">
@@ -1826,7 +1826,7 @@
         <v>281</v>
       </c>
       <c r="D101">
-        <v>0.6134422939594879</v>
+        <v>0.5841664904776647</v>
       </c>
     </row>
     <row r="102" spans="1:4">
@@ -1840,7 +1840,7 @@
         <v>282</v>
       </c>
       <c r="D102">
-        <v>0.6143174836626069</v>
+        <v>0.585399233872295</v>
       </c>
     </row>
     <row r="103" spans="1:4">
@@ -1854,7 +1854,7 @@
         <v>283</v>
       </c>
       <c r="D103">
-        <v>0.6151742171454508</v>
+        <v>0.5866296239971482</v>
       </c>
     </row>
     <row r="104" spans="1:4">
@@ -1868,7 +1868,7 @@
         <v>284</v>
       </c>
       <c r="D104">
-        <v>0.6160124944080199</v>
+        <v>0.5878573649781151</v>
       </c>
     </row>
     <row r="105" spans="1:4">
@@ -1882,7 +1882,7 @@
         <v>285</v>
       </c>
       <c r="D105">
-        <v>0.6168323154503138</v>
+        <v>0.589082160941086</v>
       </c>
     </row>
     <row r="106" spans="1:4">
@@ -1896,7 +1896,7 @@
         <v>286</v>
       </c>
       <c r="D106">
-        <v>0.6176336802723328</v>
+        <v>0.5903037160119515</v>
       </c>
     </row>
     <row r="107" spans="1:4">
@@ -1910,7 +1910,7 @@
         <v>287</v>
       </c>
       <c r="D107">
-        <v>0.6184165888740767</v>
+        <v>0.5915217343166022</v>
       </c>
     </row>
     <row r="108" spans="1:4">
@@ -1924,7 +1924,7 @@
         <v>288</v>
       </c>
       <c r="D108">
-        <v>0.6191810412555455</v>
+        <v>0.5927359199809286</v>
       </c>
     </row>
     <row r="109" spans="1:4">
@@ -1938,7 +1938,7 @@
         <v>289</v>
       </c>
       <c r="D109">
-        <v>0.6199270374167394</v>
+        <v>0.5939459771308211</v>
       </c>
     </row>
     <row r="110" spans="1:4">
@@ -1952,7 +1952,7 @@
         <v>290</v>
       </c>
       <c r="D110">
-        <v>0.6206545773576582</v>
+        <v>0.5951516098921704</v>
       </c>
     </row>
     <row r="111" spans="1:4">
@@ -1966,7 +1966,7 @@
         <v>291</v>
       </c>
       <c r="D111">
-        <v>0.621363661078302</v>
+        <v>0.596352522390867</v>
       </c>
     </row>
     <row r="112" spans="1:4">
@@ -1980,7 +1980,7 @@
         <v>292</v>
       </c>
       <c r="D112">
-        <v>0.6220542885786707</v>
+        <v>0.5975484187528015</v>
       </c>
     </row>
     <row r="113" spans="1:4">
@@ -1994,7 +1994,7 @@
         <v>293</v>
       </c>
       <c r="D113">
-        <v>0.6227264598587645</v>
+        <v>0.5987390031038644</v>
       </c>
     </row>
     <row r="114" spans="1:4">
@@ -2008,7 +2008,7 @@
         <v>294</v>
       </c>
       <c r="D114">
-        <v>0.6233801749185832</v>
+        <v>0.5999239795699463</v>
       </c>
     </row>
     <row r="115" spans="1:4">
@@ -2022,7 +2022,7 @@
         <v>295</v>
       </c>
       <c r="D115">
-        <v>0.624015433758127</v>
+        <v>0.6011030522769375</v>
       </c>
     </row>
     <row r="116" spans="1:4">
@@ -2036,7 +2036,7 @@
         <v>296</v>
       </c>
       <c r="D116">
-        <v>0.6246322363773955</v>
+        <v>0.6022759253507288</v>
       </c>
     </row>
     <row r="117" spans="1:4">
@@ -2050,7 +2050,7 @@
         <v>297</v>
       </c>
       <c r="D117">
-        <v>0.6252305827763892</v>
+        <v>0.6034423029172107</v>
       </c>
     </row>
     <row r="118" spans="1:4">
@@ -2064,7 +2064,7 @@
         <v>298</v>
       </c>
       <c r="D118">
-        <v>0.6258104729551078</v>
+        <v>0.6046018891022736</v>
       </c>
     </row>
     <row r="119" spans="1:4">
@@ -2078,7 +2078,7 @@
         <v>299</v>
       </c>
       <c r="D119">
-        <v>0.6263719069135514</v>
+        <v>0.6057543880318083</v>
       </c>
     </row>
     <row r="120" spans="1:4">
@@ -2092,7 +2092,7 @@
         <v>300</v>
       </c>
       <c r="D120">
-        <v>0.6269148846517201</v>
+        <v>0.6068995038317051</v>
       </c>
     </row>
     <row r="121" spans="1:4">
@@ -2106,7 +2106,7 @@
         <v>301</v>
       </c>
       <c r="D121">
-        <v>0.6274394061696136</v>
+        <v>0.6080369406278546</v>
       </c>
     </row>
     <row r="122" spans="1:4">
@@ -2120,7 +2120,7 @@
         <v>302</v>
       </c>
       <c r="D122">
-        <v>0.6279454714672321</v>
+        <v>0.6091664025461474</v>
       </c>
     </row>
     <row r="123" spans="1:4">
@@ -2134,7 +2134,7 @@
         <v>303</v>
       </c>
       <c r="D123">
-        <v>0.6284330805445756</v>
+        <v>0.6102875937124741</v>
       </c>
     </row>
     <row r="124" spans="1:4">
@@ -2148,7 +2148,7 @@
         <v>304</v>
       </c>
       <c r="D124">
-        <v>0.6289022334016441</v>
+        <v>0.6114002182527249</v>
       </c>
     </row>
     <row r="125" spans="1:4">
@@ -2162,7 +2162,7 @@
         <v>305</v>
       </c>
       <c r="D125">
-        <v>0.6293529300384375</v>
+        <v>0.6125039802927909</v>
       </c>
     </row>
     <row r="126" spans="1:4">
@@ -2176,7 +2176,7 @@
         <v>306</v>
       </c>
       <c r="D126">
-        <v>0.629785170454956</v>
+        <v>0.6135985839585621</v>
       </c>
     </row>
     <row r="127" spans="1:4">
@@ -2190,7 +2190,7 @@
         <v>307</v>
       </c>
       <c r="D127">
-        <v>0.6301989546511994</v>
+        <v>0.6146837333759294</v>
       </c>
     </row>
     <row r="128" spans="1:4">
@@ -2204,7 +2204,7 @@
         <v>308</v>
       </c>
       <c r="D128">
-        <v>0.6305942826271678</v>
+        <v>0.6157591326707832</v>
       </c>
     </row>
     <row r="129" spans="1:4">
@@ -2218,7 +2218,7 @@
         <v>309</v>
       </c>
       <c r="D129">
-        <v>0.6309711543828611</v>
+        <v>0.6168244859690141</v>
       </c>
     </row>
     <row r="130" spans="1:4">
@@ -2232,7 +2232,7 @@
         <v>310</v>
       </c>
       <c r="D130">
-        <v>0.6313295699182794</v>
+        <v>0.6178794973965126</v>
       </c>
     </row>
     <row r="131" spans="1:4">
@@ -2246,7 +2246,7 @@
         <v>311</v>
       </c>
       <c r="D131">
-        <v>0.6316695292334227</v>
+        <v>0.6189238710791691</v>
       </c>
     </row>
     <row r="132" spans="1:4">
@@ -2260,7 +2260,7 @@
         <v>312</v>
       </c>
       <c r="D132">
-        <v>0.631991032328291</v>
+        <v>0.6199573111428744</v>
       </c>
     </row>
     <row r="133" spans="1:4">
@@ -2274,7 +2274,7 @@
         <v>313</v>
       </c>
       <c r="D133">
-        <v>0.6322940792028842</v>
+        <v>0.620979521713519</v>
       </c>
     </row>
     <row r="134" spans="1:4">
@@ -2288,7 +2288,7 @@
         <v>314</v>
       </c>
       <c r="D134">
-        <v>0.6325786698572025</v>
+        <v>0.6219902069169934</v>
       </c>
     </row>
     <row r="135" spans="1:4">
@@ -2302,7 +2302,7 @@
         <v>315</v>
       </c>
       <c r="D135">
-        <v>0.6328448042912457</v>
+        <v>0.6229890708791879</v>
       </c>
     </row>
     <row r="136" spans="1:4">
@@ -2316,7 +2316,7 @@
         <v>316</v>
       </c>
       <c r="D136">
-        <v>0.6330924825050138</v>
+        <v>0.6239758177259934</v>
       </c>
     </row>
     <row r="137" spans="1:4">
@@ -2330,7 +2330,7 @@
         <v>317</v>
       </c>
       <c r="D137">
-        <v>0.633321704498507</v>
+        <v>0.6249501515833003</v>
       </c>
     </row>
     <row r="138" spans="1:4">
@@ -2344,7 +2344,7 @@
         <v>318</v>
       </c>
       <c r="D138">
-        <v>0.6335324702717251</v>
+        <v>0.625911776576999</v>
       </c>
     </row>
     <row r="139" spans="1:4">
@@ -2358,7 +2358,7 @@
         <v>319</v>
       </c>
       <c r="D139">
-        <v>0.6337247798246682</v>
+        <v>0.6268603968329803</v>
       </c>
     </row>
     <row r="140" spans="1:4">
@@ -2372,7 +2372,7 @@
         <v>320</v>
       </c>
       <c r="D140">
-        <v>0.6338986331573363</v>
+        <v>0.6277957164771346</v>
       </c>
     </row>
     <row r="141" spans="1:4">
@@ -2386,7 +2386,7 @@
         <v>321</v>
       </c>
       <c r="D141">
-        <v>0.6340540302697294</v>
+        <v>0.6287174396353525</v>
       </c>
     </row>
     <row r="142" spans="1:4">
@@ -2400,7 +2400,7 @@
         <v>322</v>
       </c>
       <c r="D142">
-        <v>0.6341909711618474</v>
+        <v>0.6296252704335246</v>
       </c>
     </row>
     <row r="143" spans="1:4">
@@ -2414,7 +2414,7 @@
         <v>323</v>
       </c>
       <c r="D143">
-        <v>0.6343094558336904</v>
+        <v>0.6305189129975411</v>
       </c>
     </row>
     <row r="144" spans="1:4">
@@ -2428,7 +2428,7 @@
         <v>324</v>
       </c>
       <c r="D144">
-        <v>0.6344094842852585</v>
+        <v>0.631398071453293</v>
       </c>
     </row>
     <row r="145" spans="1:4">
@@ -2442,7 +2442,7 @@
         <v>325</v>
       </c>
       <c r="D145">
-        <v>0.6344910565165514</v>
+        <v>0.6322624499266705</v>
       </c>
     </row>
     <row r="146" spans="1:4">
@@ -2456,7 +2456,7 @@
         <v>326</v>
       </c>
       <c r="D146">
-        <v>0.6345541725275693</v>
+        <v>0.6331117525435643</v>
       </c>
     </row>
     <row r="147" spans="1:4">
@@ -2470,7 +2470,7 @@
         <v>327</v>
       </c>
       <c r="D147">
-        <v>0.6345988323183123</v>
+        <v>0.633945683429865</v>
       </c>
     </row>
     <row r="148" spans="1:4">
@@ -2484,7 +2484,7 @@
         <v>328</v>
       </c>
       <c r="D148">
-        <v>0.6346250358887802</v>
+        <v>0.634763946711463</v>
       </c>
     </row>
     <row r="149" spans="1:4">
@@ -2498,7 +2498,7 @@
         <v>329</v>
       </c>
       <c r="D149">
-        <v>0.634632783238973</v>
+        <v>0.6355662465142489</v>
       </c>
     </row>
     <row r="150" spans="1:4">
@@ -2512,7 +2512,7 @@
         <v>330</v>
       </c>
       <c r="D150">
-        <v>0.6346220743688908</v>
+        <v>0.6363522869641132</v>
       </c>
     </row>
     <row r="151" spans="1:4">
@@ -2526,7 +2526,7 @@
         <v>331</v>
       </c>
       <c r="D151">
-        <v>0.6345929092785336</v>
+        <v>0.6371217721869465</v>
       </c>
     </row>
     <row r="152" spans="1:4">
@@ -2540,7 +2540,7 @@
         <v>332</v>
       </c>
       <c r="D152">
-        <v>0.6345452879679014</v>
+        <v>0.6378744063086395</v>
       </c>
     </row>
     <row r="153" spans="1:4">
@@ -2554,7 +2554,7 @@
         <v>333</v>
       </c>
       <c r="D153">
-        <v>0.6344792104369942</v>
+        <v>0.6386098934550823</v>
       </c>
     </row>
     <row r="154" spans="1:4">
@@ -2568,7 +2568,7 @@
         <v>334</v>
       </c>
       <c r="D154">
-        <v>0.634394676685812</v>
+        <v>0.6393279377521659</v>
       </c>
     </row>
     <row r="155" spans="1:4">
@@ -2582,7 +2582,7 @@
         <v>335</v>
       </c>
       <c r="D155">
-        <v>0.6342916867143547</v>
+        <v>0.6400282433257806</v>
       </c>
     </row>
     <row r="156" spans="1:4">
@@ -2596,7 +2596,7 @@
         <v>336</v>
       </c>
       <c r="D156">
-        <v>0.6341702405226224</v>
+        <v>0.6407105143018169</v>
       </c>
     </row>
     <row r="157" spans="1:4">
@@ -2610,7 +2610,7 @@
         <v>337</v>
       </c>
       <c r="D157">
-        <v>0.6340303381106149</v>
+        <v>0.6413744548061655</v>
       </c>
     </row>
     <row r="158" spans="1:4">
@@ -2624,7 +2624,7 @@
         <v>338</v>
       </c>
       <c r="D158">
-        <v>0.6338719794783326</v>
+        <v>0.6420197689647169</v>
       </c>
     </row>
     <row r="159" spans="1:4">
@@ -2638,7 +2638,7 @@
         <v>339</v>
       </c>
       <c r="D159">
-        <v>0.6336951646257752</v>
+        <v>0.6426461609033616</v>
       </c>
     </row>
     <row r="160" spans="1:4">
@@ -2652,7 +2652,7 @@
         <v>340</v>
       </c>
       <c r="D160">
-        <v>0.6334998935529428</v>
+        <v>0.6432533347479902</v>
       </c>
     </row>
     <row r="161" spans="1:4">
@@ -2666,7 +2666,7 @@
         <v>341</v>
       </c>
       <c r="D161">
-        <v>0.6332861662598354</v>
+        <v>0.6438409946244932</v>
       </c>
     </row>
     <row r="162" spans="1:4">
@@ -2680,7 +2680,7 @@
         <v>342</v>
       </c>
       <c r="D162">
-        <v>0.633053982746453</v>
+        <v>0.644408844658761</v>
       </c>
     </row>
     <row r="163" spans="1:4">
@@ -2694,7 +2694,7 @@
         <v>343</v>
       </c>
       <c r="D163">
-        <v>0.6328033430127954</v>
+        <v>0.6449565889766844</v>
       </c>
     </row>
     <row r="164" spans="1:4">
@@ -2708,7 +2708,7 @@
         <v>344</v>
       </c>
       <c r="D164">
-        <v>0.632534247058863</v>
+        <v>0.6454839317041539</v>
       </c>
     </row>
     <row r="165" spans="1:4">
@@ -2722,7 +2722,7 @@
         <v>345</v>
       </c>
       <c r="D165">
-        <v>0.6322466948846555</v>
+        <v>0.6459905769670597</v>
       </c>
     </row>
     <row r="166" spans="1:4">
@@ -2736,7 +2736,7 @@
         <v>346</v>
       </c>
       <c r="D166">
-        <v>0.6319406864901729</v>
+        <v>0.6464762288912929</v>
       </c>
     </row>
     <row r="167" spans="1:4">
@@ -2750,7 +2750,7 @@
         <v>347</v>
       </c>
       <c r="D167">
-        <v>0.6316162218754152</v>
+        <v>0.6469405916027436</v>
       </c>
     </row>
     <row r="168" spans="1:4">
@@ -2764,7 +2764,7 @@
         <v>348</v>
       </c>
       <c r="D168">
-        <v>0.6312733010403827</v>
+        <v>0.6473833692273026</v>
       </c>
     </row>
     <row r="169" spans="1:4">
@@ -2778,7 +2778,7 @@
         <v>349</v>
       </c>
       <c r="D169">
-        <v>0.630911923985075</v>
+        <v>0.6478042658908603</v>
       </c>
     </row>
     <row r="170" spans="1:4">
@@ -2792,7 +2792,7 @@
         <v>350</v>
       </c>
       <c r="D170">
-        <v>0.6305320907094923</v>
+        <v>0.6482029857193072</v>
       </c>
     </row>
     <row r="171" spans="1:4">
@@ -2806,7 +2806,7 @@
         <v>351</v>
       </c>
       <c r="D171">
-        <v>0.6301338012136347</v>
+        <v>0.648579232838534</v>
       </c>
     </row>
     <row r="172" spans="1:4">
@@ -2820,7 +2820,7 @@
         <v>352</v>
       </c>
       <c r="D172">
-        <v>0.629717055497502</v>
+        <v>0.6489327113744312</v>
       </c>
     </row>
     <row r="173" spans="1:4">
@@ -2834,7 +2834,7 @@
         <v>353</v>
       </c>
       <c r="D173">
-        <v>0.6292818535610942</v>
+        <v>0.6492631254528892</v>
       </c>
     </row>
     <row r="174" spans="1:4">
@@ -2848,7 +2848,7 @@
         <v>354</v>
       </c>
       <c r="D174">
-        <v>0.6288281954044115</v>
+        <v>0.6495701791997988</v>
       </c>
     </row>
     <row r="175" spans="1:4">
@@ -2862,7 +2862,7 @@
         <v>355</v>
       </c>
       <c r="D175">
-        <v>0.6283560810274538</v>
+        <v>0.6498535767410502</v>
       </c>
     </row>
     <row r="176" spans="1:4">
@@ -2876,7 +2876,7 @@
         <v>356</v>
       </c>
       <c r="D176">
-        <v>0.6278655104302209</v>
+        <v>0.6501130222025342</v>
       </c>
     </row>
     <row r="177" spans="1:4">
@@ -2890,7 +2890,7 @@
         <v>357</v>
       </c>
       <c r="D177">
-        <v>0.6273564836127131</v>
+        <v>0.6503482197101413</v>
       </c>
     </row>
     <row r="178" spans="1:4">
@@ -2904,7 +2904,7 @@
         <v>358</v>
       </c>
       <c r="D178">
-        <v>0.6268290005749303</v>
+        <v>0.650558873389762</v>
       </c>
     </row>
     <row r="179" spans="1:4">
@@ -2918,7 +2918,7 @@
         <v>359</v>
       </c>
       <c r="D179">
-        <v>0.6262830613168724</v>
+        <v>0.6507446873672869</v>
       </c>
     </row>
     <row r="180" spans="1:4">
@@ -2932,7 +2932,7 @@
         <v>360</v>
       </c>
       <c r="D180">
-        <v>0.6257186658385394</v>
+        <v>0.6509053657686064</v>
       </c>
     </row>
     <row r="181" spans="1:4">
@@ -2946,7 +2946,7 @@
         <v>361</v>
       </c>
       <c r="D181">
-        <v>0.6251358141399315</v>
+        <v>0.6510406127196111</v>
       </c>
     </row>
     <row r="182" spans="1:4">
@@ -2960,7 +2960,7 @@
         <v>362</v>
       </c>
       <c r="D182">
-        <v>0.6245345062210486</v>
+        <v>0.6511501323461917</v>
       </c>
     </row>
     <row r="183" spans="1:4">
@@ -2974,7 +2974,7 @@
         <v>363</v>
       </c>
       <c r="D183">
-        <v>0.6239147420818906</v>
+        <v>0.6512336287742386</v>
       </c>
     </row>
     <row r="184" spans="1:4">
@@ -2988,7 +2988,7 @@
         <v>364</v>
       </c>
       <c r="D184">
-        <v>0.6232765217224576</v>
+        <v>0.6512908061296423</v>
       </c>
     </row>
     <row r="185" spans="1:4">
@@ -3002,7 +3002,7 @@
         <v>365</v>
       </c>
       <c r="D185">
-        <v>0.6226198451427496</v>
+        <v>0.6513213685382935</v>
       </c>
     </row>
     <row r="186" spans="1:4">
@@ -3016,7 +3016,7 @@
         <v>1</v>
       </c>
       <c r="D186">
-        <v>0.6219447123427666</v>
+        <v>0.6513250201260826</v>
       </c>
     </row>
     <row r="187" spans="1:4">
@@ -3030,7 +3030,7 @@
         <v>2</v>
       </c>
       <c r="D187">
-        <v>0.6212511233225084</v>
+        <v>0.6513014650189002</v>
       </c>
     </row>
     <row r="188" spans="1:4">
@@ -3044,7 +3044,7 @@
         <v>3</v>
       </c>
       <c r="D188">
-        <v>0.6205390780819754</v>
+        <v>0.6512504073426368</v>
       </c>
     </row>
     <row r="189" spans="1:4">
@@ -3058,7 +3058,7 @@
         <v>4</v>
       </c>
       <c r="D189">
-        <v>0.6198085766211673</v>
+        <v>0.651171551223183</v>
       </c>
     </row>
     <row r="190" spans="1:4">
@@ -3072,7 +3072,7 @@
         <v>5</v>
       </c>
       <c r="D190">
-        <v>0.6190596189400841</v>
+        <v>0.6510646007864294</v>
       </c>
     </row>
     <row r="191" spans="1:4">
@@ -3086,7 +3086,7 @@
         <v>6</v>
       </c>
       <c r="D191">
-        <v>0.618292205038726</v>
+        <v>0.6509292601582664</v>
       </c>
     </row>
     <row r="192" spans="1:4">
@@ -3100,7 +3100,7 @@
         <v>7</v>
       </c>
       <c r="D192">
-        <v>0.6175063349170927</v>
+        <v>0.6507652334645846</v>
       </c>
     </row>
     <row r="193" spans="1:4">
@@ -3114,7 +3114,7 @@
         <v>8</v>
       </c>
       <c r="D193">
-        <v>0.6167020085751845</v>
+        <v>0.6505722248312744</v>
       </c>
     </row>
     <row r="194" spans="1:4">
@@ -3128,7 +3128,7 @@
         <v>9</v>
       </c>
       <c r="D194">
-        <v>0.6158792260130013</v>
+        <v>0.6503499383842266</v>
       </c>
     </row>
     <row r="195" spans="1:4">
@@ -3142,7 +3142,7 @@
         <v>10</v>
       </c>
       <c r="D195">
-        <v>0.6150379872305429</v>
+        <v>0.6500980782493317</v>
       </c>
     </row>
     <row r="196" spans="1:4">
@@ -3156,7 +3156,7 @@
         <v>11</v>
       </c>
       <c r="D196">
-        <v>0.6141782922278096</v>
+        <v>0.64981634855248</v>
       </c>
     </row>
     <row r="197" spans="1:4">
@@ -3170,7 +3170,7 @@
         <v>12</v>
       </c>
       <c r="D197">
-        <v>0.6133001410048013</v>
+        <v>0.6495044534195624</v>
       </c>
     </row>
     <row r="198" spans="1:4">
@@ -3184,7 +3184,7 @@
         <v>13</v>
       </c>
       <c r="D198">
-        <v>0.612403533561518</v>
+        <v>0.6491620969764691</v>
       </c>
     </row>
     <row r="199" spans="1:4">
@@ -3198,7 +3198,7 @@
         <v>14</v>
       </c>
       <c r="D199">
-        <v>0.6114884698979597</v>
+        <v>0.6487889833490909</v>
       </c>
     </row>
     <row r="200" spans="1:4">
@@ -3212,7 +3212,7 @@
         <v>15</v>
       </c>
       <c r="D200">
-        <v>0.6105549500141263</v>
+        <v>0.6483848166633182</v>
       </c>
     </row>
     <row r="201" spans="1:4">
@@ -3226,7 +3226,7 @@
         <v>16</v>
       </c>
       <c r="D201">
-        <v>0.6096029739100178</v>
+        <v>0.6479493010450414</v>
       </c>
     </row>
     <row r="202" spans="1:4">
@@ -3240,7 +3240,7 @@
         <v>17</v>
       </c>
       <c r="D202">
-        <v>0.6086325415856344</v>
+        <v>0.6474821406201514</v>
       </c>
     </row>
     <row r="203" spans="1:4">
@@ -3254,7 +3254,7 @@
         <v>18</v>
       </c>
       <c r="D203">
-        <v>0.6076436530409759</v>
+        <v>0.6469830395145386</v>
       </c>
     </row>
     <row r="204" spans="1:4">
@@ -3268,7 +3268,7 @@
         <v>19</v>
       </c>
       <c r="D204">
-        <v>0.6066363082760424</v>
+        <v>0.6464517018540934</v>
       </c>
     </row>
     <row r="205" spans="1:4">
@@ -3282,7 +3282,7 @@
         <v>20</v>
       </c>
       <c r="D205">
-        <v>0.605610507290834</v>
+        <v>0.6458878317647064</v>
       </c>
     </row>
     <row r="206" spans="1:4">
@@ -3296,7 +3296,7 @@
         <v>21</v>
       </c>
       <c r="D206">
-        <v>0.6045662500853504</v>
+        <v>0.6452911333722683</v>
       </c>
     </row>
     <row r="207" spans="1:4">
@@ -3310,7 +3310,7 @@
         <v>22</v>
       </c>
       <c r="D207">
-        <v>0.6035035366595918</v>
+        <v>0.6446613108026695</v>
       </c>
     </row>
     <row r="208" spans="1:4">
@@ -3324,7 +3324,7 @@
         <v>23</v>
       </c>
       <c r="D208">
-        <v>0.6024223670135582</v>
+        <v>0.6439980681818006</v>
       </c>
     </row>
     <row r="209" spans="1:4">
@@ -3338,7 +3338,7 @@
         <v>24</v>
       </c>
       <c r="D209">
-        <v>0.6013227411472496</v>
+        <v>0.6433011096355521</v>
       </c>
     </row>
     <row r="210" spans="1:4">
@@ -3352,7 +3352,7 @@
         <v>25</v>
       </c>
       <c r="D210">
-        <v>0.600204659060666</v>
+        <v>0.6425701392898144</v>
       </c>
     </row>
     <row r="211" spans="1:4">
@@ -3366,7 +3366,7 @@
         <v>26</v>
       </c>
       <c r="D211">
-        <v>0.5990681207538073</v>
+        <v>0.6418048612704783</v>
       </c>
     </row>
     <row r="212" spans="1:4">
@@ -3380,7 +3380,7 @@
         <v>27</v>
       </c>
       <c r="D212">
-        <v>0.5979131262266736</v>
+        <v>0.6410049797034343</v>
       </c>
     </row>
     <row r="213" spans="1:4">
@@ -3394,7 +3394,7 @@
         <v>28</v>
       </c>
       <c r="D213">
-        <v>0.5967396754792649</v>
+        <v>0.6401701987145728</v>
       </c>
     </row>
     <row r="214" spans="1:4">
@@ -3408,7 +3408,7 @@
         <v>29</v>
       </c>
       <c r="D214">
-        <v>0.5955477685115812</v>
+        <v>0.6393002224297845</v>
       </c>
     </row>
     <row r="215" spans="1:4">
@@ -3422,7 +3422,7 @@
         <v>30</v>
       </c>
       <c r="D215">
-        <v>0.5943374053236223</v>
+        <v>0.6383947549749598</v>
       </c>
     </row>
     <row r="216" spans="1:4">
@@ -3436,7 +3436,7 @@
         <v>31</v>
       </c>
       <c r="D216">
-        <v>0.5931085859153886</v>
+        <v>0.6374535004759894</v>
       </c>
     </row>
     <row r="217" spans="1:4">
@@ -3450,7 +3450,7 @@
         <v>32</v>
       </c>
       <c r="D217">
-        <v>0.5918613102868798</v>
+        <v>0.6364761630587635</v>
       </c>
     </row>
     <row r="218" spans="1:4">
@@ -3464,7 +3464,7 @@
         <v>33</v>
       </c>
       <c r="D218">
-        <v>0.590595578438096</v>
+        <v>0.6354624468491731</v>
       </c>
     </row>
     <row r="219" spans="1:4">
@@ -3478,7 +3478,7 @@
         <v>34</v>
       </c>
       <c r="D219">
-        <v>0.5893113903690371</v>
+        <v>0.6344120559731085</v>
       </c>
     </row>
     <row r="220" spans="1:4">
@@ -3492,7 +3492,7 @@
         <v>35</v>
       </c>
       <c r="D220">
-        <v>0.5880087460797032</v>
+        <v>0.6333246945564602</v>
       </c>
     </row>
     <row r="221" spans="1:4">
@@ -3506,7 +3506,7 @@
         <v>36</v>
       </c>
       <c r="D221">
-        <v>0.5866876455700943</v>
+        <v>0.6322000667251189</v>
       </c>
     </row>
     <row r="222" spans="1:4">
@@ -3520,7 +3520,7 @@
         <v>37</v>
       </c>
       <c r="D222">
-        <v>0.5853480888402104</v>
+        <v>0.6310378766049749</v>
       </c>
     </row>
     <row r="223" spans="1:4">
@@ -3534,7 +3534,7 @@
         <v>38</v>
       </c>
       <c r="D223">
-        <v>0.5839900758900514</v>
+        <v>0.629837828321919</v>
       </c>
     </row>
     <row r="224" spans="1:4">
@@ -3548,7 +3548,7 @@
         <v>39</v>
       </c>
       <c r="D224">
-        <v>0.5826136067196175</v>
+        <v>0.6285996260018417</v>
       </c>
     </row>
     <row r="225" spans="1:4">
@@ -3562,7 +3562,7 @@
         <v>40</v>
       </c>
       <c r="D225">
-        <v>0.5812186813289084</v>
+        <v>0.6273229737706334</v>
       </c>
     </row>
     <row r="226" spans="1:4">
@@ -3576,7 +3576,7 @@
         <v>41</v>
       </c>
       <c r="D226">
-        <v>0.5798052997179244</v>
+        <v>0.6260075757541848</v>
       </c>
     </row>
     <row r="227" spans="1:4">
@@ -3590,7 +3590,7 @@
         <v>42</v>
       </c>
       <c r="D227">
-        <v>0.5783734618866653</v>
+        <v>0.6246531360783862</v>
       </c>
     </row>
     <row r="228" spans="1:4">
@@ -3604,7 +3604,7 @@
         <v>43</v>
       </c>
       <c r="D228">
-        <v>0.5769231678351313</v>
+        <v>0.6232593588691284</v>
       </c>
     </row>
     <row r="229" spans="1:4">
@@ -3618,7 +3618,7 @@
         <v>44</v>
       </c>
       <c r="D229">
-        <v>0.5754544175633222</v>
+        <v>0.6218259482523019</v>
       </c>
     </row>
     <row r="230" spans="1:4">
@@ -3632,7 +3632,7 @@
         <v>45</v>
       </c>
       <c r="D230">
-        <v>0.573967211071238</v>
+        <v>0.6203526083537971</v>
       </c>
     </row>
     <row r="231" spans="1:4">
@@ -3646,7 +3646,7 @@
         <v>46</v>
       </c>
       <c r="D231">
-        <v>0.5724615483588789</v>
+        <v>0.6188390432995047</v>
       </c>
     </row>
     <row r="232" spans="1:4">
@@ -3660,7 +3660,7 @@
         <v>47</v>
       </c>
       <c r="D232">
-        <v>0.5709374294262447</v>
+        <v>0.6172849572153152</v>
       </c>
     </row>
     <row r="233" spans="1:4">
@@ -3674,7 +3674,7 @@
         <v>48</v>
       </c>
       <c r="D233">
-        <v>0.5693948542733355</v>
+        <v>0.6156900542271191</v>
       </c>
     </row>
     <row r="234" spans="1:4">
@@ -3688,7 +3688,7 @@
         <v>49</v>
       </c>
       <c r="D234">
-        <v>0.5678338229001513</v>
+        <v>0.6140540384608069</v>
       </c>
     </row>
     <row r="235" spans="1:4">
@@ -3702,7 +3702,7 @@
         <v>50</v>
       </c>
       <c r="D235">
-        <v>0.566254335306692</v>
+        <v>0.6123766140422692</v>
       </c>
     </row>
     <row r="236" spans="1:4">
@@ -3716,7 +3716,7 @@
         <v>51</v>
       </c>
       <c r="D236">
-        <v>0.5646563914929578</v>
+        <v>0.6106574850973966</v>
       </c>
     </row>
     <row r="237" spans="1:4">
@@ -3730,7 +3730,7 @@
         <v>52</v>
       </c>
       <c r="D237">
-        <v>0.5630399914589485</v>
+        <v>0.6088963557520795</v>
       </c>
     </row>
     <row r="238" spans="1:4">
@@ -3744,7 +3744,7 @@
         <v>53</v>
       </c>
       <c r="D238">
-        <v>0.5614051352046641</v>
+        <v>0.6070929301322086</v>
       </c>
     </row>
     <row r="239" spans="1:4">
@@ -3758,7 +3758,7 @@
         <v>54</v>
       </c>
       <c r="D239">
-        <v>0.5597518227301047</v>
+        <v>0.6052469123636743</v>
       </c>
     </row>
     <row r="240" spans="1:4">
@@ -3772,7 +3772,7 @@
         <v>55</v>
       </c>
       <c r="D240">
-        <v>0.5580800540352704</v>
+        <v>0.6033580065723673</v>
       </c>
     </row>
     <row r="241" spans="1:4">
@@ -3786,7 +3786,7 @@
         <v>56</v>
       </c>
       <c r="D241">
-        <v>0.556389829120161</v>
+        <v>0.601425916884178</v>
       </c>
     </row>
     <row r="242" spans="1:4">
@@ -3800,7 +3800,7 @@
         <v>57</v>
       </c>
       <c r="D242">
-        <v>0.5546811479847765</v>
+        <v>0.5994503474249969</v>
       </c>
     </row>
     <row r="243" spans="1:4">
@@ -3814,7 +3814,7 @@
         <v>58</v>
       </c>
       <c r="D243">
-        <v>0.5529540106291171</v>
+        <v>0.5974310023207148</v>
       </c>
     </row>
     <row r="244" spans="1:4">
@@ -3828,7 +3828,7 @@
         <v>59</v>
       </c>
       <c r="D244">
-        <v>0.5512084170531827</v>
+        <v>0.595367585697222</v>
       </c>
     </row>
     <row r="245" spans="1:4">
@@ -3842,7 +3842,7 @@
         <v>60</v>
       </c>
       <c r="D245">
-        <v>0.5494443672569731</v>
+        <v>0.5932598016804091</v>
       </c>
     </row>
     <row r="246" spans="1:4">
@@ -3856,7 +3856,7 @@
         <v>61</v>
       </c>
       <c r="D246">
-        <v>0.5476618612404885</v>
+        <v>0.5911073543961667</v>
       </c>
     </row>
     <row r="247" spans="1:4">
@@ -3870,7 +3870,7 @@
         <v>62</v>
       </c>
       <c r="D247">
-        <v>0.545860899003729</v>
+        <v>0.5889099479703852</v>
       </c>
     </row>
     <row r="248" spans="1:4">
@@ -3884,7 +3884,7 @@
         <v>63</v>
       </c>
       <c r="D248">
-        <v>0.5440414805466945</v>
+        <v>0.5866672865289554</v>
       </c>
     </row>
     <row r="249" spans="1:4">
@@ -3898,7 +3898,7 @@
         <v>64</v>
       </c>
       <c r="D249">
-        <v>0.5422036058693849</v>
+        <v>0.5843790741977676</v>
       </c>
     </row>
     <row r="250" spans="1:4">
@@ -3912,7 +3912,7 @@
         <v>65</v>
       </c>
       <c r="D250">
-        <v>0.5403472749718002</v>
+        <v>0.5820450151027123</v>
       </c>
     </row>
     <row r="251" spans="1:4">
@@ -3926,7 +3926,7 @@
         <v>66</v>
       </c>
       <c r="D251">
-        <v>0.5384724878539405</v>
+        <v>0.5796648133696803</v>
       </c>
     </row>
     <row r="252" spans="1:4">
@@ -3940,7 +3940,7 @@
         <v>67</v>
       </c>
       <c r="D252">
-        <v>0.536579244515806</v>
+        <v>0.577238173124562</v>
       </c>
     </row>
     <row r="253" spans="1:4">
@@ -3954,7 +3954,7 @@
         <v>68</v>
       </c>
       <c r="D253">
-        <v>0.5346675449573962</v>
+        <v>0.574764798493248</v>
       </c>
     </row>
     <row r="254" spans="1:4">
@@ -3968,7 +3968,7 @@
         <v>69</v>
       </c>
       <c r="D254">
-        <v>0.5327373891787115</v>
+        <v>0.5722443936016288</v>
       </c>
     </row>
     <row r="255" spans="1:4">
@@ -3982,7 +3982,7 @@
         <v>70</v>
       </c>
       <c r="D255">
-        <v>0.5307887771797517</v>
+        <v>0.5696766625755949</v>
       </c>
     </row>
     <row r="256" spans="1:4">
@@ -3996,7 +3996,7 @@
         <v>71</v>
       </c>
       <c r="D256">
-        <v>0.5288217089605171</v>
+        <v>0.5670613095410368</v>
       </c>
     </row>
     <row r="257" spans="1:4">
@@ -4010,7 +4010,7 @@
         <v>72</v>
       </c>
       <c r="D257">
-        <v>0.5268361845210072</v>
+        <v>0.5643980386238452</v>
       </c>
     </row>
     <row r="258" spans="1:4">
@@ -4024,7 +4024,7 @@
         <v>73</v>
       </c>
       <c r="D258">
-        <v>0.5248322038612223</v>
+        <v>0.5616865539499105</v>
       </c>
     </row>
     <row r="259" spans="1:4">
@@ -4038,7 +4038,7 @@
         <v>74</v>
       </c>
       <c r="D259">
-        <v>0.5228097669811624</v>
+        <v>0.5589265596451234</v>
       </c>
     </row>
     <row r="260" spans="1:4">
@@ -4052,7 +4052,7 @@
         <v>75</v>
       </c>
       <c r="D260">
-        <v>0.5207688738808276</v>
+        <v>0.5561177598353743</v>
       </c>
     </row>
     <row r="261" spans="1:4">
@@ -4066,7 +4066,7 @@
         <v>76</v>
       </c>
       <c r="D261">
-        <v>0.5187095245602178</v>
+        <v>0.5532598586465538</v>
       </c>
     </row>
     <row r="262" spans="1:4">
@@ -4080,7 +4080,7 @@
         <v>77</v>
       </c>
       <c r="D262">
-        <v>0.5166317190193328</v>
+        <v>0.5503525602045524</v>
       </c>
     </row>
     <row r="263" spans="1:4">
@@ -4094,7 +4094,7 @@
         <v>78</v>
       </c>
       <c r="D263">
-        <v>0.5145354572581728</v>
+        <v>0.5473955686352606</v>
       </c>
     </row>
     <row r="264" spans="1:4">
@@ -4108,7 +4108,7 @@
         <v>79</v>
       </c>
       <c r="D264">
-        <v>0.5124207392767379</v>
+        <v>0.5443885880645691</v>
       </c>
     </row>
     <row r="265" spans="1:4">
@@ -4122,7 +4122,7 @@
         <v>80</v>
       </c>
       <c r="D265">
-        <v>0.5102875650750279</v>
+        <v>0.5413313226183684</v>
       </c>
     </row>
     <row r="266" spans="1:4">
@@ -4136,7 +4136,7 @@
         <v>81</v>
       </c>
       <c r="D266">
-        <v>0.508135934653043</v>
+        <v>0.538223476422549</v>
       </c>
     </row>
     <row r="267" spans="1:4">
@@ -4150,7 +4150,7 @@
         <v>82</v>
       </c>
       <c r="D267">
-        <v>0.5059658480107828</v>
+        <v>0.5350647536030013</v>
       </c>
     </row>
     <row r="268" spans="1:4">
@@ -4164,7 +4164,7 @@
         <v>83</v>
       </c>
       <c r="D268">
-        <v>0.5037773051482477</v>
+        <v>0.5318548582856161</v>
       </c>
     </row>
     <row r="269" spans="1:4">
@@ -4178,7 +4178,7 @@
         <v>84</v>
       </c>
       <c r="D269">
-        <v>0.5015703060654377</v>
+        <v>0.5285934945962838</v>
       </c>
     </row>
     <row r="270" spans="1:4">
@@ -4192,7 +4192,7 @@
         <v>85</v>
       </c>
       <c r="D270">
-        <v>0.4993448507623526</v>
+        <v>0.5252803666608948</v>
       </c>
     </row>
     <row r="271" spans="1:4">
@@ -4206,7 +4206,7 @@
         <v>86</v>
       </c>
       <c r="D271">
-        <v>0.4971009392389925</v>
+        <v>0.52191517860534</v>
       </c>
     </row>
     <row r="272" spans="1:4">
@@ -4220,7 +4220,7 @@
         <v>87</v>
       </c>
       <c r="D272">
-        <v>0.4948385714953573</v>
+        <v>0.5184976345555097</v>
       </c>
     </row>
     <row r="273" spans="1:4">
@@ -4234,7 +4234,7 @@
         <v>88</v>
       </c>
       <c r="D273">
-        <v>0.4925577475314472</v>
+        <v>0.5150274386372945</v>
       </c>
     </row>
     <row r="274" spans="1:4">
@@ -4248,7 +4248,7 @@
         <v>89</v>
       </c>
       <c r="D274">
-        <v>0.4902584673472619</v>
+        <v>0.5115042949765849</v>
       </c>
     </row>
     <row r="275" spans="1:4">
@@ -4262,7 +4262,7 @@
         <v>90</v>
       </c>
       <c r="D275">
-        <v>0.4879407309428017</v>
+        <v>0.5079279076992715</v>
       </c>
     </row>
     <row r="276" spans="1:4">
@@ -4276,7 +4276,7 @@
         <v>91</v>
       </c>
       <c r="D276">
-        <v>0.4856045383180664</v>
+        <v>0.5042979809312448</v>
       </c>
     </row>
     <row r="277" spans="1:4">
@@ -4290,7 +4290,7 @@
         <v>92</v>
       </c>
       <c r="D277">
-        <v>0.4832498894730561</v>
+        <v>0.5006142187983954</v>
       </c>
     </row>
     <row r="278" spans="1:4">
@@ -4304,7 +4304,7 @@
         <v>93</v>
       </c>
       <c r="D278">
-        <v>0.4808767844077708</v>
+        <v>0.4968763254266137</v>
       </c>
     </row>
     <row r="279" spans="1:4">
@@ -4318,7 +4318,7 @@
         <v>94</v>
       </c>
       <c r="D279">
-        <v>0.4784852231222104</v>
+        <v>0.4930840049417904</v>
       </c>
     </row>
     <row r="280" spans="1:4">
@@ -4332,7 +4332,7 @@
         <v>95</v>
       </c>
       <c r="D280">
-        <v>0.4760752056163751</v>
+        <v>0.489236961469816</v>
       </c>
     </row>
     <row r="281" spans="1:4">
@@ -4346,7 +4346,7 @@
         <v>96</v>
       </c>
       <c r="D281">
-        <v>0.4736467318902647</v>
+        <v>0.485334899136581</v>
       </c>
     </row>
     <row r="282" spans="1:4">
@@ -4360,7 +4360,7 @@
         <v>97</v>
       </c>
       <c r="D282">
-        <v>0.4711998019438793</v>
+        <v>0.481377522067976</v>
       </c>
     </row>
     <row r="283" spans="1:4">
@@ -4374,7 +4374,7 @@
         <v>98</v>
       </c>
       <c r="D283">
-        <v>0.4687344157772189</v>
+        <v>0.4773645343898914</v>
       </c>
     </row>
     <row r="284" spans="1:4">
@@ -4388,7 +4388,7 @@
         <v>99</v>
       </c>
       <c r="D284">
-        <v>0.4662505733902834</v>
+        <v>0.473295640228218</v>
       </c>
     </row>
     <row r="285" spans="1:4">
@@ -4402,7 +4402,7 @@
         <v>100</v>
       </c>
       <c r="D285">
-        <v>0.463748274783073</v>
+        <v>0.469170543708846</v>
       </c>
     </row>
     <row r="286" spans="1:4">
@@ -4416,7 +4416,7 @@
         <v>101</v>
       </c>
       <c r="D286">
-        <v>0.4612275199555874</v>
+        <v>0.4649889489576663</v>
       </c>
     </row>
     <row r="287" spans="1:4">
@@ -4430,7 +4430,7 @@
         <v>102</v>
       </c>
       <c r="D287">
-        <v>0.4586883089078269</v>
+        <v>0.4607505601005693</v>
       </c>
     </row>
     <row r="288" spans="1:4">
@@ -4444,7 +4444,7 @@
         <v>103</v>
       </c>
       <c r="D288">
-        <v>0.4561306416397913</v>
+        <v>0.4564550812634454</v>
       </c>
     </row>
     <row r="289" spans="1:4">
@@ -4458,7 +4458,7 @@
         <v>104</v>
       </c>
       <c r="D289">
-        <v>0.4535545181514808</v>
+        <v>0.4521022165721852</v>
       </c>
     </row>
     <row r="290" spans="1:4">
@@ -4472,7 +4472,7 @@
         <v>105</v>
       </c>
       <c r="D290">
-        <v>0.4509599384428952</v>
+        <v>0.4476916701526795</v>
       </c>
     </row>
     <row r="291" spans="1:4">
@@ -4486,7 +4486,7 @@
         <v>106</v>
       </c>
       <c r="D291">
-        <v>0.4483469025140345</v>
+        <v>0.4432231461308184</v>
       </c>
     </row>
     <row r="292" spans="1:4">
@@ -4500,7 +4500,7 @@
         <v>107</v>
       </c>
       <c r="D292">
-        <v>0.4457154103648988</v>
+        <v>0.4386963486324928</v>
       </c>
     </row>
     <row r="293" spans="1:4">
@@ -4514,7 +4514,7 @@
         <v>108</v>
       </c>
       <c r="D293">
-        <v>0.4430654619954882</v>
+        <v>0.4341109817835931</v>
       </c>
     </row>
     <row r="294" spans="1:4">
@@ -4528,7 +4528,7 @@
         <v>109</v>
       </c>
       <c r="D294">
-        <v>0.4403970574058025</v>
+        <v>0.4294667497100099</v>
       </c>
     </row>
     <row r="295" spans="1:4">
@@ -4542,7 +4542,7 @@
         <v>110</v>
       </c>
       <c r="D295">
-        <v>0.4377101965958417</v>
+        <v>0.4247633565376338</v>
       </c>
     </row>
     <row r="296" spans="1:4">
@@ -4556,7 +4556,7 @@
         <v>111</v>
       </c>
       <c r="D296">
-        <v>0.435004879565606</v>
+        <v>0.4200005063923551</v>
       </c>
     </row>
     <row r="297" spans="1:4">
@@ -4570,7 +4570,7 @@
         <v>112</v>
       </c>
       <c r="D297">
-        <v>0.4322811063150953</v>
+        <v>0.4151779034000646</v>
       </c>
     </row>
     <row r="298" spans="1:4">
@@ -4584,7 +4584,7 @@
         <v>113</v>
       </c>
       <c r="D298">
-        <v>0.4295388768443094</v>
+        <v>0.4102952516866527</v>
       </c>
     </row>
     <row r="299" spans="1:4">
@@ -4598,7 +4598,7 @@
         <v>114</v>
       </c>
       <c r="D299">
-        <v>0.4267781911532486</v>
+        <v>0.40535225537801</v>
       </c>
     </row>
     <row r="300" spans="1:4">
@@ -4612,7 +4612,7 @@
         <v>115</v>
       </c>
       <c r="D300">
-        <v>0.4239990492419127</v>
+        <v>0.400348618600027</v>
       </c>
     </row>
     <row r="301" spans="1:4">
@@ -4626,7 +4626,7 @@
         <v>116</v>
       </c>
       <c r="D301">
-        <v>0.4212014511103019</v>
+        <v>0.3952840454785942</v>
       </c>
     </row>
     <row r="302" spans="1:4">
@@ -4640,7 +4640,7 @@
         <v>117</v>
       </c>
       <c r="D302">
-        <v>0.418385396758416</v>
+        <v>0.3901582401396023</v>
       </c>
     </row>
     <row r="303" spans="1:4">
@@ -4654,7 +4654,7 @@
         <v>118</v>
       </c>
       <c r="D303">
-        <v>0.415550886186255</v>
+        <v>0.3849709067089417</v>
       </c>
     </row>
     <row r="304" spans="1:4">
@@ -4668,7 +4668,7 @@
         <v>119</v>
       </c>
       <c r="D304">
-        <v>0.412697919393819</v>
+        <v>0.379721749312503</v>
       </c>
     </row>
     <row r="305" spans="1:4">
@@ -4682,7 +4682,7 @@
         <v>120</v>
       </c>
       <c r="D305">
-        <v>0.4098264963811081</v>
+        <v>0.3744104720761767</v>
       </c>
     </row>
     <row r="306" spans="1:4">
@@ -4696,7 +4696,7 @@
         <v>121</v>
       </c>
       <c r="D306">
-        <v>0.4069366171481221</v>
+        <v>0.3690367791258534</v>
       </c>
     </row>
     <row r="307" spans="1:4">
@@ -4710,7 +4710,7 @@
         <v>122</v>
       </c>
       <c r="D307">
-        <v>0.404028281694861</v>
+        <v>0.3636003745874236</v>
       </c>
     </row>
     <row r="308" spans="1:4">
@@ -4724,7 +4724,7 @@
         <v>123</v>
       </c>
       <c r="D308">
-        <v>0.4011014900213249</v>
+        <v>0.3581009625867779</v>
       </c>
     </row>
     <row r="309" spans="1:4">
@@ -4738,7 +4738,7 @@
         <v>124</v>
       </c>
       <c r="D309">
-        <v>0.398156242127514</v>
+        <v>0.3525382472498068</v>
       </c>
     </row>
     <row r="310" spans="1:4">
@@ -4752,7 +4752,7 @@
         <v>125</v>
       </c>
       <c r="D310">
-        <v>0.3951925380134279</v>
+        <v>0.3469119327024007</v>
       </c>
     </row>
     <row r="311" spans="1:4">
@@ -4766,7 +4766,7 @@
         <v>126</v>
       </c>
       <c r="D311">
-        <v>0.3922103776790667</v>
+        <v>0.3412217230704503</v>
       </c>
     </row>
     <row r="312" spans="1:4">
@@ -4780,7 +4780,7 @@
         <v>127</v>
       </c>
       <c r="D312">
-        <v>0.3892097611244305</v>
+        <v>0.3354673224798464</v>
       </c>
     </row>
     <row r="313" spans="1:4">
@@ -4794,7 +4794,7 @@
         <v>128</v>
       </c>
       <c r="D313">
-        <v>0.3861906883495195</v>
+        <v>0.3296484350564791</v>
       </c>
     </row>
     <row r="314" spans="1:4">
@@ -4808,7 +4808,7 @@
         <v>129</v>
       </c>
       <c r="D314">
-        <v>0.3831531593543333</v>
+        <v>0.323764764926239</v>
       </c>
     </row>
     <row r="315" spans="1:4">
@@ -4822,7 +4822,7 @@
         <v>130</v>
       </c>
       <c r="D315">
-        <v>0.380097174138872</v>
+        <v>0.3178160162150168</v>
       </c>
     </row>
     <row r="316" spans="1:4">
@@ -4836,7 +4836,7 @@
         <v>131</v>
       </c>
       <c r="D316">
-        <v>0.3770227327031357</v>
+        <v>0.311801893048703</v>
       </c>
     </row>
     <row r="317" spans="1:4">
@@ -4850,7 +4850,7 @@
         <v>132</v>
       </c>
       <c r="D317">
-        <v>0.3739298350471245</v>
+        <v>0.3057220995531882</v>
       </c>
     </row>
     <row r="318" spans="1:4">
@@ -4864,7 +4864,7 @@
         <v>133</v>
       </c>
       <c r="D318">
-        <v>0.3708184811708382</v>
+        <v>0.2995763398543627</v>
       </c>
     </row>
     <row r="319" spans="1:4">
@@ -4878,7 +4878,7 @@
         <v>134</v>
       </c>
       <c r="D319">
-        <v>0.3676886710742768</v>
+        <v>0.2933643180781174</v>
       </c>
     </row>
     <row r="320" spans="1:4">
@@ -4892,7 +4892,7 @@
         <v>135</v>
       </c>
       <c r="D320">
-        <v>0.3645404047574404</v>
+        <v>0.2870857383503425</v>
       </c>
     </row>
     <row r="321" spans="1:4">
@@ -4906,7 +4906,7 @@
         <v>136</v>
       </c>
       <c r="D321">
-        <v>0.3613736822203292</v>
+        <v>0.2807403047969287</v>
       </c>
     </row>
     <row r="322" spans="1:4">
@@ -4920,7 +4920,7 @@
         <v>137</v>
       </c>
       <c r="D322">
-        <v>0.3581885034629427</v>
+        <v>0.2743277215437667</v>
       </c>
     </row>
     <row r="323" spans="1:4">
@@ -4934,7 +4934,7 @@
         <v>138</v>
       </c>
       <c r="D323">
-        <v>0.3549848684852813</v>
+        <v>0.2678476927167464</v>
       </c>
     </row>
     <row r="324" spans="1:4">
@@ -4948,7 +4948,7 @@
         <v>139</v>
       </c>
       <c r="D324">
-        <v>0.3517627772873448</v>
+        <v>0.2612999224417591</v>
       </c>
     </row>
     <row r="325" spans="1:4">
@@ -4962,7 +4962,7 @@
         <v>140</v>
       </c>
       <c r="D325">
-        <v>0.3485222298691333</v>
+        <v>0.2546841148446952</v>
       </c>
     </row>
     <row r="326" spans="1:4">
@@ -4976,7 +4976,7 @@
         <v>141</v>
       </c>
       <c r="D326">
-        <v>0.3452632262306469</v>
+        <v>0.2479999740514451</v>
       </c>
     </row>
     <row r="327" spans="1:4">
@@ -4990,7 +4990,7 @@
         <v>142</v>
       </c>
       <c r="D327">
-        <v>0.3419857663718854</v>
+        <v>0.2412472041878994</v>
       </c>
     </row>
     <row r="328" spans="1:4">
@@ -5004,7 +5004,7 @@
         <v>143</v>
       </c>
       <c r="D328">
-        <v>0.3386898502928488</v>
+        <v>0.2344255093799485</v>
       </c>
     </row>
     <row r="329" spans="1:4">
@@ -5018,7 +5018,7 @@
         <v>144</v>
       </c>
       <c r="D329">
-        <v>0.3353754779935372</v>
+        <v>0.227534593753483</v>
       </c>
     </row>
     <row r="330" spans="1:4">
@@ -5032,7 +5032,7 @@
         <v>145</v>
       </c>
       <c r="D330">
-        <v>0.3320426494739507</v>
+        <v>0.2205741614343935</v>
       </c>
     </row>
     <row r="331" spans="1:4">
@@ -5046,7 +5046,7 @@
         <v>146</v>
       </c>
       <c r="D331">
-        <v>0.3286913647340891</v>
+        <v>0.2135439165485706</v>
       </c>
     </row>
     <row r="332" spans="1:4">
@@ -5060,7 +5060,7 @@
         <v>147</v>
       </c>
       <c r="D332">
-        <v>0.3253216237739524</v>
+        <v>0.2064435632219047</v>
       </c>
     </row>
     <row r="333" spans="1:4">
@@ -5074,7 +5074,7 @@
         <v>148</v>
       </c>
       <c r="D333">
-        <v>0.3219334265935407</v>
+        <v>0.1992728055802864</v>
       </c>
     </row>
     <row r="334" spans="1:4">
@@ -5088,7 +5088,7 @@
         <v>149</v>
       </c>
       <c r="D334">
-        <v>0.3185267731928541</v>
+        <v>0.1920313477496062</v>
       </c>
     </row>
     <row r="335" spans="1:4">
@@ -5102,7 +5102,7 @@
         <v>150</v>
       </c>
       <c r="D335">
-        <v>0.3151016635718924</v>
+        <v>0.1847188938557547</v>
       </c>
     </row>
     <row r="336" spans="1:4">
@@ -5116,7 +5116,7 @@
         <v>151</v>
       </c>
       <c r="D336">
-        <v>0.3116580977306556</v>
+        <v>0.1773351480246225</v>
       </c>
     </row>
     <row r="337" spans="1:4">
@@ -5130,7 +5130,7 @@
         <v>152</v>
       </c>
       <c r="D337">
-        <v>0.3081960756691438</v>
+        <v>0.1698798143821</v>
       </c>
     </row>
     <row r="338" spans="1:4">
@@ -5144,7 +5144,7 @@
         <v>153</v>
       </c>
       <c r="D338">
-        <v>0.3047155973873571</v>
+        <v>0.1623525970540778</v>
       </c>
     </row>
     <row r="339" spans="1:4">
@@ -5158,7 +5158,7 @@
         <v>154</v>
       </c>
       <c r="D339">
-        <v>0.3012166628852952</v>
+        <v>0.1547532001664465</v>
       </c>
     </row>
     <row r="340" spans="1:4">
@@ -5172,7 +5172,7 @@
         <v>155</v>
       </c>
       <c r="D340">
-        <v>0.2976992721629584</v>
+        <v>0.1470813278450965</v>
       </c>
     </row>
     <row r="341" spans="1:4">
@@ -5186,7 +5186,7 @@
         <v>156</v>
       </c>
       <c r="D341">
-        <v>0.2941634252203465</v>
+        <v>0.1393366842159186</v>
       </c>
     </row>
     <row r="342" spans="1:4">
@@ -5200,7 +5200,7 @@
         <v>157</v>
       </c>
       <c r="D342">
-        <v>0.2906091220574597</v>
+        <v>0.131518973404803</v>
       </c>
     </row>
     <row r="343" spans="1:4">
@@ -5214,7 +5214,7 @@
         <v>158</v>
       </c>
       <c r="D343">
-        <v>0.2870363626742978</v>
+        <v>0.1236278995376405</v>
       </c>
     </row>
     <row r="344" spans="1:4">
@@ -5228,7 +5228,7 @@
         <v>159</v>
       </c>
       <c r="D344">
-        <v>0.2834451470708608</v>
+        <v>0.1156631667403216</v>
       </c>
     </row>
     <row r="345" spans="1:4">
@@ -5242,7 +5242,7 @@
         <v>160</v>
       </c>
       <c r="D345">
-        <v>0.2798354752471488</v>
+        <v>0.1076244791387367</v>
       </c>
     </row>
     <row r="346" spans="1:4">
@@ -5256,7 +5256,7 @@
         <v>161</v>
       </c>
       <c r="D346">
-        <v>0.2762073472031619</v>
+        <v>0.09951154085877656</v>
       </c>
     </row>
     <row r="347" spans="1:4">
@@ -5270,7 +5270,7 @@
         <v>162</v>
       </c>
       <c r="D347">
-        <v>0.2725607629388999</v>
+        <v>0.09132405602633153</v>
       </c>
     </row>
     <row r="348" spans="1:4">
@@ -5284,7 +5284,7 @@
         <v>163</v>
       </c>
       <c r="D348">
-        <v>0.2688957224543628</v>
+        <v>0.08306172876729218</v>
       </c>
     </row>
     <row r="349" spans="1:4">
@@ -5298,7 +5298,7 @@
         <v>164</v>
       </c>
       <c r="D349">
-        <v>0.2652122257495507</v>
+        <v>0.07472426320754916</v>
       </c>
     </row>
     <row r="350" spans="1:4">
@@ -5312,7 +5312,7 @@
         <v>165</v>
       </c>
       <c r="D350">
-        <v>0.2615102728244638</v>
+        <v>0.06631136347299299</v>
       </c>
     </row>
     <row r="351" spans="1:4">
@@ -5326,7 +5326,7 @@
         <v>166</v>
       </c>
       <c r="D351">
-        <v>0.2577898636791016</v>
+        <v>0.05782273368951413</v>
       </c>
     </row>
     <row r="352" spans="1:4">
@@ -5340,7 +5340,7 @@
         <v>167</v>
       </c>
       <c r="D352">
-        <v>0.2540509983134644</v>
+        <v>0.04925807798300319</v>
       </c>
     </row>
     <row r="353" spans="1:4">
@@ -5354,7 +5354,7 @@
         <v>168</v>
       </c>
       <c r="D353">
-        <v>0.2502936767275522</v>
+        <v>0.04061710047935069</v>
       </c>
     </row>
     <row r="354" spans="1:4">
@@ -5368,7 +5368,7 @@
         <v>169</v>
       </c>
       <c r="D354">
-        <v>0.2465178989213652</v>
+        <v>0.03189950530444713</v>
       </c>
     </row>
     <row r="355" spans="1:4">
@@ -5382,7 +5382,7 @@
         <v>170</v>
       </c>
       <c r="D355">
-        <v>0.2427236648949029</v>
+        <v>0.02310499658418308</v>
       </c>
     </row>
     <row r="356" spans="1:4">
@@ -5396,7 +5396,7 @@
         <v>171</v>
       </c>
       <c r="D356">
-        <v>0.2389109746481657</v>
+        <v>0.01423327844444916</v>
       </c>
     </row>
     <row r="357" spans="1:4">
@@ -5410,7 +5410,7 @@
         <v>172</v>
       </c>
       <c r="D357">
-        <v>0.2350798281811534</v>
+        <v>0.005284055011135769</v>
       </c>
     </row>
     <row r="358" spans="1:4">
@@ -5424,7 +5424,7 @@
         <v>173</v>
       </c>
       <c r="D358">
-        <v>0.2312302254938662</v>
+        <v>0.005284055011135769</v>
       </c>
     </row>
     <row r="359" spans="1:4">
@@ -5438,7 +5438,7 @@
         <v>174</v>
       </c>
       <c r="D359">
-        <v>0.2273621665863039</v>
+        <v>0.005284055011135769</v>
       </c>
     </row>
     <row r="360" spans="1:4">
@@ -5452,7 +5452,7 @@
         <v>175</v>
       </c>
       <c r="D360">
-        <v>0.2234756514584665</v>
+        <v>0.005284055011135769</v>
       </c>
     </row>
     <row r="361" spans="1:4">
@@ -5466,7 +5466,7 @@
         <v>176</v>
       </c>
       <c r="D361">
-        <v>0.2195706801103541</v>
+        <v>0.005284055011135769</v>
       </c>
     </row>
     <row r="362" spans="1:4">
@@ -5480,7 +5480,7 @@
         <v>177</v>
       </c>
       <c r="D362">
-        <v>0.2156472525419668</v>
+        <v>0.005284055011135769</v>
       </c>
     </row>
     <row r="363" spans="1:4">
@@ -5494,7 +5494,7 @@
         <v>178</v>
       </c>
       <c r="D363">
-        <v>0.2117053687533044</v>
+        <v>0.005284055011135769</v>
       </c>
     </row>
     <row r="364" spans="1:4">
@@ -5508,7 +5508,7 @@
         <v>179</v>
       </c>
       <c r="D364">
-        <v>0.2077450287443669</v>
+        <v>0.005284055011135769</v>
       </c>
     </row>
     <row r="365" spans="1:4">
@@ -5522,7 +5522,7 @@
         <v>180</v>
       </c>
       <c r="D365">
-        <v>0.2037662325151544</v>
+        <v>0.005284055011135769</v>
       </c>
     </row>
     <row r="366" spans="1:4">
@@ -5536,7 +5536,7 @@
         <v>181</v>
       </c>
       <c r="D366">
-        <v>0.1997689800656671</v>
+        <v>0.005284055011135769</v>
       </c>
     </row>
   </sheetData>
@@ -5577,7 +5577,7 @@
         <v>26</v>
       </c>
       <c r="D2">
-        <v>0.4434550084189977</v>
+        <v>0.4999202621011481</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -5591,7 +5591,7 @@
         <v>27</v>
       </c>
       <c r="D3">
-        <v>0.4615963357398717</v>
+        <v>0.5010202998862483</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -5605,7 +5605,7 @@
         <v>28</v>
       </c>
       <c r="D4">
-        <v>0.4788333082672697</v>
+        <v>0.5033098322749846</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -5619,7 +5619,7 @@
         <v>29</v>
       </c>
       <c r="D5">
-        <v>0.4951659260011914</v>
+        <v>0.506687374447813</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -5633,7 +5633,7 @@
         <v>30</v>
       </c>
       <c r="D6">
-        <v>0.510594188941637</v>
+        <v>0.5110514415851893</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -5647,7 +5647,7 @@
         <v>31</v>
       </c>
       <c r="D7">
-        <v>0.5251180970886062</v>
+        <v>0.5163005488675693</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -5661,7 +5661,7 @@
         <v>32</v>
       </c>
       <c r="D8">
-        <v>0.5387376504420994</v>
+        <v>0.522333211475409</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -5675,7 +5675,7 @@
         <v>33</v>
       </c>
       <c r="D9">
-        <v>0.5514528490021163</v>
+        <v>0.5290479445891642</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -5689,7 +5689,7 @@
         <v>34</v>
       </c>
       <c r="D10">
-        <v>0.563263692768657</v>
+        <v>0.5363432633892906</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -5703,7 +5703,7 @@
         <v>35</v>
       </c>
       <c r="D11">
-        <v>0.5741701817417215</v>
+        <v>0.5441176830562443</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -5717,7 +5717,7 @@
         <v>36</v>
       </c>
       <c r="D12">
-        <v>0.5841723159213098</v>
+        <v>0.5522697187704811</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -5731,7 +5731,7 @@
         <v>37</v>
       </c>
       <c r="D13">
-        <v>0.5932700953074219</v>
+        <v>0.5606978857124567</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -5745,7 +5745,7 @@
         <v>38</v>
       </c>
       <c r="D14">
-        <v>0.6014635199000578</v>
+        <v>0.5693006990626269</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -5759,7 +5759,7 @@
         <v>39</v>
       </c>
       <c r="D15">
-        <v>0.6087525896992174</v>
+        <v>0.577976674001448</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -5773,7 +5773,7 @@
         <v>40</v>
       </c>
       <c r="D16">
-        <v>0.6151373047049009</v>
+        <v>0.5866243257093754</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -5787,7 +5787,7 @@
         <v>41</v>
       </c>
       <c r="D17">
-        <v>0.6206176649171081</v>
+        <v>0.5951421693668651</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -5801,7 +5801,7 @@
         <v>42</v>
       </c>
       <c r="D18">
-        <v>0.6251936703358393</v>
+        <v>0.6034287201543729</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -5815,7 +5815,7 @@
         <v>43</v>
       </c>
       <c r="D19">
-        <v>0.628865320961094</v>
+        <v>0.6113824932523547</v>
       </c>
     </row>
     <row r="20" spans="1:4">
@@ -5829,7 +5829,7 @@
         <v>44</v>
       </c>
       <c r="D20">
-        <v>0.6316326167928726</v>
+        <v>0.6189020038412665</v>
       </c>
     </row>
     <row r="21" spans="1:4">
@@ -5843,7 +5843,7 @@
         <v>45</v>
       </c>
       <c r="D21">
-        <v>0.6334955578311751</v>
+        <v>0.625885767101564</v>
       </c>
     </row>
     <row r="22" spans="1:4">
@@ -5857,7 +5857,7 @@
         <v>46</v>
       </c>
       <c r="D22">
-        <v>0.6344541440760013</v>
+        <v>0.632232298213703</v>
       </c>
     </row>
     <row r="23" spans="1:4">
@@ -5871,7 +5871,7 @@
         <v>47</v>
       </c>
       <c r="D23">
-        <v>0.6345083755273515</v>
+        <v>0.6378401123581395</v>
       </c>
     </row>
     <row r="24" spans="1:4">
@@ -5885,7 +5885,7 @@
         <v>48</v>
       </c>
       <c r="D24">
-        <v>0.6336582521852251</v>
+        <v>0.6426077247153293</v>
       </c>
     </row>
     <row r="25" spans="1:4">
@@ -5899,7 +5899,7 @@
         <v>49</v>
       </c>
       <c r="D25">
-        <v>0.6319037740496228</v>
+        <v>0.6464336504657282</v>
       </c>
     </row>
     <row r="26" spans="1:4">
@@ -5913,7 +5913,7 @@
         <v>50</v>
       </c>
       <c r="D26">
-        <v>0.6292449411205442</v>
+        <v>0.6492164047897921</v>
       </c>
     </row>
     <row r="27" spans="1:4">
@@ -5927,7 +5927,7 @@
         <v>51</v>
       </c>
       <c r="D27">
-        <v>0.6256817533979894</v>
+        <v>0.650854502867977</v>
       </c>
     </row>
     <row r="28" spans="1:4">
@@ -5941,7 +5941,7 @@
         <v>52</v>
       </c>
       <c r="D28">
-        <v>0.6212142108819584</v>
+        <v>0.6512464598807384</v>
       </c>
     </row>
     <row r="29" spans="1:4">
@@ -5955,7 +5955,7 @@
         <v>1</v>
       </c>
       <c r="D29">
-        <v>0.6158423135724512</v>
+        <v>0.6502907910085324</v>
       </c>
     </row>
     <row r="30" spans="1:4">
@@ -5969,7 +5969,7 @@
         <v>2</v>
       </c>
       <c r="D30">
-        <v>0.6095660614694678</v>
+        <v>0.6478860114318147</v>
       </c>
     </row>
     <row r="31" spans="1:4">
@@ -5983,7 +5983,7 @@
         <v>3</v>
       </c>
       <c r="D31">
-        <v>0.6023854545730083</v>
+        <v>0.6439306363310414</v>
       </c>
     </row>
     <row r="32" spans="1:4">
@@ -5997,7 +5997,7 @@
         <v>4</v>
       </c>
       <c r="D32">
-        <v>0.5943004928830724</v>
+        <v>0.6383231808866682</v>
       </c>
     </row>
     <row r="33" spans="1:4">
@@ -6011,7 +6011,7 @@
         <v>5</v>
       </c>
       <c r="D33">
-        <v>0.5853111763996602</v>
+        <v>0.630962160279151</v>
       </c>
     </row>
     <row r="34" spans="1:4">
@@ -6025,7 +6025,7 @@
         <v>6</v>
       </c>
       <c r="D34">
-        <v>0.5754175051227721</v>
+        <v>0.6217460896889454</v>
       </c>
     </row>
     <row r="35" spans="1:4">
@@ -6039,7 +6039,7 @@
         <v>7</v>
       </c>
       <c r="D35">
-        <v>0.5646194790524077</v>
+        <v>0.6105734842965077</v>
       </c>
     </row>
     <row r="36" spans="1:4">
@@ -6053,7 +6053,7 @@
         <v>8</v>
       </c>
       <c r="D36">
-        <v>0.552917098188567</v>
+        <v>0.5973428592822935</v>
       </c>
     </row>
     <row r="37" spans="1:4">
@@ -6067,7 +6067,7 @@
         <v>9</v>
       </c>
       <c r="D37">
-        <v>0.5403103625312502</v>
+        <v>0.5819527298267586</v>
       </c>
     </row>
     <row r="38" spans="1:4">
@@ -6081,7 +6081,7 @@
         <v>10</v>
       </c>
       <c r="D38">
-        <v>0.5267992720804572</v>
+        <v>0.5643016111103593</v>
       </c>
     </row>
     <row r="39" spans="1:4">
@@ -6095,7 +6095,7 @@
         <v>11</v>
       </c>
       <c r="D39">
-        <v>0.5123838268361879</v>
+        <v>0.5442880183135507</v>
       </c>
     </row>
     <row r="40" spans="1:4">
@@ -6109,7 +6109,7 @@
         <v>12</v>
       </c>
       <c r="D40">
-        <v>0.4970640267984424</v>
+        <v>0.5218104666167891</v>
       </c>
     </row>
     <row r="41" spans="1:4">
@@ -6123,7 +6123,7 @@
         <v>13</v>
       </c>
       <c r="D41">
-        <v>0.4808398719672207</v>
+        <v>0.4967674712005303</v>
       </c>
     </row>
     <row r="42" spans="1:4">
@@ -6137,7 +6137,7 @@
         <v>14</v>
       </c>
       <c r="D42">
-        <v>0.4637113623425229</v>
+        <v>0.4690575472452303</v>
       </c>
     </row>
     <row r="43" spans="1:4">
@@ -6151,7 +6151,7 @@
         <v>15</v>
       </c>
       <c r="D43">
-        <v>0.4456784979243489</v>
+        <v>0.4385792099313446</v>
       </c>
     </row>
     <row r="44" spans="1:4">
@@ -6165,7 +6165,7 @@
         <v>16</v>
       </c>
       <c r="D44">
-        <v>0.4267412787126985</v>
+        <v>0.4052309744393295</v>
       </c>
     </row>
     <row r="45" spans="1:4">
@@ -6179,7 +6179,7 @@
         <v>17</v>
       </c>
       <c r="D45">
-        <v>0.406899704707572</v>
+        <v>0.3689113559496405</v>
       </c>
     </row>
     <row r="46" spans="1:4">
@@ -6193,7 +6193,7 @@
         <v>18</v>
       </c>
       <c r="D46">
-        <v>0.3861537759089693</v>
+        <v>0.3295188696427336</v>
       </c>
     </row>
     <row r="47" spans="1:4">
@@ -6207,7 +6207,7 @@
         <v>19</v>
       </c>
       <c r="D47">
-        <v>0.3645034923168904</v>
+        <v>0.2869520306990647</v>
       </c>
     </row>
     <row r="48" spans="1:4">
@@ -6221,7 +6221,7 @@
         <v>20</v>
       </c>
       <c r="D48">
-        <v>0.3419488539313353</v>
+        <v>0.2411093542990891</v>
       </c>
     </row>
     <row r="49" spans="1:4">
@@ -6235,7 +6235,7 @@
         <v>21</v>
       </c>
       <c r="D49">
-        <v>0.318489860752304</v>
+        <v>0.1918893556232635</v>
       </c>
     </row>
     <row r="50" spans="1:4">
@@ -6249,7 +6249,7 @@
         <v>22</v>
       </c>
       <c r="D50">
-        <v>0.2941265127797965</v>
+        <v>0.1391905498520435</v>
       </c>
     </row>
     <row r="51" spans="1:4">
@@ -6263,7 +6263,7 @@
         <v>23</v>
       </c>
       <c r="D51">
-        <v>0.2688588100138128</v>
+        <v>0.08291145216588476</v>
       </c>
     </row>
     <row r="52" spans="1:4">
@@ -6277,7 +6277,7 @@
         <v>24</v>
       </c>
       <c r="D52">
-        <v>0.2426867524543529</v>
+        <v>0.02424015268824354</v>
       </c>
     </row>
     <row r="53" spans="1:4">
@@ -6291,7 +6291,7 @@
         <v>25</v>
       </c>
       <c r="D53">
-        <v>0.2156103401014167</v>
+        <v>0.005284055011135769</v>
       </c>
     </row>
   </sheetData>
@@ -6332,7 +6332,7 @@
         <v>7</v>
       </c>
       <c r="D2">
-        <v>0.4732994037046516</v>
+        <v>0.503406469767758</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -6346,7 +6346,7 @@
         <v>8</v>
       </c>
       <c r="D3">
-        <v>0.5399081396696188</v>
+        <v>0.5237707760583156</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -6360,7 +6360,7 @@
         <v>9</v>
       </c>
       <c r="D4">
-        <v>0.588179823152965</v>
+        <v>0.556618728880796</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -6374,7 +6374,7 @@
         <v>10</v>
       </c>
       <c r="D5">
-        <v>0.6191887886057382</v>
+        <v>0.5937690015890918</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -6388,7 +6388,7 @@
         <v>11</v>
       </c>
       <c r="D6">
-        <v>0.6331226742674013</v>
+        <v>0.6268259774968072</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -6402,7 +6402,7 @@
         <v>12</v>
       </c>
       <c r="D7">
-        <v>0.6297938418984913</v>
+        <v>0.6473040773505002</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -6416,7 +6416,7 @@
         <v>1</v>
       </c>
       <c r="D8">
-        <v>0.6088647250990167</v>
+        <v>0.6466835087805062</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -6430,7 +6430,7 @@
         <v>2</v>
       </c>
       <c r="D9">
-        <v>0.57261455255612</v>
+        <v>0.618283700309273</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -6444,7 +6444,7 @@
         <v>3</v>
       </c>
       <c r="D10">
-        <v>0.5200306250698267</v>
+        <v>0.5541537046725179</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -6458,7 +6458,7 @@
         <v>4</v>
       </c>
       <c r="D11">
-        <v>0.4489643882548638</v>
+        <v>0.4432873880037798</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -6472,7 +6472,7 @@
         <v>5</v>
       </c>
       <c r="D12">
-        <v>0.3606354334093281</v>
+        <v>0.2780543168069942</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -6486,7 +6486,7 @@
         <v>6</v>
       </c>
       <c r="D13">
-        <v>0.2552313987726821</v>
+        <v>0.06455157791381295</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Incorporated API updates which includes Tmin Tmax T_24hour_avg and heat_units.  Added try-except block where try-block uses WMA and except-block uses Polynomial Fit.
</commit_message>
<xml_diff>
--- a/DATA/collate_cultivar_data/data/binned_kcp_data.xlsx
+++ b/DATA/collate_cultivar_data/data/binned_kcp_data.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="day_frequency" sheetId="1" state="visible" r:id="rId2"/>
@@ -175,8 +175,8 @@
   </sheetPr>
   <dimension ref="A1:D367"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F17" activeCellId="0" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -213,7 +213,7 @@
         <v>182</v>
       </c>
       <c r="D2" s="0" t="n">
-        <v>0.1152267</v>
+        <v>0.0854995</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -227,7 +227,7 @@
         <v>183</v>
       </c>
       <c r="D3" s="0" t="n">
-        <v>0.1152795</v>
+        <v>0.0854995</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -241,7 +241,7 @@
         <v>184</v>
       </c>
       <c r="D4" s="0" t="n">
-        <v>0.1153333</v>
+        <v>0.0854995</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -255,7 +255,7 @@
         <v>185</v>
       </c>
       <c r="D5" s="0" t="n">
-        <v>0.115388</v>
+        <v>0.0854995</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -269,7 +269,7 @@
         <v>186</v>
       </c>
       <c r="D6" s="0" t="n">
-        <v>0.1154437</v>
+        <v>0.0854995</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -283,7 +283,7 @@
         <v>187</v>
       </c>
       <c r="D7" s="0" t="n">
-        <v>0.1155002</v>
+        <v>0.0854995</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -297,7 +297,7 @@
         <v>188</v>
       </c>
       <c r="D8" s="0" t="n">
-        <v>0.1155576</v>
+        <v>0.0854995</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -311,7 +311,7 @@
         <v>189</v>
       </c>
       <c r="D9" s="0" t="n">
-        <v>0.1156159</v>
+        <v>0.0854995</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -325,7 +325,7 @@
         <v>190</v>
       </c>
       <c r="D10" s="0" t="n">
-        <v>0.115675</v>
+        <v>0.0854995</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -339,7 +339,7 @@
         <v>191</v>
       </c>
       <c r="D11" s="0" t="n">
-        <v>0.1157349</v>
+        <v>0.0854995</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -353,7 +353,7 @@
         <v>192</v>
       </c>
       <c r="D12" s="0" t="n">
-        <v>0.1157954</v>
+        <v>0.0854995</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -367,7 +367,7 @@
         <v>193</v>
       </c>
       <c r="D13" s="0" t="n">
-        <v>0.1158566</v>
+        <v>0.0854995</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -381,7 +381,7 @@
         <v>194</v>
       </c>
       <c r="D14" s="0" t="n">
-        <v>0.1159184</v>
+        <v>0.0854995</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -395,7 +395,7 @@
         <v>195</v>
       </c>
       <c r="D15" s="0" t="n">
-        <v>0.1159807</v>
+        <v>0.0854995</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -409,7 +409,7 @@
         <v>196</v>
       </c>
       <c r="D16" s="0" t="n">
-        <v>0.1160434</v>
+        <v>0.0854995</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -423,7 +423,7 @@
         <v>197</v>
       </c>
       <c r="D17" s="0" t="n">
-        <v>0.1161064</v>
+        <v>0.0854995</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -437,7 +437,7 @@
         <v>198</v>
       </c>
       <c r="D18" s="0" t="n">
-        <v>0.1161697</v>
+        <v>0.0854995</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -451,7 +451,7 @@
         <v>199</v>
       </c>
       <c r="D19" s="0" t="n">
-        <v>0.116233</v>
+        <v>0.0854995</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -465,7 +465,7 @@
         <v>200</v>
       </c>
       <c r="D20" s="0" t="n">
-        <v>0.1162963</v>
+        <v>0.0854995</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -479,7 +479,7 @@
         <v>201</v>
       </c>
       <c r="D21" s="0" t="n">
-        <v>0.1163594</v>
+        <v>0.0854995</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -493,7 +493,7 @@
         <v>202</v>
       </c>
       <c r="D22" s="0" t="n">
-        <v>0.1164221</v>
+        <v>0.0854995</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -507,7 +507,7 @@
         <v>203</v>
       </c>
       <c r="D23" s="0" t="n">
-        <v>0.1164844</v>
+        <v>0.0854995</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -521,7 +521,7 @@
         <v>204</v>
       </c>
       <c r="D24" s="0" t="n">
-        <v>0.116546</v>
+        <v>0.0854995</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -535,7 +535,7 @@
         <v>205</v>
       </c>
       <c r="D25" s="0" t="n">
-        <v>0.1166067</v>
+        <v>0.0854995</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -549,7 +549,7 @@
         <v>206</v>
       </c>
       <c r="D26" s="0" t="n">
-        <v>0.1166663</v>
+        <v>0.0854995</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -563,7 +563,7 @@
         <v>207</v>
       </c>
       <c r="D27" s="0" t="n">
-        <v>0.1167247</v>
+        <v>0.0854995</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -577,7 +577,7 @@
         <v>208</v>
       </c>
       <c r="D28" s="0" t="n">
-        <v>0.1167815</v>
+        <v>0.0854995</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -591,7 +591,7 @@
         <v>209</v>
       </c>
       <c r="D29" s="0" t="n">
-        <v>0.1168366</v>
+        <v>0.0854995</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -605,7 +605,7 @@
         <v>210</v>
       </c>
       <c r="D30" s="0" t="n">
-        <v>0.1168897</v>
+        <v>0.0854995</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -619,7 +619,7 @@
         <v>211</v>
       </c>
       <c r="D31" s="0" t="n">
-        <v>0.1169406</v>
+        <v>0.0854995</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -633,7 +633,7 @@
         <v>212</v>
       </c>
       <c r="D32" s="0" t="n">
-        <v>0.1169891</v>
+        <v>0.0854995</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -647,7 +647,7 @@
         <v>213</v>
       </c>
       <c r="D33" s="0" t="n">
-        <v>0.117035</v>
+        <v>0.0854995</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -661,7 +661,7 @@
         <v>214</v>
       </c>
       <c r="D34" s="0" t="n">
-        <v>0.1170781</v>
+        <v>0.0854995</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -675,7 +675,7 @@
         <v>215</v>
       </c>
       <c r="D35" s="0" t="n">
-        <v>0.1171182</v>
+        <v>0.0854995</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -689,7 +689,7 @@
         <v>216</v>
       </c>
       <c r="D36" s="0" t="n">
-        <v>0.1171551</v>
+        <v>0.0854995</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -703,7 +703,7 @@
         <v>217</v>
       </c>
       <c r="D37" s="0" t="n">
-        <v>0.1171887</v>
+        <v>0.0854995</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -717,7 +717,7 @@
         <v>218</v>
       </c>
       <c r="D38" s="0" t="n">
-        <v>0.1172191</v>
+        <v>0.0854995</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -731,7 +731,7 @@
         <v>219</v>
       </c>
       <c r="D39" s="0" t="n">
-        <v>0.1172461</v>
+        <v>0.0854995</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -745,7 +745,7 @@
         <v>220</v>
       </c>
       <c r="D40" s="0" t="n">
-        <v>0.11727</v>
+        <v>0.0854995</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -759,7 +759,7 @@
         <v>221</v>
       </c>
       <c r="D41" s="0" t="n">
-        <v>0.1172908</v>
+        <v>0.0854995</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -773,7 +773,7 @@
         <v>222</v>
       </c>
       <c r="D42" s="0" t="n">
-        <v>0.1173088</v>
+        <v>0.0854995</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -787,7 +787,7 @@
         <v>223</v>
       </c>
       <c r="D43" s="0" t="n">
-        <v>0.1173244</v>
+        <v>0.0854995</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -801,7 +801,7 @@
         <v>224</v>
       </c>
       <c r="D44" s="0" t="n">
-        <v>0.1173381</v>
+        <v>0.0854995</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -815,7 +815,7 @@
         <v>225</v>
       </c>
       <c r="D45" s="0" t="n">
-        <v>0.1173505</v>
+        <v>0.0854995</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -829,7 +829,7 @@
         <v>226</v>
       </c>
       <c r="D46" s="0" t="n">
-        <v>0.1173624</v>
+        <v>0.0854995</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -843,7 +843,7 @@
         <v>227</v>
       </c>
       <c r="D47" s="0" t="n">
-        <v>0.1173747</v>
+        <v>0.0854995</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -857,7 +857,7 @@
         <v>228</v>
       </c>
       <c r="D48" s="0" t="n">
-        <v>0.1173886</v>
+        <v>0.0854995</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -871,7 +871,7 @@
         <v>229</v>
       </c>
       <c r="D49" s="0" t="n">
-        <v>0.1174052</v>
+        <v>0.0854995</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -885,7 +885,7 @@
         <v>230</v>
       </c>
       <c r="D50" s="0" t="n">
-        <v>0.117426</v>
+        <v>0.0854995</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -899,7 +899,7 @@
         <v>231</v>
       </c>
       <c r="D51" s="0" t="n">
-        <v>0.1174525</v>
+        <v>0.0854995</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -913,7 +913,7 @@
         <v>232</v>
       </c>
       <c r="D52" s="0" t="n">
-        <v>0.1174863</v>
+        <v>0.0854995</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -927,7 +927,7 @@
         <v>233</v>
       </c>
       <c r="D53" s="0" t="n">
-        <v>0.1175294</v>
+        <v>0.0854995</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -941,7 +941,7 @@
         <v>234</v>
       </c>
       <c r="D54" s="0" t="n">
-        <v>0.1175837</v>
+        <v>0.0854995</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -955,7 +955,7 @@
         <v>235</v>
       </c>
       <c r="D55" s="0" t="n">
-        <v>0.1176511</v>
+        <v>0.0855216</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -969,7 +969,7 @@
         <v>236</v>
       </c>
       <c r="D56" s="0" t="n">
-        <v>0.1177337</v>
+        <v>0.0856544</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -983,7 +983,7 @@
         <v>237</v>
       </c>
       <c r="D57" s="0" t="n">
-        <v>0.1178335</v>
+        <v>0.0858959</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -997,7 +997,7 @@
         <v>238</v>
       </c>
       <c r="D58" s="0" t="n">
-        <v>0.1179527</v>
+        <v>0.0862443</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1011,7 +1011,7 @@
         <v>239</v>
       </c>
       <c r="D59" s="0" t="n">
-        <v>0.1180933</v>
+        <v>0.0866975</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1025,7 +1025,7 @@
         <v>240</v>
       </c>
       <c r="D60" s="0" t="n">
-        <v>0.1182571</v>
+        <v>0.0872535</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1039,7 +1039,7 @@
         <v>241</v>
       </c>
       <c r="D61" s="0" t="n">
-        <v>0.1184461</v>
+        <v>0.0879104</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1053,7 +1053,7 @@
         <v>242</v>
       </c>
       <c r="D62" s="0" t="n">
-        <v>0.1186619</v>
+        <v>0.0886664</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1067,7 +1067,7 @@
         <v>243</v>
       </c>
       <c r="D63" s="0" t="n">
-        <v>0.118906</v>
+        <v>0.0895193</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1081,7 +1081,7 @@
         <v>244</v>
       </c>
       <c r="D64" s="0" t="n">
-        <v>0.1191798</v>
+        <v>0.0904674</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1095,7 +1095,7 @@
         <v>245</v>
       </c>
       <c r="D65" s="0" t="n">
-        <v>0.1194844</v>
+        <v>0.0915088</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1109,7 +1109,7 @@
         <v>246</v>
       </c>
       <c r="D66" s="0" t="n">
-        <v>0.1198209</v>
+        <v>0.0926415</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1123,7 +1123,7 @@
         <v>247</v>
       </c>
       <c r="D67" s="0" t="n">
-        <v>0.1201899</v>
+        <v>0.0938637</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1137,7 +1137,7 @@
         <v>248</v>
       </c>
       <c r="D68" s="0" t="n">
-        <v>0.1205919</v>
+        <v>0.0951735</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1151,7 +1151,7 @@
         <v>249</v>
       </c>
       <c r="D69" s="0" t="n">
-        <v>0.1210273</v>
+        <v>0.0965691</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1165,7 +1165,7 @@
         <v>250</v>
       </c>
       <c r="D70" s="0" t="n">
-        <v>0.1214962</v>
+        <v>0.0980486</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1179,7 +1179,7 @@
         <v>251</v>
       </c>
       <c r="D71" s="0" t="n">
-        <v>0.1219986</v>
+        <v>0.0996102</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1193,7 +1193,7 @@
         <v>252</v>
       </c>
       <c r="D72" s="0" t="n">
-        <v>0.1225343</v>
+        <v>0.1012521</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1207,7 +1207,7 @@
         <v>253</v>
       </c>
       <c r="D73" s="0" t="n">
-        <v>0.123103</v>
+        <v>0.1029724</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1221,7 +1221,7 @@
         <v>254</v>
       </c>
       <c r="D74" s="0" t="n">
-        <v>0.1237042</v>
+        <v>0.1047695</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1235,7 +1235,7 @@
         <v>255</v>
       </c>
       <c r="D75" s="0" t="n">
-        <v>0.1243375</v>
+        <v>0.1066414</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1249,7 +1249,7 @@
         <v>256</v>
       </c>
       <c r="D76" s="0" t="n">
-        <v>0.1250022</v>
+        <v>0.1085865</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1263,7 +1263,7 @@
         <v>257</v>
       </c>
       <c r="D77" s="0" t="n">
-        <v>0.1256977</v>
+        <v>0.110603</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1277,7 +1277,7 @@
         <v>258</v>
       </c>
       <c r="D78" s="0" t="n">
-        <v>0.1264235</v>
+        <v>0.1126891</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1291,7 +1291,7 @@
         <v>259</v>
       </c>
       <c r="D79" s="0" t="n">
-        <v>0.1271788</v>
+        <v>0.1148432</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1305,7 +1305,7 @@
         <v>260</v>
       </c>
       <c r="D80" s="0" t="n">
-        <v>0.1279632</v>
+        <v>0.1170634</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1319,7 +1319,7 @@
         <v>261</v>
       </c>
       <c r="D81" s="0" t="n">
-        <v>0.1287759</v>
+        <v>0.119348</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1333,7 +1333,7 @@
         <v>262</v>
       </c>
       <c r="D82" s="0" t="n">
-        <v>0.1296167</v>
+        <v>0.1216955</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1347,7 +1347,7 @@
         <v>263</v>
       </c>
       <c r="D83" s="0" t="n">
-        <v>0.130485</v>
+        <v>0.124104</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1361,7 +1361,7 @@
         <v>264</v>
       </c>
       <c r="D84" s="0" t="n">
-        <v>0.1313806</v>
+        <v>0.126572</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1375,7 +1375,7 @@
         <v>265</v>
       </c>
       <c r="D85" s="0" t="n">
-        <v>0.1323033</v>
+        <v>0.1290978</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1389,7 +1389,7 @@
         <v>266</v>
       </c>
       <c r="D86" s="0" t="n">
-        <v>0.1332531</v>
+        <v>0.1316796</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1403,7 +1403,7 @@
         <v>267</v>
       </c>
       <c r="D87" s="0" t="n">
-        <v>0.1342302</v>
+        <v>0.1343159</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1417,7 +1417,7 @@
         <v>268</v>
       </c>
       <c r="D88" s="0" t="n">
-        <v>0.1352348</v>
+        <v>0.1370051</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1431,7 +1431,7 @@
         <v>269</v>
       </c>
       <c r="D89" s="0" t="n">
-        <v>0.1362673</v>
+        <v>0.1397455</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1445,7 +1445,7 @@
         <v>270</v>
       </c>
       <c r="D90" s="0" t="n">
-        <v>0.1373285</v>
+        <v>0.1425355</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1459,7 +1459,7 @@
         <v>271</v>
       </c>
       <c r="D91" s="0" t="n">
-        <v>0.1384192</v>
+        <v>0.1453736</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1473,7 +1473,7 @@
         <v>272</v>
       </c>
       <c r="D92" s="0" t="n">
-        <v>0.1395406</v>
+        <v>0.1482581</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1487,7 +1487,7 @@
         <v>273</v>
       </c>
       <c r="D93" s="0" t="n">
-        <v>0.1406939</v>
+        <v>0.1511875</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1501,7 +1501,7 @@
         <v>274</v>
       </c>
       <c r="D94" s="0" t="n">
-        <v>0.1418807</v>
+        <v>0.1541603</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1515,7 +1515,7 @@
         <v>275</v>
       </c>
       <c r="D95" s="0" t="n">
-        <v>0.1431029</v>
+        <v>0.1571749</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1529,7 +1529,7 @@
         <v>276</v>
       </c>
       <c r="D96" s="0" t="n">
-        <v>0.1443626</v>
+        <v>0.1602297</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1543,7 +1543,7 @@
         <v>277</v>
       </c>
       <c r="D97" s="0" t="n">
-        <v>0.1456622</v>
+        <v>0.1633233</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1557,7 +1557,7 @@
         <v>278</v>
       </c>
       <c r="D98" s="0" t="n">
-        <v>0.1470044</v>
+        <v>0.1664542</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1571,7 +1571,7 @@
         <v>279</v>
       </c>
       <c r="D99" s="0" t="n">
-        <v>0.1483923</v>
+        <v>0.1696208</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1585,7 +1585,7 @@
         <v>280</v>
       </c>
       <c r="D100" s="0" t="n">
-        <v>0.1498293</v>
+        <v>0.1728216</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1599,7 +1599,7 @@
         <v>281</v>
       </c>
       <c r="D101" s="0" t="n">
-        <v>0.1513191</v>
+        <v>0.1760553</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1613,7 +1613,7 @@
         <v>282</v>
       </c>
       <c r="D102" s="0" t="n">
-        <v>0.1528658</v>
+        <v>0.1793203</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1627,7 +1627,7 @@
         <v>283</v>
       </c>
       <c r="D103" s="0" t="n">
-        <v>0.1544738</v>
+        <v>0.1826152</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1641,7 +1641,7 @@
         <v>284</v>
       </c>
       <c r="D104" s="0" t="n">
-        <v>0.1561481</v>
+        <v>0.1859386</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1655,7 +1655,7 @@
         <v>285</v>
       </c>
       <c r="D105" s="0" t="n">
-        <v>0.1578938</v>
+        <v>0.1892889</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1669,7 +1669,7 @@
         <v>286</v>
       </c>
       <c r="D106" s="0" t="n">
-        <v>0.1597168</v>
+        <v>0.1926649</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1683,7 +1683,7 @@
         <v>287</v>
       </c>
       <c r="D107" s="0" t="n">
-        <v>0.161623</v>
+        <v>0.1960652</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1697,7 +1697,7 @@
         <v>288</v>
       </c>
       <c r="D108" s="0" t="n">
-        <v>0.1636188</v>
+        <v>0.1994882</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1711,7 +1711,7 @@
         <v>289</v>
       </c>
       <c r="D109" s="0" t="n">
-        <v>0.1657112</v>
+        <v>0.2029327</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1725,7 +1725,7 @@
         <v>290</v>
       </c>
       <c r="D110" s="0" t="n">
-        <v>0.1679074</v>
+        <v>0.2063973</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1739,7 +1739,7 @@
         <v>291</v>
       </c>
       <c r="D111" s="0" t="n">
-        <v>0.1702149</v>
+        <v>0.2098807</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1753,7 +1753,7 @@
         <v>292</v>
       </c>
       <c r="D112" s="0" t="n">
-        <v>0.1726417</v>
+        <v>0.2133814</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1767,7 +1767,7 @@
         <v>293</v>
       </c>
       <c r="D113" s="0" t="n">
-        <v>0.1751957</v>
+        <v>0.2168983</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1781,7 +1781,7 @@
         <v>294</v>
       </c>
       <c r="D114" s="0" t="n">
-        <v>0.1778855</v>
+        <v>0.2204298</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1795,7 +1795,7 @@
         <v>295</v>
       </c>
       <c r="D115" s="0" t="n">
-        <v>0.1807194</v>
+        <v>0.2239749</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1809,7 +1809,7 @@
         <v>296</v>
       </c>
       <c r="D116" s="0" t="n">
-        <v>0.1837058</v>
+        <v>0.2275321</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1823,7 +1823,7 @@
         <v>297</v>
       </c>
       <c r="D117" s="0" t="n">
-        <v>0.1868532</v>
+        <v>0.2311002</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1837,7 +1837,7 @@
         <v>298</v>
       </c>
       <c r="D118" s="0" t="n">
-        <v>0.1901697</v>
+        <v>0.2346778</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1851,7 +1851,7 @@
         <v>299</v>
       </c>
       <c r="D119" s="0" t="n">
-        <v>0.193663</v>
+        <v>0.2382639</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1865,7 +1865,7 @@
         <v>300</v>
       </c>
       <c r="D120" s="0" t="n">
-        <v>0.1973402</v>
+        <v>0.241857</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1879,7 +1879,7 @@
         <v>301</v>
       </c>
       <c r="D121" s="0" t="n">
-        <v>0.2012079</v>
+        <v>0.245456</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1893,7 +1893,7 @@
         <v>302</v>
       </c>
       <c r="D122" s="0" t="n">
-        <v>0.2052715</v>
+        <v>0.2490597</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1907,7 +1907,7 @@
         <v>303</v>
       </c>
       <c r="D123" s="0" t="n">
-        <v>0.2095352</v>
+        <v>0.2526669</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1921,7 +1921,7 @@
         <v>304</v>
       </c>
       <c r="D124" s="0" t="n">
-        <v>0.214002</v>
+        <v>0.2562762</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1935,7 +1935,7 @@
         <v>305</v>
       </c>
       <c r="D125" s="0" t="n">
-        <v>0.218673</v>
+        <v>0.2598867</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1949,7 +1949,7 @@
         <v>306</v>
       </c>
       <c r="D126" s="0" t="n">
-        <v>0.2235476</v>
+        <v>0.263497</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1963,7 +1963,7 @@
         <v>307</v>
       </c>
       <c r="D127" s="0" t="n">
-        <v>0.2286231</v>
+        <v>0.267106</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1977,7 +1977,7 @@
         <v>308</v>
       </c>
       <c r="D128" s="0" t="n">
-        <v>0.2338948</v>
+        <v>0.2707127</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1991,7 +1991,7 @@
         <v>309</v>
       </c>
       <c r="D129" s="0" t="n">
-        <v>0.2393553</v>
+        <v>0.2743157</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2005,7 +2005,7 @@
         <v>310</v>
       </c>
       <c r="D130" s="0" t="n">
-        <v>0.244995</v>
+        <v>0.2779141</v>
       </c>
     </row>
     <row r="131" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2019,7 +2019,7 @@
         <v>311</v>
       </c>
       <c r="D131" s="0" t="n">
-        <v>0.2508019</v>
+        <v>0.2815067</v>
       </c>
     </row>
     <row r="132" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2033,7 +2033,7 @@
         <v>312</v>
       </c>
       <c r="D132" s="0" t="n">
-        <v>0.2567615</v>
+        <v>0.2850924</v>
       </c>
     </row>
     <row r="133" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2047,7 +2047,7 @@
         <v>313</v>
       </c>
       <c r="D133" s="0" t="n">
-        <v>0.2628572</v>
+        <v>0.28867</v>
       </c>
     </row>
     <row r="134" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2061,7 +2061,7 @@
         <v>314</v>
       </c>
       <c r="D134" s="0" t="n">
-        <v>0.2690702</v>
+        <v>0.2922387</v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2075,7 +2075,7 @@
         <v>315</v>
       </c>
       <c r="D135" s="0" t="n">
-        <v>0.2753801</v>
+        <v>0.2957971</v>
       </c>
     </row>
     <row r="136" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2089,7 +2089,7 @@
         <v>316</v>
       </c>
       <c r="D136" s="0" t="n">
-        <v>0.2817648</v>
+        <v>0.2993444</v>
       </c>
     </row>
     <row r="137" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2103,7 +2103,7 @@
         <v>317</v>
       </c>
       <c r="D137" s="0" t="n">
-        <v>0.2882016</v>
+        <v>0.3028794</v>
       </c>
     </row>
     <row r="138" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2117,7 +2117,7 @@
         <v>318</v>
       </c>
       <c r="D138" s="0" t="n">
-        <v>0.2946666</v>
+        <v>0.3064012</v>
       </c>
     </row>
     <row r="139" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2131,7 +2131,7 @@
         <v>319</v>
       </c>
       <c r="D139" s="0" t="n">
-        <v>0.3011364</v>
+        <v>0.3099087</v>
       </c>
     </row>
     <row r="140" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2145,7 +2145,7 @@
         <v>320</v>
       </c>
       <c r="D140" s="0" t="n">
-        <v>0.3075873</v>
+        <v>0.3134009</v>
       </c>
     </row>
     <row r="141" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2159,7 +2159,7 @@
         <v>321</v>
       </c>
       <c r="D141" s="0" t="n">
-        <v>0.3139967</v>
+        <v>0.3168768</v>
       </c>
     </row>
     <row r="142" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2173,7 +2173,7 @@
         <v>322</v>
       </c>
       <c r="D142" s="0" t="n">
-        <v>0.320343</v>
+        <v>0.3203354</v>
       </c>
     </row>
     <row r="143" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2187,7 +2187,7 @@
         <v>323</v>
       </c>
       <c r="D143" s="0" t="n">
-        <v>0.3266062</v>
+        <v>0.3237758</v>
       </c>
     </row>
     <row r="144" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2201,7 +2201,7 @@
         <v>324</v>
       </c>
       <c r="D144" s="0" t="n">
-        <v>0.3327679</v>
+        <v>0.327197</v>
       </c>
     </row>
     <row r="145" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2215,7 +2215,7 @@
         <v>325</v>
       </c>
       <c r="D145" s="0" t="n">
-        <v>0.338812</v>
+        <v>0.330598</v>
       </c>
     </row>
     <row r="146" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2229,7 +2229,7 @@
         <v>326</v>
       </c>
       <c r="D146" s="0" t="n">
-        <v>0.3447243</v>
+        <v>0.333978</v>
       </c>
     </row>
     <row r="147" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2243,7 +2243,7 @@
         <v>327</v>
       </c>
       <c r="D147" s="0" t="n">
-        <v>0.3504932</v>
+        <v>0.3373359</v>
       </c>
     </row>
     <row r="148" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2257,7 +2257,7 @@
         <v>328</v>
       </c>
       <c r="D148" s="0" t="n">
-        <v>0.356109</v>
+        <v>0.3406709</v>
       </c>
     </row>
     <row r="149" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2271,7 +2271,7 @@
         <v>329</v>
       </c>
       <c r="D149" s="0" t="n">
-        <v>0.3615645</v>
+        <v>0.3439821</v>
       </c>
     </row>
     <row r="150" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2285,7 +2285,7 @@
         <v>330</v>
       </c>
       <c r="D150" s="0" t="n">
-        <v>0.3668547</v>
+        <v>0.3472686</v>
       </c>
     </row>
     <row r="151" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2299,7 +2299,7 @@
         <v>331</v>
       </c>
       <c r="D151" s="0" t="n">
-        <v>0.3719765</v>
+        <v>0.3505295</v>
       </c>
     </row>
     <row r="152" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2313,7 +2313,7 @@
         <v>332</v>
       </c>
       <c r="D152" s="0" t="n">
-        <v>0.3769286</v>
+        <v>0.3537639</v>
       </c>
     </row>
     <row r="153" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2327,7 +2327,7 @@
         <v>333</v>
       </c>
       <c r="D153" s="0" t="n">
-        <v>0.3817115</v>
+        <v>0.3569711</v>
       </c>
     </row>
     <row r="154" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2341,7 +2341,7 @@
         <v>334</v>
       </c>
       <c r="D154" s="0" t="n">
-        <v>0.386327</v>
+        <v>0.3601501</v>
       </c>
     </row>
     <row r="155" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2355,7 +2355,7 @@
         <v>335</v>
       </c>
       <c r="D155" s="0" t="n">
-        <v>0.3907783</v>
+        <v>0.3633001</v>
       </c>
     </row>
     <row r="156" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2369,7 +2369,7 @@
         <v>336</v>
       </c>
       <c r="D156" s="0" t="n">
-        <v>0.3950694</v>
+        <v>0.3664203</v>
       </c>
     </row>
     <row r="157" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2383,7 +2383,7 @@
         <v>337</v>
       </c>
       <c r="D157" s="0" t="n">
-        <v>0.3992052</v>
+        <v>0.36951</v>
       </c>
     </row>
     <row r="158" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2397,7 +2397,7 @@
         <v>338</v>
       </c>
       <c r="D158" s="0" t="n">
-        <v>0.4031914</v>
+        <v>0.3725682</v>
       </c>
     </row>
     <row r="159" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2411,7 +2411,7 @@
         <v>339</v>
       </c>
       <c r="D159" s="0" t="n">
-        <v>0.407034</v>
+        <v>0.3755943</v>
       </c>
     </row>
     <row r="160" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2425,7 +2425,7 @@
         <v>340</v>
       </c>
       <c r="D160" s="0" t="n">
-        <v>0.4107393</v>
+        <v>0.3785874</v>
       </c>
     </row>
     <row r="161" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2439,7 +2439,7 @@
         <v>341</v>
       </c>
       <c r="D161" s="0" t="n">
-        <v>0.4143137</v>
+        <v>0.3815469</v>
       </c>
     </row>
     <row r="162" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2453,7 +2453,7 @@
         <v>342</v>
       </c>
       <c r="D162" s="0" t="n">
-        <v>0.4177638</v>
+        <v>0.3844718</v>
       </c>
     </row>
     <row r="163" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2467,7 +2467,7 @@
         <v>343</v>
       </c>
       <c r="D163" s="0" t="n">
-        <v>0.4210961</v>
+        <v>0.3873617</v>
       </c>
     </row>
     <row r="164" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2481,7 +2481,7 @@
         <v>344</v>
       </c>
       <c r="D164" s="0" t="n">
-        <v>0.4243167</v>
+        <v>0.3902156</v>
       </c>
     </row>
     <row r="165" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2495,7 +2495,7 @@
         <v>345</v>
       </c>
       <c r="D165" s="0" t="n">
-        <v>0.4274317</v>
+        <v>0.3930329</v>
       </c>
     </row>
     <row r="166" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2509,7 +2509,7 @@
         <v>346</v>
       </c>
       <c r="D166" s="0" t="n">
-        <v>0.4304467</v>
+        <v>0.3958129</v>
       </c>
     </row>
     <row r="167" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2523,7 +2523,7 @@
         <v>347</v>
       </c>
       <c r="D167" s="0" t="n">
-        <v>0.4333672</v>
+        <v>0.3985549</v>
       </c>
     </row>
     <row r="168" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2537,7 +2537,7 @@
         <v>348</v>
       </c>
       <c r="D168" s="0" t="n">
-        <v>0.436198</v>
+        <v>0.4012583</v>
       </c>
     </row>
     <row r="169" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2551,7 +2551,7 @@
         <v>349</v>
       </c>
       <c r="D169" s="0" t="n">
-        <v>0.4389437</v>
+        <v>0.4039223</v>
       </c>
     </row>
     <row r="170" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2565,7 +2565,7 @@
         <v>350</v>
       </c>
       <c r="D170" s="0" t="n">
-        <v>0.4416083</v>
+        <v>0.4065464</v>
       </c>
     </row>
     <row r="171" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2579,7 +2579,7 @@
         <v>351</v>
       </c>
       <c r="D171" s="0" t="n">
-        <v>0.4441953</v>
+        <v>0.4091298</v>
       </c>
     </row>
     <row r="172" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2593,7 +2593,7 @@
         <v>352</v>
       </c>
       <c r="D172" s="0" t="n">
-        <v>0.4467081</v>
+        <v>0.411672</v>
       </c>
     </row>
     <row r="173" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2607,7 +2607,7 @@
         <v>353</v>
       </c>
       <c r="D173" s="0" t="n">
-        <v>0.4491491</v>
+        <v>0.4141723</v>
       </c>
     </row>
     <row r="174" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2621,7 +2621,7 @@
         <v>354</v>
       </c>
       <c r="D174" s="0" t="n">
-        <v>0.4515206</v>
+        <v>0.4166302</v>
       </c>
     </row>
     <row r="175" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2635,7 +2635,7 @@
         <v>355</v>
       </c>
       <c r="D175" s="0" t="n">
-        <v>0.4538244</v>
+        <v>0.419045</v>
       </c>
     </row>
     <row r="176" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2649,7 +2649,7 @@
         <v>356</v>
       </c>
       <c r="D176" s="0" t="n">
-        <v>0.4560619</v>
+        <v>0.4214162</v>
       </c>
     </row>
     <row r="177" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2663,7 +2663,7 @@
         <v>357</v>
       </c>
       <c r="D177" s="0" t="n">
-        <v>0.4582341</v>
+        <v>0.4237432</v>
       </c>
     </row>
     <row r="178" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2677,7 +2677,7 @@
         <v>358</v>
       </c>
       <c r="D178" s="0" t="n">
-        <v>0.4603416</v>
+        <v>0.4260254</v>
       </c>
     </row>
     <row r="179" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2691,7 +2691,7 @@
         <v>359</v>
       </c>
       <c r="D179" s="0" t="n">
-        <v>0.4623847</v>
+        <v>0.4282624</v>
       </c>
     </row>
     <row r="180" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2705,7 +2705,7 @@
         <v>360</v>
       </c>
       <c r="D180" s="0" t="n">
-        <v>0.4643636</v>
+        <v>0.4304535</v>
       </c>
     </row>
     <row r="181" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2719,7 +2719,7 @@
         <v>361</v>
       </c>
       <c r="D181" s="0" t="n">
-        <v>0.466278</v>
+        <v>0.4325983</v>
       </c>
     </row>
     <row r="182" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2733,7 +2733,7 @@
         <v>362</v>
       </c>
       <c r="D182" s="0" t="n">
-        <v>0.4681276</v>
+        <v>0.4346962</v>
       </c>
     </row>
     <row r="183" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2747,7 +2747,7 @@
         <v>363</v>
       </c>
       <c r="D183" s="0" t="n">
-        <v>0.4699119</v>
+        <v>0.4367467</v>
       </c>
     </row>
     <row r="184" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2761,7 +2761,7 @@
         <v>364</v>
       </c>
       <c r="D184" s="0" t="n">
-        <v>0.4716301</v>
+        <v>0.4387495</v>
       </c>
     </row>
     <row r="185" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2775,7 +2775,7 @@
         <v>365</v>
       </c>
       <c r="D185" s="0" t="n">
-        <v>0.4732816</v>
+        <v>0.4407039</v>
       </c>
     </row>
     <row r="186" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2789,7 +2789,7 @@
         <v>1</v>
       </c>
       <c r="D186" s="0" t="n">
-        <v>0.4748655</v>
+        <v>0.4426095</v>
       </c>
     </row>
     <row r="187" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2803,7 +2803,7 @@
         <v>2</v>
       </c>
       <c r="D187" s="0" t="n">
-        <v>0.4763811</v>
+        <v>0.444466</v>
       </c>
     </row>
     <row r="188" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2817,7 +2817,7 @@
         <v>3</v>
       </c>
       <c r="D188" s="0" t="n">
-        <v>0.4778275</v>
+        <v>0.4462727</v>
       </c>
     </row>
     <row r="189" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2831,7 +2831,7 @@
         <v>4</v>
       </c>
       <c r="D189" s="0" t="n">
-        <v>0.479204</v>
+        <v>0.4480295</v>
       </c>
     </row>
     <row r="190" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2845,7 +2845,7 @@
         <v>5</v>
       </c>
       <c r="D190" s="0" t="n">
-        <v>0.4805098</v>
+        <v>0.4497357</v>
       </c>
     </row>
     <row r="191" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2859,7 +2859,7 @@
         <v>6</v>
       </c>
       <c r="D191" s="0" t="n">
-        <v>0.4817443</v>
+        <v>0.451391</v>
       </c>
     </row>
     <row r="192" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2873,7 +2873,7 @@
         <v>7</v>
       </c>
       <c r="D192" s="0" t="n">
-        <v>0.4829069</v>
+        <v>0.4529951</v>
       </c>
     </row>
     <row r="193" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2887,7 +2887,7 @@
         <v>8</v>
       </c>
       <c r="D193" s="0" t="n">
-        <v>0.4839969</v>
+        <v>0.4545475</v>
       </c>
     </row>
     <row r="194" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2901,7 +2901,7 @@
         <v>9</v>
       </c>
       <c r="D194" s="0" t="n">
-        <v>0.4850141</v>
+        <v>0.4560479</v>
       </c>
     </row>
     <row r="195" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2915,7 +2915,7 @@
         <v>10</v>
       </c>
       <c r="D195" s="0" t="n">
-        <v>0.485958</v>
+        <v>0.4574959</v>
       </c>
     </row>
     <row r="196" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2929,7 +2929,7 @@
         <v>11</v>
       </c>
       <c r="D196" s="0" t="n">
-        <v>0.4868284</v>
+        <v>0.4588912</v>
       </c>
     </row>
     <row r="197" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2943,7 +2943,7 @@
         <v>12</v>
       </c>
       <c r="D197" s="0" t="n">
-        <v>0.487625</v>
+        <v>0.4602334</v>
       </c>
     </row>
     <row r="198" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2957,7 +2957,7 @@
         <v>13</v>
       </c>
       <c r="D198" s="0" t="n">
-        <v>0.4883478</v>
+        <v>0.4615223</v>
       </c>
     </row>
     <row r="199" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2971,7 +2971,7 @@
         <v>14</v>
       </c>
       <c r="D199" s="0" t="n">
-        <v>0.4889967</v>
+        <v>0.4627575</v>
       </c>
     </row>
     <row r="200" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2985,7 +2985,7 @@
         <v>15</v>
       </c>
       <c r="D200" s="0" t="n">
-        <v>0.4895718</v>
+        <v>0.4639388</v>
       </c>
     </row>
     <row r="201" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2999,7 +2999,7 @@
         <v>16</v>
       </c>
       <c r="D201" s="0" t="n">
-        <v>0.4900732</v>
+        <v>0.4650658</v>
       </c>
     </row>
     <row r="202" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3013,7 +3013,7 @@
         <v>17</v>
       </c>
       <c r="D202" s="0" t="n">
-        <v>0.490501</v>
+        <v>0.4661383</v>
       </c>
     </row>
     <row r="203" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3027,7 +3027,7 @@
         <v>18</v>
       </c>
       <c r="D203" s="0" t="n">
-        <v>0.4908556</v>
+        <v>0.4671561</v>
       </c>
     </row>
     <row r="204" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3041,7 +3041,7 @@
         <v>19</v>
       </c>
       <c r="D204" s="0" t="n">
-        <v>0.4911372</v>
+        <v>0.4681188</v>
       </c>
     </row>
     <row r="205" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3055,7 +3055,7 @@
         <v>20</v>
       </c>
       <c r="D205" s="0" t="n">
-        <v>0.4913463</v>
+        <v>0.4690263</v>
       </c>
     </row>
     <row r="206" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3069,7 +3069,7 @@
         <v>21</v>
       </c>
       <c r="D206" s="0" t="n">
-        <v>0.4914833</v>
+        <v>0.4698783</v>
       </c>
     </row>
     <row r="207" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3083,7 +3083,7 @@
         <v>22</v>
       </c>
       <c r="D207" s="0" t="n">
-        <v>0.4915487</v>
+        <v>0.4706746</v>
       </c>
     </row>
     <row r="208" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3097,7 +3097,7 @@
         <v>23</v>
       </c>
       <c r="D208" s="0" t="n">
-        <v>0.4915431</v>
+        <v>0.4714151</v>
       </c>
     </row>
     <row r="209" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3111,7 +3111,7 @@
         <v>24</v>
       </c>
       <c r="D209" s="0" t="n">
-        <v>0.4914673</v>
+        <v>0.4720994</v>
       </c>
     </row>
     <row r="210" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3125,7 +3125,7 @@
         <v>25</v>
       </c>
       <c r="D210" s="0" t="n">
-        <v>0.4913219</v>
+        <v>0.4727276</v>
       </c>
     </row>
     <row r="211" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3139,7 +3139,7 @@
         <v>26</v>
       </c>
       <c r="D211" s="0" t="n">
-        <v>0.4911079</v>
+        <v>0.4732993</v>
       </c>
     </row>
     <row r="212" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3153,7 +3153,7 @@
         <v>27</v>
       </c>
       <c r="D212" s="0" t="n">
-        <v>0.4908261</v>
+        <v>0.4738145</v>
       </c>
     </row>
     <row r="213" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3167,7 +3167,7 @@
         <v>28</v>
       </c>
       <c r="D213" s="0" t="n">
-        <v>0.4904778</v>
+        <v>0.474273</v>
       </c>
     </row>
     <row r="214" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3181,7 +3181,7 @@
         <v>29</v>
       </c>
       <c r="D214" s="0" t="n">
-        <v>0.4900641</v>
+        <v>0.4746746</v>
       </c>
     </row>
     <row r="215" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3195,7 +3195,7 @@
         <v>30</v>
       </c>
       <c r="D215" s="0" t="n">
-        <v>0.4895863</v>
+        <v>0.4750193</v>
       </c>
     </row>
     <row r="216" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3209,7 +3209,7 @@
         <v>31</v>
       </c>
       <c r="D216" s="0" t="n">
-        <v>0.489046</v>
+        <v>0.475307</v>
       </c>
     </row>
     <row r="217" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3223,7 +3223,7 @@
         <v>32</v>
       </c>
       <c r="D217" s="0" t="n">
-        <v>0.4884448</v>
+        <v>0.4755376</v>
       </c>
     </row>
     <row r="218" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3237,7 +3237,7 @@
         <v>33</v>
       </c>
       <c r="D218" s="0" t="n">
-        <v>0.4877844</v>
+        <v>0.4757109</v>
       </c>
     </row>
     <row r="219" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3251,7 +3251,7 @@
         <v>34</v>
       </c>
       <c r="D219" s="0" t="n">
-        <v>0.4870669</v>
+        <v>0.475827</v>
       </c>
     </row>
     <row r="220" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3265,7 +3265,7 @@
         <v>35</v>
       </c>
       <c r="D220" s="0" t="n">
-        <v>0.4862944</v>
+        <v>0.4758857</v>
       </c>
     </row>
     <row r="221" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3279,7 +3279,7 @@
         <v>36</v>
       </c>
       <c r="D221" s="0" t="n">
-        <v>0.4854694</v>
+        <v>0.4758871</v>
       </c>
     </row>
     <row r="222" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3293,7 +3293,7 @@
         <v>37</v>
       </c>
       <c r="D222" s="0" t="n">
-        <v>0.4845942</v>
+        <v>0.475831</v>
       </c>
     </row>
     <row r="223" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3307,7 +3307,7 @@
         <v>38</v>
       </c>
       <c r="D223" s="0" t="n">
-        <v>0.4836718</v>
+        <v>0.4757175</v>
       </c>
     </row>
     <row r="224" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3321,7 +3321,7 @@
         <v>39</v>
       </c>
       <c r="D224" s="0" t="n">
-        <v>0.482705</v>
+        <v>0.4755466</v>
       </c>
     </row>
     <row r="225" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3335,7 +3335,7 @@
         <v>40</v>
       </c>
       <c r="D225" s="0" t="n">
-        <v>0.4816969</v>
+        <v>0.4753182</v>
       </c>
     </row>
     <row r="226" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3349,7 +3349,7 @@
         <v>41</v>
       </c>
       <c r="D226" s="0" t="n">
-        <v>0.480651</v>
+        <v>0.4750324</v>
       </c>
     </row>
     <row r="227" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3363,7 +3363,7 @@
         <v>42</v>
       </c>
       <c r="D227" s="0" t="n">
-        <v>0.4795705</v>
+        <v>0.4746892</v>
       </c>
     </row>
     <row r="228" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3377,7 +3377,7 @@
         <v>43</v>
       </c>
       <c r="D228" s="0" t="n">
-        <v>0.4784592</v>
+        <v>0.4742887</v>
       </c>
     </row>
     <row r="229" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3391,7 +3391,7 @@
         <v>44</v>
       </c>
       <c r="D229" s="0" t="n">
-        <v>0.4773209</v>
+        <v>0.4738309</v>
       </c>
     </row>
     <row r="230" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3405,7 +3405,7 @@
         <v>45</v>
       </c>
       <c r="D230" s="0" t="n">
-        <v>0.4761594</v>
+        <v>0.4733158</v>
       </c>
     </row>
     <row r="231" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3419,7 +3419,7 @@
         <v>46</v>
       </c>
       <c r="D231" s="0" t="n">
-        <v>0.4749787</v>
+        <v>0.4727436</v>
       </c>
     </row>
     <row r="232" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3433,7 +3433,7 @@
         <v>47</v>
       </c>
       <c r="D232" s="0" t="n">
-        <v>0.4737828</v>
+        <v>0.4721143</v>
       </c>
     </row>
     <row r="233" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3447,7 +3447,7 @@
         <v>48</v>
       </c>
       <c r="D233" s="0" t="n">
-        <v>0.4725756</v>
+        <v>0.471428</v>
       </c>
     </row>
     <row r="234" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3461,7 +3461,7 @@
         <v>49</v>
       </c>
       <c r="D234" s="0" t="n">
-        <v>0.4713612</v>
+        <v>0.4706848</v>
       </c>
     </row>
     <row r="235" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3475,7 +3475,7 @@
         <v>50</v>
       </c>
       <c r="D235" s="0" t="n">
-        <v>0.4701435</v>
+        <v>0.4698849</v>
       </c>
     </row>
     <row r="236" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3489,7 +3489,7 @@
         <v>51</v>
       </c>
       <c r="D236" s="0" t="n">
-        <v>0.4689262</v>
+        <v>0.4690284</v>
       </c>
     </row>
     <row r="237" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3503,7 +3503,7 @@
         <v>52</v>
       </c>
       <c r="D237" s="0" t="n">
-        <v>0.467713</v>
+        <v>0.4681155</v>
       </c>
     </row>
     <row r="238" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3517,7 +3517,7 @@
         <v>53</v>
       </c>
       <c r="D238" s="0" t="n">
-        <v>0.4665073</v>
+        <v>0.4671462</v>
       </c>
     </row>
     <row r="239" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3531,7 +3531,7 @@
         <v>54</v>
       </c>
       <c r="D239" s="0" t="n">
-        <v>0.4653122</v>
+        <v>0.4661208</v>
       </c>
     </row>
     <row r="240" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3545,7 +3545,7 @@
         <v>55</v>
       </c>
       <c r="D240" s="0" t="n">
-        <v>0.4641306</v>
+        <v>0.4650394</v>
       </c>
     </row>
     <row r="241" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3559,7 +3559,7 @@
         <v>56</v>
       </c>
       <c r="D241" s="0" t="n">
-        <v>0.462965</v>
+        <v>0.4639023</v>
       </c>
     </row>
     <row r="242" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3573,7 +3573,7 @@
         <v>57</v>
       </c>
       <c r="D242" s="0" t="n">
-        <v>0.4618175</v>
+        <v>0.4627096</v>
       </c>
     </row>
     <row r="243" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3587,7 +3587,7 @@
         <v>58</v>
       </c>
       <c r="D243" s="0" t="n">
-        <v>0.4606897</v>
+        <v>0.4614616</v>
       </c>
     </row>
     <row r="244" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3601,7 +3601,7 @@
         <v>59</v>
       </c>
       <c r="D244" s="0" t="n">
-        <v>0.459583</v>
+        <v>0.4601585</v>
       </c>
     </row>
     <row r="245" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3615,7 +3615,7 @@
         <v>60</v>
       </c>
       <c r="D245" s="0" t="n">
-        <v>0.4584981</v>
+        <v>0.4588005</v>
       </c>
     </row>
     <row r="246" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3629,7 +3629,7 @@
         <v>61</v>
       </c>
       <c r="D246" s="0" t="n">
-        <v>0.4574352</v>
+        <v>0.4573879</v>
       </c>
     </row>
     <row r="247" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3643,7 +3643,7 @@
         <v>62</v>
       </c>
       <c r="D247" s="0" t="n">
-        <v>0.4563943</v>
+        <v>0.455921</v>
       </c>
     </row>
     <row r="248" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3657,7 +3657,7 @@
         <v>63</v>
       </c>
       <c r="D248" s="0" t="n">
-        <v>0.4553745</v>
+        <v>0.4544</v>
       </c>
     </row>
     <row r="249" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3671,7 +3671,7 @@
         <v>64</v>
       </c>
       <c r="D249" s="0" t="n">
-        <v>0.4543747</v>
+        <v>0.4528252</v>
       </c>
     </row>
     <row r="250" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3685,7 +3685,7 @@
         <v>65</v>
       </c>
       <c r="D250" s="0" t="n">
-        <v>0.4533931</v>
+        <v>0.451197</v>
       </c>
     </row>
     <row r="251" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3699,7 +3699,7 @@
         <v>66</v>
       </c>
       <c r="D251" s="0" t="n">
-        <v>0.4524276</v>
+        <v>0.4495155</v>
       </c>
     </row>
     <row r="252" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3713,7 +3713,7 @@
         <v>67</v>
       </c>
       <c r="D252" s="0" t="n">
-        <v>0.4514756</v>
+        <v>0.4477813</v>
       </c>
     </row>
     <row r="253" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3727,7 +3727,7 @@
         <v>68</v>
       </c>
       <c r="D253" s="0" t="n">
-        <v>0.4505341</v>
+        <v>0.4459945</v>
       </c>
     </row>
     <row r="254" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3741,7 +3741,7 @@
         <v>69</v>
       </c>
       <c r="D254" s="0" t="n">
-        <v>0.4495997</v>
+        <v>0.4441556</v>
       </c>
     </row>
     <row r="255" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3755,7 +3755,7 @@
         <v>70</v>
       </c>
       <c r="D255" s="0" t="n">
-        <v>0.4486685</v>
+        <v>0.4422649</v>
       </c>
     </row>
     <row r="256" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3769,7 +3769,7 @@
         <v>71</v>
       </c>
       <c r="D256" s="0" t="n">
-        <v>0.4477367</v>
+        <v>0.4403227</v>
       </c>
     </row>
     <row r="257" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3783,7 +3783,7 @@
         <v>72</v>
       </c>
       <c r="D257" s="0" t="n">
-        <v>0.4467997</v>
+        <v>0.4383296</v>
       </c>
     </row>
     <row r="258" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3797,7 +3797,7 @@
         <v>73</v>
       </c>
       <c r="D258" s="0" t="n">
-        <v>0.4458532</v>
+        <v>0.4362858</v>
       </c>
     </row>
     <row r="259" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3811,7 +3811,7 @@
         <v>74</v>
       </c>
       <c r="D259" s="0" t="n">
-        <v>0.4448922</v>
+        <v>0.4341917</v>
       </c>
     </row>
     <row r="260" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3825,7 +3825,7 @@
         <v>75</v>
       </c>
       <c r="D260" s="0" t="n">
-        <v>0.4439119</v>
+        <v>0.4320478</v>
       </c>
     </row>
     <row r="261" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3839,7 +3839,7 @@
         <v>76</v>
       </c>
       <c r="D261" s="0" t="n">
-        <v>0.4429074</v>
+        <v>0.4298546</v>
       </c>
     </row>
     <row r="262" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3853,7 +3853,7 @@
         <v>77</v>
       </c>
       <c r="D262" s="0" t="n">
-        <v>0.4418735</v>
+        <v>0.4276124</v>
       </c>
     </row>
     <row r="263" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3867,7 +3867,7 @@
         <v>78</v>
       </c>
       <c r="D263" s="0" t="n">
-        <v>0.4408051</v>
+        <v>0.4253217</v>
       </c>
     </row>
     <row r="264" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3881,7 +3881,7 @@
         <v>79</v>
       </c>
       <c r="D264" s="0" t="n">
-        <v>0.439697</v>
+        <v>0.4229831</v>
       </c>
     </row>
     <row r="265" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3895,7 +3895,7 @@
         <v>80</v>
       </c>
       <c r="D265" s="0" t="n">
-        <v>0.4385441</v>
+        <v>0.4205968</v>
       </c>
     </row>
     <row r="266" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3909,7 +3909,7 @@
         <v>81</v>
       </c>
       <c r="D266" s="0" t="n">
-        <v>0.4373412</v>
+        <v>0.4181636</v>
       </c>
     </row>
     <row r="267" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3923,7 +3923,7 @@
         <v>82</v>
       </c>
       <c r="D267" s="0" t="n">
-        <v>0.4360833</v>
+        <v>0.4156838</v>
       </c>
     </row>
     <row r="268" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3937,7 +3937,7 @@
         <v>83</v>
       </c>
       <c r="D268" s="0" t="n">
-        <v>0.4347653</v>
+        <v>0.4131579</v>
       </c>
     </row>
     <row r="269" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3951,7 +3951,7 @@
         <v>84</v>
       </c>
       <c r="D269" s="0" t="n">
-        <v>0.4333824</v>
+        <v>0.4105866</v>
       </c>
     </row>
     <row r="270" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3965,7 +3965,7 @@
         <v>85</v>
       </c>
       <c r="D270" s="0" t="n">
-        <v>0.4319295</v>
+        <v>0.4079703</v>
       </c>
     </row>
     <row r="271" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3979,7 +3979,7 @@
         <v>86</v>
       </c>
       <c r="D271" s="0" t="n">
-        <v>0.430402</v>
+        <v>0.4053096</v>
       </c>
     </row>
     <row r="272" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3993,7 +3993,7 @@
         <v>87</v>
       </c>
       <c r="D272" s="0" t="n">
-        <v>0.4287951</v>
+        <v>0.4026051</v>
       </c>
     </row>
     <row r="273" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4007,7 +4007,7 @@
         <v>88</v>
       </c>
       <c r="D273" s="0" t="n">
-        <v>0.4271042</v>
+        <v>0.3998572</v>
       </c>
     </row>
     <row r="274" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4021,7 +4021,7 @@
         <v>89</v>
       </c>
       <c r="D274" s="0" t="n">
-        <v>0.4253248</v>
+        <v>0.3970667</v>
       </c>
     </row>
     <row r="275" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4035,7 +4035,7 @@
         <v>90</v>
       </c>
       <c r="D275" s="0" t="n">
-        <v>0.4234525</v>
+        <v>0.3942341</v>
       </c>
     </row>
     <row r="276" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4049,7 +4049,7 @@
         <v>91</v>
       </c>
       <c r="D276" s="0" t="n">
-        <v>0.4214829</v>
+        <v>0.3913601</v>
       </c>
     </row>
     <row r="277" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4063,7 +4063,7 @@
         <v>92</v>
       </c>
       <c r="D277" s="0" t="n">
-        <v>0.419412</v>
+        <v>0.3884451</v>
       </c>
     </row>
     <row r="278" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4077,7 +4077,7 @@
         <v>93</v>
       </c>
       <c r="D278" s="0" t="n">
-        <v>0.4172356</v>
+        <v>0.38549</v>
       </c>
     </row>
     <row r="279" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4091,7 +4091,7 @@
         <v>94</v>
       </c>
       <c r="D279" s="0" t="n">
-        <v>0.4149498</v>
+        <v>0.3824953</v>
       </c>
     </row>
     <row r="280" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4105,7 +4105,7 @@
         <v>95</v>
       </c>
       <c r="D280" s="0" t="n">
-        <v>0.4125509</v>
+        <v>0.3794616</v>
       </c>
     </row>
     <row r="281" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4119,7 +4119,7 @@
         <v>96</v>
       </c>
       <c r="D281" s="0" t="n">
-        <v>0.4100353</v>
+        <v>0.3763897</v>
       </c>
     </row>
     <row r="282" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4133,7 +4133,7 @@
         <v>97</v>
       </c>
       <c r="D282" s="0" t="n">
-        <v>0.4073996</v>
+        <v>0.3732803</v>
       </c>
     </row>
     <row r="283" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4147,7 +4147,7 @@
         <v>98</v>
       </c>
       <c r="D283" s="0" t="n">
-        <v>0.4046409</v>
+        <v>0.3701339</v>
       </c>
     </row>
     <row r="284" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4161,7 +4161,7 @@
         <v>99</v>
       </c>
       <c r="D284" s="0" t="n">
-        <v>0.4017563</v>
+        <v>0.3669514</v>
       </c>
     </row>
     <row r="285" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4175,7 +4175,7 @@
         <v>100</v>
       </c>
       <c r="D285" s="0" t="n">
-        <v>0.3987435</v>
+        <v>0.3637335</v>
       </c>
     </row>
     <row r="286" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4189,7 +4189,7 @@
         <v>101</v>
       </c>
       <c r="D286" s="0" t="n">
-        <v>0.3956004</v>
+        <v>0.3604808</v>
       </c>
     </row>
     <row r="287" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4203,7 +4203,7 @@
         <v>102</v>
       </c>
       <c r="D287" s="0" t="n">
-        <v>0.3923256</v>
+        <v>0.3571941</v>
       </c>
     </row>
     <row r="288" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4217,7 +4217,7 @@
         <v>103</v>
       </c>
       <c r="D288" s="0" t="n">
-        <v>0.3889181</v>
+        <v>0.3538743</v>
       </c>
     </row>
     <row r="289" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4231,7 +4231,7 @@
         <v>104</v>
       </c>
       <c r="D289" s="0" t="n">
-        <v>0.3853778</v>
+        <v>0.3505219</v>
       </c>
     </row>
     <row r="290" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4245,7 +4245,7 @@
         <v>105</v>
       </c>
       <c r="D290" s="0" t="n">
-        <v>0.381705</v>
+        <v>0.3471379</v>
       </c>
     </row>
     <row r="291" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4259,7 +4259,7 @@
         <v>106</v>
       </c>
       <c r="D291" s="0" t="n">
-        <v>0.377901</v>
+        <v>0.3437229</v>
       </c>
     </row>
     <row r="292" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4273,7 +4273,7 @@
         <v>107</v>
       </c>
       <c r="D292" s="0" t="n">
-        <v>0.373968</v>
+        <v>0.3402779</v>
       </c>
     </row>
     <row r="293" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4287,7 +4287,7 @@
         <v>108</v>
       </c>
       <c r="D293" s="0" t="n">
-        <v>0.3699091</v>
+        <v>0.3368036</v>
       </c>
     </row>
     <row r="294" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4301,7 +4301,7 @@
         <v>109</v>
       </c>
       <c r="D294" s="0" t="n">
-        <v>0.3657284</v>
+        <v>0.3333008</v>
       </c>
     </row>
     <row r="295" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4315,7 +4315,7 @@
         <v>110</v>
       </c>
       <c r="D295" s="0" t="n">
-        <v>0.3614312</v>
+        <v>0.3297704</v>
       </c>
     </row>
     <row r="296" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4329,7 +4329,7 @@
         <v>111</v>
       </c>
       <c r="D296" s="0" t="n">
-        <v>0.3570238</v>
+        <v>0.3262133</v>
       </c>
     </row>
     <row r="297" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4343,7 +4343,7 @@
         <v>112</v>
       </c>
       <c r="D297" s="0" t="n">
-        <v>0.3525136</v>
+        <v>0.3226302</v>
       </c>
     </row>
     <row r="298" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4357,7 +4357,7 @@
         <v>113</v>
       </c>
       <c r="D298" s="0" t="n">
-        <v>0.3479094</v>
+        <v>0.319022</v>
       </c>
     </row>
     <row r="299" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4371,7 +4371,7 @@
         <v>114</v>
       </c>
       <c r="D299" s="0" t="n">
-        <v>0.3432207</v>
+        <v>0.3153897</v>
       </c>
     </row>
     <row r="300" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4385,7 +4385,7 @@
         <v>115</v>
       </c>
       <c r="D300" s="0" t="n">
-        <v>0.3384584</v>
+        <v>0.3117342</v>
       </c>
     </row>
     <row r="301" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4399,7 +4399,7 @@
         <v>116</v>
       </c>
       <c r="D301" s="0" t="n">
-        <v>0.3336341</v>
+        <v>0.3080562</v>
       </c>
     </row>
     <row r="302" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4413,7 +4413,7 @@
         <v>117</v>
       </c>
       <c r="D302" s="0" t="n">
-        <v>0.3287605</v>
+        <v>0.3043569</v>
       </c>
     </row>
     <row r="303" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4427,7 +4427,7 @@
         <v>118</v>
       </c>
       <c r="D303" s="0" t="n">
-        <v>0.3238509</v>
+        <v>0.300637</v>
       </c>
     </row>
     <row r="304" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4441,7 +4441,7 @@
         <v>119</v>
       </c>
       <c r="D304" s="0" t="n">
-        <v>0.3189191</v>
+        <v>0.2968976</v>
       </c>
     </row>
     <row r="305" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4455,7 +4455,7 @@
         <v>120</v>
       </c>
       <c r="D305" s="0" t="n">
-        <v>0.3139794</v>
+        <v>0.2931395</v>
       </c>
     </row>
     <row r="306" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4469,7 +4469,7 @@
         <v>121</v>
       </c>
       <c r="D306" s="0" t="n">
-        <v>0.3090462</v>
+        <v>0.2893639</v>
       </c>
     </row>
     <row r="307" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4483,7 +4483,7 @@
         <v>122</v>
       </c>
       <c r="D307" s="0" t="n">
-        <v>0.3041339</v>
+        <v>0.2855715</v>
       </c>
     </row>
     <row r="308" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4497,7 +4497,7 @@
         <v>123</v>
       </c>
       <c r="D308" s="0" t="n">
-        <v>0.2992567</v>
+        <v>0.2817635</v>
       </c>
     </row>
     <row r="309" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4511,7 +4511,7 @@
         <v>124</v>
       </c>
       <c r="D309" s="0" t="n">
-        <v>0.2944284</v>
+        <v>0.2779408</v>
       </c>
     </row>
     <row r="310" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4525,7 +4525,7 @@
         <v>125</v>
       </c>
       <c r="D310" s="0" t="n">
-        <v>0.2896622</v>
+        <v>0.2741045</v>
       </c>
     </row>
     <row r="311" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4539,7 +4539,7 @@
         <v>126</v>
       </c>
       <c r="D311" s="0" t="n">
-        <v>0.2849704</v>
+        <v>0.2702555</v>
       </c>
     </row>
     <row r="312" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4553,7 +4553,7 @@
         <v>127</v>
       </c>
       <c r="D312" s="0" t="n">
-        <v>0.2803644</v>
+        <v>0.2663949</v>
       </c>
     </row>
     <row r="313" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4567,7 +4567,7 @@
         <v>128</v>
       </c>
       <c r="D313" s="0" t="n">
-        <v>0.2758547</v>
+        <v>0.2625238</v>
       </c>
     </row>
     <row r="314" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4581,7 +4581,7 @@
         <v>129</v>
       </c>
       <c r="D314" s="0" t="n">
-        <v>0.2714503</v>
+        <v>0.2586432</v>
       </c>
     </row>
     <row r="315" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4595,7 +4595,7 @@
         <v>130</v>
       </c>
       <c r="D315" s="0" t="n">
-        <v>0.2671592</v>
+        <v>0.2547542</v>
       </c>
     </row>
     <row r="316" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4609,7 +4609,7 @@
         <v>131</v>
       </c>
       <c r="D316" s="0" t="n">
-        <v>0.2629879</v>
+        <v>0.2508579</v>
       </c>
     </row>
     <row r="317" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4623,7 +4623,7 @@
         <v>132</v>
       </c>
       <c r="D317" s="0" t="n">
-        <v>0.2589417</v>
+        <v>0.2469554</v>
       </c>
     </row>
     <row r="318" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4637,7 +4637,7 @@
         <v>133</v>
       </c>
       <c r="D318" s="0" t="n">
-        <v>0.2550246</v>
+        <v>0.2430478</v>
       </c>
     </row>
     <row r="319" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4651,7 +4651,7 @@
         <v>134</v>
       </c>
       <c r="D319" s="0" t="n">
-        <v>0.2512391</v>
+        <v>0.2391361</v>
       </c>
     </row>
     <row r="320" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4665,7 +4665,7 @@
         <v>135</v>
       </c>
       <c r="D320" s="0" t="n">
-        <v>0.2475867</v>
+        <v>0.2352217</v>
       </c>
     </row>
     <row r="321" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4679,7 +4679,7 @@
         <v>136</v>
       </c>
       <c r="D321" s="0" t="n">
-        <v>0.2440675</v>
+        <v>0.2313055</v>
       </c>
     </row>
     <row r="322" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4693,7 +4693,7 @@
         <v>137</v>
       </c>
       <c r="D322" s="0" t="n">
-        <v>0.2406806</v>
+        <v>0.2273887</v>
       </c>
     </row>
     <row r="323" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4707,7 +4707,7 @@
         <v>138</v>
       </c>
       <c r="D323" s="0" t="n">
-        <v>0.2374243</v>
+        <v>0.2234726</v>
       </c>
     </row>
     <row r="324" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4721,7 +4721,7 @@
         <v>139</v>
       </c>
       <c r="D324" s="0" t="n">
-        <v>0.2342956</v>
+        <v>0.2195582</v>
       </c>
     </row>
     <row r="325" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4735,7 +4735,7 @@
         <v>140</v>
       </c>
       <c r="D325" s="0" t="n">
-        <v>0.2312911</v>
+        <v>0.2156469</v>
       </c>
     </row>
     <row r="326" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4749,7 +4749,7 @@
         <v>141</v>
       </c>
       <c r="D326" s="0" t="n">
-        <v>0.2284063</v>
+        <v>0.2117397</v>
       </c>
     </row>
     <row r="327" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4763,7 +4763,7 @@
         <v>142</v>
       </c>
       <c r="D327" s="0" t="n">
-        <v>0.2256364</v>
+        <v>0.207838</v>
       </c>
     </row>
     <row r="328" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4777,7 +4777,7 @@
         <v>143</v>
       </c>
       <c r="D328" s="0" t="n">
-        <v>0.2229761</v>
+        <v>0.2039429</v>
       </c>
     </row>
     <row r="329" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4791,7 +4791,7 @@
         <v>144</v>
       </c>
       <c r="D329" s="0" t="n">
-        <v>0.2204196</v>
+        <v>0.2000557</v>
       </c>
     </row>
     <row r="330" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4805,7 +4805,7 @@
         <v>145</v>
       </c>
       <c r="D330" s="0" t="n">
-        <v>0.2179607</v>
+        <v>0.1961776</v>
       </c>
     </row>
     <row r="331" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4819,7 +4819,7 @@
         <v>146</v>
       </c>
       <c r="D331" s="0" t="n">
-        <v>0.2155932</v>
+        <v>0.1923099</v>
       </c>
     </row>
     <row r="332" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4833,7 +4833,7 @@
         <v>147</v>
       </c>
       <c r="D332" s="0" t="n">
-        <v>0.2133106</v>
+        <v>0.1884539</v>
       </c>
     </row>
     <row r="333" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4847,7 +4847,7 @@
         <v>148</v>
       </c>
       <c r="D333" s="0" t="n">
-        <v>0.2111065</v>
+        <v>0.1846108</v>
       </c>
     </row>
     <row r="334" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4861,7 +4861,7 @@
         <v>149</v>
       </c>
       <c r="D334" s="0" t="n">
-        <v>0.2089741</v>
+        <v>0.180782</v>
       </c>
     </row>
     <row r="335" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4875,7 +4875,7 @@
         <v>150</v>
       </c>
       <c r="D335" s="0" t="n">
-        <v>0.2069071</v>
+        <v>0.1769688</v>
       </c>
     </row>
     <row r="336" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4889,7 +4889,7 @@
         <v>151</v>
       </c>
       <c r="D336" s="0" t="n">
-        <v>0.204899</v>
+        <v>0.1731725</v>
       </c>
     </row>
     <row r="337" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4903,7 +4903,7 @@
         <v>152</v>
       </c>
       <c r="D337" s="0" t="n">
-        <v>0.2029436</v>
+        <v>0.1693944</v>
       </c>
     </row>
     <row r="338" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4917,7 +4917,7 @@
         <v>153</v>
       </c>
       <c r="D338" s="0" t="n">
-        <v>0.2010348</v>
+        <v>0.1656358</v>
       </c>
     </row>
     <row r="339" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4931,7 +4931,7 @@
         <v>154</v>
       </c>
       <c r="D339" s="0" t="n">
-        <v>0.1991668</v>
+        <v>0.1618983</v>
       </c>
     </row>
     <row r="340" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4945,7 +4945,7 @@
         <v>155</v>
       </c>
       <c r="D340" s="0" t="n">
-        <v>0.1973339</v>
+        <v>0.158183</v>
       </c>
     </row>
     <row r="341" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4959,7 +4959,7 @@
         <v>156</v>
       </c>
       <c r="D341" s="0" t="n">
-        <v>0.195531</v>
+        <v>0.1544914</v>
       </c>
     </row>
     <row r="342" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4973,7 +4973,7 @@
         <v>157</v>
       </c>
       <c r="D342" s="0" t="n">
-        <v>0.1937529</v>
+        <v>0.1508249</v>
       </c>
     </row>
     <row r="343" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4987,7 +4987,7 @@
         <v>158</v>
       </c>
       <c r="D343" s="0" t="n">
-        <v>0.1919952</v>
+        <v>0.1471849</v>
       </c>
     </row>
     <row r="344" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5001,7 +5001,7 @@
         <v>159</v>
       </c>
       <c r="D344" s="0" t="n">
-        <v>0.1902536</v>
+        <v>0.1435729</v>
       </c>
     </row>
     <row r="345" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5015,7 +5015,7 @@
         <v>160</v>
       </c>
       <c r="D345" s="0" t="n">
-        <v>0.1885242</v>
+        <v>0.1399901</v>
       </c>
     </row>
     <row r="346" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5029,7 +5029,7 @@
         <v>161</v>
       </c>
       <c r="D346" s="0" t="n">
-        <v>0.1868036</v>
+        <v>0.1364382</v>
       </c>
     </row>
     <row r="347" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5043,7 +5043,7 @@
         <v>162</v>
       </c>
       <c r="D347" s="0" t="n">
-        <v>0.1850889</v>
+        <v>0.1329185</v>
       </c>
     </row>
     <row r="348" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5057,7 +5057,7 @@
         <v>163</v>
       </c>
       <c r="D348" s="0" t="n">
-        <v>0.1833774</v>
+        <v>0.1294325</v>
       </c>
     </row>
     <row r="349" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5071,7 +5071,7 @@
         <v>164</v>
       </c>
       <c r="D349" s="0" t="n">
-        <v>0.1816672</v>
+        <v>0.1259817</v>
       </c>
     </row>
     <row r="350" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5085,7 +5085,7 @@
         <v>165</v>
       </c>
       <c r="D350" s="0" t="n">
-        <v>0.1799565</v>
+        <v>0.1225676</v>
       </c>
     </row>
     <row r="351" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5099,7 +5099,7 @@
         <v>166</v>
       </c>
       <c r="D351" s="0" t="n">
-        <v>0.1782442</v>
+        <v>0.1191916</v>
       </c>
     </row>
     <row r="352" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5113,7 +5113,7 @@
         <v>167</v>
       </c>
       <c r="D352" s="0" t="n">
-        <v>0.1765296</v>
+        <v>0.1158553</v>
       </c>
     </row>
     <row r="353" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5127,7 +5127,7 @@
         <v>168</v>
       </c>
       <c r="D353" s="0" t="n">
-        <v>0.1748126</v>
+        <v>0.1125603</v>
       </c>
     </row>
     <row r="354" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5141,7 +5141,7 @@
         <v>169</v>
       </c>
       <c r="D354" s="0" t="n">
-        <v>0.1730934</v>
+        <v>0.109308</v>
       </c>
     </row>
     <row r="355" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5155,7 +5155,7 @@
         <v>170</v>
       </c>
       <c r="D355" s="0" t="n">
-        <v>0.1713725</v>
+        <v>0.1061001</v>
       </c>
     </row>
     <row r="356" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5169,7 +5169,7 @@
         <v>171</v>
       </c>
       <c r="D356" s="0" t="n">
-        <v>0.1696511</v>
+        <v>0.1029379</v>
       </c>
     </row>
     <row r="357" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5183,7 +5183,7 @@
         <v>172</v>
       </c>
       <c r="D357" s="0" t="n">
-        <v>0.1679306</v>
+        <v>0.0998233</v>
       </c>
     </row>
     <row r="358" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5197,7 +5197,7 @@
         <v>173</v>
       </c>
       <c r="D358" s="0" t="n">
-        <v>0.1662129</v>
+        <v>0.0967576</v>
       </c>
     </row>
     <row r="359" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5211,7 +5211,7 @@
         <v>174</v>
       </c>
       <c r="D359" s="0" t="n">
-        <v>0.1645001</v>
+        <v>0.0937426</v>
       </c>
     </row>
     <row r="360" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5225,7 +5225,7 @@
         <v>175</v>
       </c>
       <c r="D360" s="0" t="n">
-        <v>0.1627945</v>
+        <v>0.0907799</v>
       </c>
     </row>
     <row r="361" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5239,7 +5239,7 @@
         <v>176</v>
       </c>
       <c r="D361" s="0" t="n">
-        <v>0.1610988</v>
+        <v>0.0878709</v>
       </c>
     </row>
     <row r="362" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5253,7 +5253,7 @@
         <v>177</v>
       </c>
       <c r="D362" s="0" t="n">
-        <v>0.1594158</v>
+        <v>0.0850175</v>
       </c>
     </row>
     <row r="363" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5267,7 +5267,7 @@
         <v>178</v>
       </c>
       <c r="D363" s="0" t="n">
-        <v>0.1577484</v>
+        <v>0.0822212</v>
       </c>
     </row>
     <row r="364" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5281,7 +5281,7 @@
         <v>179</v>
       </c>
       <c r="D364" s="0" t="n">
-        <v>0.1560997</v>
+        <v>0.0794837</v>
       </c>
     </row>
     <row r="365" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5295,7 +5295,7 @@
         <v>180</v>
       </c>
       <c r="D365" s="0" t="n">
-        <v>0.1544726</v>
+        <v>0.0768066</v>
       </c>
     </row>
     <row r="366" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5309,7 +5309,7 @@
         <v>181</v>
       </c>
       <c r="D366" s="0" t="n">
-        <v>0.1528702</v>
+        <v>0.0741917</v>
       </c>
     </row>
     <row r="367" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5323,7 +5323,7 @@
         <v>182</v>
       </c>
       <c r="D367" s="0" t="n">
-        <v>0.1512954</v>
+        <v>0.0716406</v>
       </c>
     </row>
   </sheetData>
@@ -5344,8 +5344,8 @@
   </sheetPr>
   <dimension ref="A1:D53"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5382,7 +5382,7 @@
         <v>26</v>
       </c>
       <c r="D2" s="0" t="n">
-        <v>0.1153899</v>
+        <v>0.0854995</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5396,7 +5396,7 @@
         <v>27</v>
       </c>
       <c r="D3" s="0" t="n">
-        <v>0.1157967</v>
+        <v>0.0854995</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5410,7 +5410,7 @@
         <v>28</v>
       </c>
       <c r="D4" s="0" t="n">
-        <v>0.1162329</v>
+        <v>0.0854995</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5424,7 +5424,7 @@
         <v>29</v>
       </c>
       <c r="D5" s="0" t="n">
-        <v>0.1166637</v>
+        <v>0.0854995</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5438,7 +5438,7 @@
         <v>30</v>
       </c>
       <c r="D6" s="0" t="n">
-        <v>0.1170294</v>
+        <v>0.0854995</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5452,7 +5452,7 @@
         <v>31</v>
       </c>
       <c r="D7" s="0" t="n">
-        <v>0.117264</v>
+        <v>0.0854995</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5466,7 +5466,7 @@
         <v>32</v>
       </c>
       <c r="D8" s="0" t="n">
-        <v>0.1173779</v>
+        <v>0.0854995</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5480,7 +5480,7 @@
         <v>33</v>
       </c>
       <c r="D9" s="0" t="n">
-        <v>0.11761</v>
+        <v>0.0855814</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5494,7 +5494,7 @@
         <v>34</v>
       </c>
       <c r="D10" s="0" t="n">
-        <v>0.1184996</v>
+        <v>0.0881084</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5508,7 +5508,7 @@
         <v>35</v>
       </c>
       <c r="D11" s="0" t="n">
-        <v>0.1206585</v>
+        <v>0.0953451</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5522,7 +5522,7 @@
         <v>36</v>
       </c>
       <c r="D12" s="0" t="n">
-        <v>0.1244003</v>
+        <v>0.1067877</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5536,7 +5536,7 @@
         <v>37</v>
       </c>
       <c r="D13" s="0" t="n">
-        <v>0.1296719</v>
+        <v>0.1218177</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5550,7 +5550,7 @@
         <v>38</v>
       </c>
       <c r="D14" s="0" t="n">
-        <v>0.1363248</v>
+        <v>0.1398448</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5564,7 +5564,7 @@
         <v>39</v>
       </c>
       <c r="D15" s="0" t="n">
-        <v>0.1444427</v>
+        <v>0.1603072</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5578,7 +5578,7 @@
         <v>40</v>
       </c>
       <c r="D16" s="0" t="n">
-        <v>0.1546067</v>
+        <v>0.1826721</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5592,7 +5592,7 @@
         <v>41</v>
       </c>
       <c r="D17" s="0" t="n">
-        <v>0.1681304</v>
+        <v>0.2064348</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5606,7 +5606,7 @@
         <v>42</v>
       </c>
       <c r="D18" s="0" t="n">
-        <v>0.187191</v>
+        <v>0.2311194</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5620,7 +5620,7 @@
         <v>43</v>
       </c>
       <c r="D19" s="0" t="n">
-        <v>0.2144086</v>
+        <v>0.2562784</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5634,7 +5634,7 @@
         <v>44</v>
       </c>
       <c r="D20" s="0" t="n">
-        <v>0.2511051</v>
+        <v>0.2814929</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5648,7 +5648,7 @@
         <v>45</v>
       </c>
       <c r="D21" s="0" t="n">
-        <v>0.2946762</v>
+        <v>0.3063726</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5662,7 +5662,7 @@
         <v>46</v>
       </c>
       <c r="D22" s="0" t="n">
-        <v>0.3385508</v>
+        <v>0.3305559</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5676,7 +5676,7 @@
         <v>47</v>
       </c>
       <c r="D23" s="0" t="n">
-        <v>0.3765916</v>
+        <v>0.3537093</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5690,7 +5690,7 @@
         <v>48</v>
       </c>
       <c r="D24" s="0" t="n">
-        <v>0.4067595</v>
+        <v>0.3755284</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5704,7 +5704,7 @@
         <v>49</v>
       </c>
       <c r="D25" s="0" t="n">
-        <v>0.4302572</v>
+        <v>0.3957369</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5718,7 +5718,7 @@
         <v>50</v>
       </c>
       <c r="D26" s="0" t="n">
-        <v>0.4490097</v>
+        <v>0.4140874</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5732,7 +5732,7 @@
         <v>51</v>
       </c>
       <c r="D27" s="0" t="n">
-        <v>0.4642345</v>
+        <v>0.4303608</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5746,7 +5746,7 @@
         <v>52</v>
       </c>
       <c r="D28" s="0" t="n">
-        <v>0.4762428</v>
+        <v>0.4443667</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5760,7 +5760,7 @@
         <v>1</v>
       </c>
       <c r="D29" s="0" t="n">
-        <v>0.4848677</v>
+        <v>0.4559431</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5774,7 +5774,7 @@
         <v>2</v>
       </c>
       <c r="D30" s="0" t="n">
-        <v>0.4899262</v>
+        <v>0.4649568</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5788,7 +5788,7 @@
         <v>3</v>
       </c>
       <c r="D31" s="0" t="n">
-        <v>0.4914026</v>
+        <v>0.4713029</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5802,7 +5802,7 @@
         <v>4</v>
       </c>
       <c r="D32" s="0" t="n">
-        <v>0.4894614</v>
+        <v>0.4749053</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5816,7 +5816,7 @@
         <v>5</v>
       </c>
       <c r="D33" s="0" t="n">
-        <v>0.4844998</v>
+        <v>0.4757162</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5830,7 +5830,7 @@
         <v>6</v>
       </c>
       <c r="D34" s="0" t="n">
-        <v>0.4772746</v>
+        <v>0.4737164</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5844,7 +5844,7 @@
         <v>7</v>
       </c>
       <c r="D35" s="0" t="n">
-        <v>0.4689341</v>
+        <v>0.4689155</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5858,7 +5858,7 @@
         <v>8</v>
       </c>
       <c r="D36" s="0" t="n">
-        <v>0.4607313</v>
+        <v>0.4613514</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5872,7 +5872,7 @@
         <v>9</v>
       </c>
       <c r="D37" s="0" t="n">
-        <v>0.4534248</v>
+        <v>0.4510906</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5886,7 +5886,7 @@
         <v>10</v>
       </c>
       <c r="D38" s="0" t="n">
-        <v>0.4467803</v>
+        <v>0.4382283</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5900,7 +5900,7 @@
         <v>11</v>
       </c>
       <c r="D39" s="0" t="n">
-        <v>0.4396074</v>
+        <v>0.422888</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5914,7 +5914,7 @@
         <v>12</v>
       </c>
       <c r="D40" s="0" t="n">
-        <v>0.4302433</v>
+        <v>0.4052219</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5928,7 +5928,7 @@
         <v>13</v>
       </c>
       <c r="D41" s="0" t="n">
-        <v>0.417017</v>
+        <v>0.3854108</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5942,7 +5942,7 @@
         <v>14</v>
       </c>
       <c r="D42" s="0" t="n">
-        <v>0.3984835</v>
+        <v>0.363664</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5956,7 +5956,7 @@
         <v>15</v>
       </c>
       <c r="D43" s="0" t="n">
-        <v>0.3737172</v>
+        <v>0.3402193</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5970,7 +5970,7 @@
         <v>16</v>
       </c>
       <c r="D44" s="0" t="n">
-        <v>0.3430744</v>
+        <v>0.3153432</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5984,7 +5984,7 @@
         <v>17</v>
       </c>
       <c r="D45" s="0" t="n">
-        <v>0.3090878</v>
+        <v>0.2893305</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5998,7 +5998,7 @@
         <v>18</v>
       </c>
       <c r="D46" s="0" t="n">
-        <v>0.2760642</v>
+        <v>0.2625049</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6012,7 +6012,7 @@
         <v>19</v>
       </c>
       <c r="D47" s="0" t="n">
-        <v>0.2478521</v>
+        <v>0.2352183</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6026,7 +6026,7 @@
         <v>20</v>
       </c>
       <c r="D48" s="0" t="n">
-        <v>0.2258551</v>
+        <v>0.2078513</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6040,7 +6040,7 @@
         <v>21</v>
       </c>
       <c r="D49" s="0" t="n">
-        <v>0.2091049</v>
+        <v>0.1808132</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6054,7 +6054,7 @@
         <v>22</v>
       </c>
       <c r="D50" s="0" t="n">
-        <v>0.1955812</v>
+        <v>0.1545416</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6068,7 +6068,7 @@
         <v>23</v>
       </c>
       <c r="D51" s="0" t="n">
-        <v>0.1833803</v>
+        <v>0.1295029</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6082,7 +6082,7 @@
         <v>24</v>
       </c>
       <c r="D52" s="0" t="n">
-        <v>0.1713718</v>
+        <v>0.1061918</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6096,7 +6096,7 @@
         <v>25</v>
       </c>
       <c r="D53" s="0" t="n">
-        <v>0.1594471</v>
+        <v>0.0851318</v>
       </c>
     </row>
   </sheetData>
@@ -6118,16 +6118,12 @@
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="16.24"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="22.74"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="5" style="0" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.53"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6155,7 +6151,7 @@
         <v>7</v>
       </c>
       <c r="D2" s="0" t="n">
-        <v>0.1172093</v>
+        <v>0.0850664</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6169,7 +6165,7 @@
         <v>8</v>
       </c>
       <c r="D3" s="0" t="n">
-        <v>0.1175635</v>
+        <v>0.0859468</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6183,7 +6179,7 @@
         <v>9</v>
       </c>
       <c r="D4" s="0" t="n">
-        <v>0.1279088</v>
+        <v>0.116274</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6197,7 +6193,7 @@
         <v>10</v>
       </c>
       <c r="D5" s="0" t="n">
-        <v>0.1699974</v>
+        <v>0.2037421</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6211,7 +6207,7 @@
         <v>11</v>
       </c>
       <c r="D6" s="0" t="n">
-        <v>0.303551</v>
+        <v>0.3110702</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6225,7 +6221,7 @@
         <v>12</v>
       </c>
       <c r="D7" s="0" t="n">
-        <v>0.438307</v>
+        <v>0.4049274</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6239,7 +6235,7 @@
         <v>1</v>
       </c>
       <c r="D8" s="0" t="n">
-        <v>0.4871666</v>
+        <v>0.462891</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6253,7 +6249,7 @@
         <v>2</v>
       </c>
       <c r="D9" s="0" t="n">
-        <v>0.4750134</v>
+        <v>0.471177</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6267,7 +6263,7 @@
         <v>3</v>
       </c>
       <c r="D10" s="0" t="n">
-        <v>0.442896</v>
+        <v>0.4300782</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6281,7 +6277,7 @@
         <v>4</v>
       </c>
       <c r="D11" s="0" t="n">
-        <v>0.3753114</v>
+        <v>0.3442967</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6295,7 +6291,7 @@
         <v>5</v>
       </c>
       <c r="D12" s="0" t="n">
-        <v>0.248905</v>
+        <v>0.231289</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6309,7 +6305,7 @@
         <v>6</v>
       </c>
       <c r="D13" s="0" t="n">
-        <v>0.1774759</v>
+        <v>0.1190387</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Made the WMA methodology even more sophisticated!
</commit_message>
<xml_diff>
--- a/DATA/collate_cultivar_data/data/binned_kcp_data.xlsx
+++ b/DATA/collate_cultivar_data/data/binned_kcp_data.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="day_frequency" sheetId="1" state="visible" r:id="rId2"/>
@@ -175,8 +175,8 @@
   </sheetPr>
   <dimension ref="A1:D367"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F17" activeCellId="0" sqref="F17"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F6" activeCellId="0" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5344,7 +5344,7 @@
   </sheetPr>
   <dimension ref="A1:D53"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Projected weekly data onto daily bins.
</commit_message>
<xml_diff>
--- a/DATA/collate_cultivar_data/data/binned_kcp_data.xlsx
+++ b/DATA/collate_cultivar_data/data/binned_kcp_data.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="day_frequency" sheetId="1" state="visible" r:id="rId2"/>
@@ -175,7 +175,7 @@
   </sheetPr>
   <dimension ref="A1:D367"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="F6" activeCellId="0" sqref="F6"/>
     </sheetView>
   </sheetViews>
@@ -5344,16 +5344,16 @@
   </sheetPr>
   <dimension ref="A1:D53"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.48"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="15.02"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="21.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="14.74"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="21.2"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="5" style="0" width="9.14"/>
   </cols>
   <sheetData>
@@ -6117,7 +6117,7 @@
   </sheetPr>
   <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Cleaning Code, Round 3.
</commit_message>
<xml_diff>
--- a/DATA/collate_cultivar_data/data/binned_kcp_data.xlsx
+++ b/DATA/collate_cultivar_data/data/binned_kcp_data.xlsx
@@ -3058,7 +3058,7 @@
         <v>4</v>
       </c>
       <c r="D189">
-        <v>0.4435496</v>
+        <v>0.4435497</v>
       </c>
     </row>
     <row r="190" spans="1:4">
@@ -3310,7 +3310,7 @@
         <v>22</v>
       </c>
       <c r="D207">
-        <v>0.4537514</v>
+        <v>0.4537515</v>
       </c>
     </row>
     <row r="208" spans="1:4">
@@ -3338,7 +3338,7 @@
         <v>24</v>
       </c>
       <c r="D209">
-        <v>0.4543518</v>
+        <v>0.4543519</v>
       </c>
     </row>
     <row r="210" spans="1:4">
@@ -3352,7 +3352,7 @@
         <v>25</v>
       </c>
       <c r="D210">
-        <v>0.4546299</v>
+        <v>0.45463</v>
       </c>
     </row>
     <row r="211" spans="1:4">
@@ -3366,7 +3366,7 @@
         <v>26</v>
       </c>
       <c r="D211">
-        <v>0.4548948</v>
+        <v>0.4548949</v>
       </c>
     </row>
     <row r="212" spans="1:4">
@@ -3380,7 +3380,7 @@
         <v>27</v>
       </c>
       <c r="D212">
-        <v>0.4551474</v>
+        <v>0.4551475</v>
       </c>
     </row>
     <row r="213" spans="1:4">
@@ -3394,7 +3394,7 @@
         <v>28</v>
       </c>
       <c r="D213">
-        <v>0.4553886</v>
+        <v>0.4553887</v>
       </c>
     </row>
     <row r="214" spans="1:4">
@@ -3408,7 +3408,7 @@
         <v>29</v>
       </c>
       <c r="D214">
-        <v>0.4556191</v>
+        <v>0.4556192</v>
       </c>
     </row>
     <row r="215" spans="1:4">
@@ -3422,7 +3422,7 @@
         <v>30</v>
       </c>
       <c r="D215">
-        <v>0.4558395</v>
+        <v>0.4558397</v>
       </c>
     </row>
     <row r="216" spans="1:4">
@@ -3436,7 +3436,7 @@
         <v>31</v>
       </c>
       <c r="D216">
-        <v>0.4560503</v>
+        <v>0.4560505</v>
       </c>
     </row>
     <row r="217" spans="1:4">
@@ -3450,7 +3450,7 @@
         <v>32</v>
       </c>
       <c r="D217">
-        <v>0.4562519</v>
+        <v>0.4562522</v>
       </c>
     </row>
     <row r="218" spans="1:4">
@@ -3464,7 +3464,7 @@
         <v>33</v>
       </c>
       <c r="D218">
-        <v>0.4564445</v>
+        <v>0.4564449</v>
       </c>
     </row>
     <row r="219" spans="1:4">
@@ -3478,7 +3478,7 @@
         <v>34</v>
       </c>
       <c r="D219">
-        <v>0.4566282</v>
+        <v>0.4566287</v>
       </c>
     </row>
     <row r="220" spans="1:4">
@@ -3492,7 +3492,7 @@
         <v>35</v>
       </c>
       <c r="D220">
-        <v>0.4568031</v>
+        <v>0.4568037</v>
       </c>
     </row>
     <row r="221" spans="1:4">
@@ -3506,7 +3506,7 @@
         <v>36</v>
       </c>
       <c r="D221">
-        <v>0.456969</v>
+        <v>0.4569697</v>
       </c>
     </row>
     <row r="222" spans="1:4">
@@ -3520,7 +3520,7 @@
         <v>37</v>
       </c>
       <c r="D222">
-        <v>0.4571256</v>
+        <v>0.4571265</v>
       </c>
     </row>
     <row r="223" spans="1:4">
@@ -3534,7 +3534,7 @@
         <v>38</v>
       </c>
       <c r="D223">
-        <v>0.4572725</v>
+        <v>0.4572737</v>
       </c>
     </row>
     <row r="224" spans="1:4">
@@ -3548,7 +3548,7 @@
         <v>39</v>
       </c>
       <c r="D224">
-        <v>0.4574093</v>
+        <v>0.4574107</v>
       </c>
     </row>
     <row r="225" spans="1:4">
@@ -3562,7 +3562,7 @@
         <v>40</v>
       </c>
       <c r="D225">
-        <v>0.4575354</v>
+        <v>0.457537</v>
       </c>
     </row>
     <row r="226" spans="1:4">
@@ -3576,7 +3576,7 @@
         <v>41</v>
       </c>
       <c r="D226">
-        <v>0.4576498</v>
+        <v>0.4576518</v>
       </c>
     </row>
     <row r="227" spans="1:4">
@@ -3590,7 +3590,7 @@
         <v>42</v>
       </c>
       <c r="D227">
-        <v>0.4577518</v>
+        <v>0.4577543</v>
       </c>
     </row>
     <row r="228" spans="1:4">
@@ -3604,7 +3604,7 @@
         <v>43</v>
       </c>
       <c r="D228">
-        <v>0.4578403</v>
+        <v>0.4578434</v>
       </c>
     </row>
     <row r="229" spans="1:4">
@@ -3618,7 +3618,7 @@
         <v>44</v>
       </c>
       <c r="D229">
-        <v>0.4579143</v>
+        <v>0.457918</v>
       </c>
     </row>
     <row r="230" spans="1:4">
@@ -3632,7 +3632,7 @@
         <v>45</v>
       </c>
       <c r="D230">
-        <v>0.4579724</v>
+        <v>0.4579769</v>
       </c>
     </row>
     <row r="231" spans="1:4">
@@ -3646,7 +3646,7 @@
         <v>46</v>
       </c>
       <c r="D231">
-        <v>0.4580133</v>
+        <v>0.4580188</v>
       </c>
     </row>
     <row r="232" spans="1:4">
@@ -3660,7 +3660,7 @@
         <v>47</v>
       </c>
       <c r="D232">
-        <v>0.4580356</v>
+        <v>0.4580422</v>
       </c>
     </row>
     <row r="233" spans="1:4">
@@ -3674,7 +3674,7 @@
         <v>48</v>
       </c>
       <c r="D233">
-        <v>0.4580377</v>
+        <v>0.4580458</v>
       </c>
     </row>
     <row r="234" spans="1:4">
@@ -3688,7 +3688,7 @@
         <v>49</v>
       </c>
       <c r="D234">
-        <v>0.458018</v>
+        <v>0.4580277</v>
       </c>
     </row>
     <row r="235" spans="1:4">
@@ -3702,7 +3702,7 @@
         <v>50</v>
       </c>
       <c r="D235">
-        <v>0.4579747</v>
+        <v>0.4579864</v>
       </c>
     </row>
     <row r="236" spans="1:4">
@@ -3716,7 +3716,7 @@
         <v>51</v>
       </c>
       <c r="D236">
-        <v>0.4579059</v>
+        <v>0.4579201</v>
       </c>
     </row>
     <row r="237" spans="1:4">
@@ -3730,7 +3730,7 @@
         <v>52</v>
       </c>
       <c r="D237">
-        <v>0.4578099</v>
+        <v>0.4578269</v>
       </c>
     </row>
     <row r="238" spans="1:4">
@@ -3744,7 +3744,7 @@
         <v>53</v>
       </c>
       <c r="D238">
-        <v>0.4576845</v>
+        <v>0.4577049</v>
       </c>
     </row>
     <row r="239" spans="1:4">
@@ -3758,7 +3758,7 @@
         <v>54</v>
       </c>
       <c r="D239">
-        <v>0.4575277</v>
+        <v>0.4575523</v>
       </c>
     </row>
     <row r="240" spans="1:4">
@@ -3772,7 +3772,7 @@
         <v>55</v>
       </c>
       <c r="D240">
-        <v>0.4573376</v>
+        <v>0.457367</v>
       </c>
     </row>
     <row r="241" spans="1:4">
@@ -3786,7 +3786,7 @@
         <v>56</v>
       </c>
       <c r="D241">
-        <v>0.4571117</v>
+        <v>0.457147</v>
       </c>
     </row>
     <row r="242" spans="1:4">
@@ -3800,7 +3800,7 @@
         <v>57</v>
       </c>
       <c r="D242">
-        <v>0.4568481</v>
+        <v>0.4568902</v>
       </c>
     </row>
     <row r="243" spans="1:4">
@@ -3814,7 +3814,7 @@
         <v>58</v>
       </c>
       <c r="D243">
-        <v>0.4565444</v>
+        <v>0.4565946</v>
       </c>
     </row>
     <row r="244" spans="1:4">
@@ -3828,7 +3828,7 @@
         <v>59</v>
       </c>
       <c r="D244">
-        <v>0.4561984</v>
+        <v>0.4562582</v>
       </c>
     </row>
     <row r="245" spans="1:4">
@@ -3842,7 +3842,7 @@
         <v>60</v>
       </c>
       <c r="D245">
-        <v>0.4558076</v>
+        <v>0.4558788</v>
       </c>
     </row>
     <row r="246" spans="1:4">
@@ -3856,7 +3856,7 @@
         <v>61</v>
       </c>
       <c r="D246">
-        <v>0.4553698</v>
+        <v>0.4554544</v>
       </c>
     </row>
     <row r="247" spans="1:4">
@@ -3870,7 +3870,7 @@
         <v>62</v>
       </c>
       <c r="D247">
-        <v>0.4548827</v>
+        <v>0.454983</v>
       </c>
     </row>
     <row r="248" spans="1:4">
@@ -3884,7 +3884,7 @@
         <v>63</v>
       </c>
       <c r="D248">
-        <v>0.4543437</v>
+        <v>0.4544625</v>
       </c>
     </row>
     <row r="249" spans="1:4">
@@ -3898,7 +3898,7 @@
         <v>64</v>
       </c>
       <c r="D249">
-        <v>0.4537504</v>
+        <v>0.453891</v>
       </c>
     </row>
     <row r="250" spans="1:4">
@@ -3912,7 +3912,7 @@
         <v>65</v>
       </c>
       <c r="D250">
-        <v>0.4531004</v>
+        <v>0.4532664</v>
       </c>
     </row>
     <row r="251" spans="1:4">
@@ -3926,7 +3926,7 @@
         <v>66</v>
       </c>
       <c r="D251">
-        <v>0.4523913</v>
+        <v>0.4525869</v>
       </c>
     </row>
     <row r="252" spans="1:4">
@@ -3940,7 +3940,7 @@
         <v>67</v>
       </c>
       <c r="D252">
-        <v>0.4516203</v>
+        <v>0.4518506</v>
       </c>
     </row>
     <row r="253" spans="1:4">
@@ -3954,7 +3954,7 @@
         <v>68</v>
       </c>
       <c r="D253">
-        <v>0.4507851</v>
+        <v>0.4510556</v>
       </c>
     </row>
     <row r="254" spans="1:4">
@@ -3968,7 +3968,7 @@
         <v>69</v>
       </c>
       <c r="D254">
-        <v>0.4498829</v>
+        <v>0.4502002</v>
       </c>
     </row>
     <row r="255" spans="1:4">
@@ -3982,7 +3982,7 @@
         <v>70</v>
       </c>
       <c r="D255">
-        <v>0.4489111</v>
+        <v>0.4492828</v>
       </c>
     </row>
     <row r="256" spans="1:4">
@@ -3996,7 +3996,7 @@
         <v>71</v>
       </c>
       <c r="D256">
-        <v>0.4478669</v>
+        <v>0.4483015</v>
       </c>
     </row>
     <row r="257" spans="1:4">
@@ -4010,7 +4010,7 @@
         <v>72</v>
       </c>
       <c r="D257">
-        <v>0.4467476</v>
+        <v>0.4472549</v>
       </c>
     </row>
     <row r="258" spans="1:4">
@@ -4024,7 +4024,7 @@
         <v>73</v>
       </c>
       <c r="D258">
-        <v>0.4455501</v>
+        <v>0.4461413</v>
       </c>
     </row>
     <row r="259" spans="1:4">
@@ -4038,7 +4038,7 @@
         <v>74</v>
       </c>
       <c r="D259">
-        <v>0.4442714</v>
+        <v>0.4449593</v>
       </c>
     </row>
     <row r="260" spans="1:4">
@@ -4052,7 +4052,7 @@
         <v>75</v>
       </c>
       <c r="D260">
-        <v>0.4429085</v>
+        <v>0.4437074</v>
       </c>
     </row>
     <row r="261" spans="1:4">
@@ -4066,7 +4066,7 @@
         <v>76</v>
       </c>
       <c r="D261">
-        <v>0.441458</v>
+        <v>0.4423843</v>
       </c>
     </row>
     <row r="262" spans="1:4">
@@ -4080,7 +4080,7 @@
         <v>77</v>
       </c>
       <c r="D262">
-        <v>0.4399164</v>
+        <v>0.4409886</v>
       </c>
     </row>
     <row r="263" spans="1:4">
@@ -4094,7 +4094,7 @@
         <v>78</v>
       </c>
       <c r="D263">
-        <v>0.4382803</v>
+        <v>0.4395192</v>
       </c>
     </row>
     <row r="264" spans="1:4">
@@ -4108,7 +4108,7 @@
         <v>79</v>
       </c>
       <c r="D264">
-        <v>0.4365457</v>
+        <v>0.4379747</v>
       </c>
     </row>
     <row r="265" spans="1:4">
@@ -4122,7 +4122,7 @@
         <v>80</v>
       </c>
       <c r="D265">
-        <v>0.4347088</v>
+        <v>0.436354</v>
       </c>
     </row>
     <row r="266" spans="1:4">
@@ -4136,7 +4136,7 @@
         <v>81</v>
       </c>
       <c r="D266">
-        <v>0.4327652</v>
+        <v>0.4346561</v>
       </c>
     </row>
     <row r="267" spans="1:4">
@@ -4150,7 +4150,7 @@
         <v>82</v>
       </c>
       <c r="D267">
-        <v>0.4307107</v>
+        <v>0.4328798</v>
       </c>
     </row>
     <row r="268" spans="1:4">
@@ -4164,7 +4164,7 @@
         <v>83</v>
       </c>
       <c r="D268">
-        <v>0.4285405</v>
+        <v>0.4310242</v>
       </c>
     </row>
     <row r="269" spans="1:4">
@@ -4178,7 +4178,7 @@
         <v>84</v>
       </c>
       <c r="D269">
-        <v>0.4262497</v>
+        <v>0.4290882</v>
       </c>
     </row>
     <row r="270" spans="1:4">
@@ -4192,7 +4192,7 @@
         <v>85</v>
       </c>
       <c r="D270">
-        <v>0.4238332</v>
+        <v>0.4270711</v>
       </c>
     </row>
     <row r="271" spans="1:4">
@@ -4206,7 +4206,7 @@
         <v>86</v>
       </c>
       <c r="D271">
-        <v>0.4212857</v>
+        <v>0.4249719</v>
       </c>
     </row>
     <row r="272" spans="1:4">
@@ -4220,7 +4220,7 @@
         <v>87</v>
       </c>
       <c r="D272">
-        <v>0.4186017</v>
+        <v>0.4227898</v>
       </c>
     </row>
     <row r="273" spans="1:4">
@@ -4234,7 +4234,7 @@
         <v>88</v>
       </c>
       <c r="D273">
-        <v>0.4157753</v>
+        <v>0.4205241</v>
       </c>
     </row>
     <row r="274" spans="1:4">
@@ -4248,7 +4248,7 @@
         <v>89</v>
       </c>
       <c r="D274">
-        <v>0.4128006</v>
+        <v>0.418174</v>
       </c>
     </row>
     <row r="275" spans="1:4">
@@ -4262,7 +4262,7 @@
         <v>90</v>
       </c>
       <c r="D275">
-        <v>0.4096716</v>
+        <v>0.4157388</v>
       </c>
     </row>
     <row r="276" spans="1:4">
@@ -4276,7 +4276,7 @@
         <v>91</v>
       </c>
       <c r="D276">
-        <v>0.4063822</v>
+        <v>0.4132181</v>
       </c>
     </row>
     <row r="277" spans="1:4">
@@ -4290,7 +4290,7 @@
         <v>92</v>
       </c>
       <c r="D277">
-        <v>0.4029264</v>
+        <v>0.4106111</v>
       </c>
     </row>
     <row r="278" spans="1:4">
@@ -4304,7 +4304,7 @@
         <v>93</v>
       </c>
       <c r="D278">
-        <v>0.3992981</v>
+        <v>0.4079175</v>
       </c>
     </row>
     <row r="279" spans="1:4">
@@ -4318,7 +4318,7 @@
         <v>94</v>
       </c>
       <c r="D279">
-        <v>0.3954915</v>
+        <v>0.4051368</v>
       </c>
     </row>
     <row r="280" spans="1:4">
@@ -4332,7 +4332,7 @@
         <v>95</v>
       </c>
       <c r="D280">
-        <v>0.3915011</v>
+        <v>0.4022686</v>
       </c>
     </row>
     <row r="281" spans="1:4">
@@ -4346,7 +4346,7 @@
         <v>96</v>
       </c>
       <c r="D281">
-        <v>0.3873219</v>
+        <v>0.3993126</v>
       </c>
     </row>
     <row r="282" spans="1:4">
@@ -4360,7 +4360,7 @@
         <v>97</v>
       </c>
       <c r="D282">
-        <v>0.3829493</v>
+        <v>0.3962687</v>
       </c>
     </row>
     <row r="283" spans="1:4">
@@ -4374,7 +4374,7 @@
         <v>98</v>
       </c>
       <c r="D283">
-        <v>0.3783798</v>
+        <v>0.3931366</v>
       </c>
     </row>
     <row r="284" spans="1:4">
@@ -4388,7 +4388,7 @@
         <v>99</v>
       </c>
       <c r="D284">
-        <v>0.3736103</v>
+        <v>0.3899162</v>
       </c>
     </row>
     <row r="285" spans="1:4">
@@ -4402,7 +4402,7 @@
         <v>100</v>
       </c>
       <c r="D285">
-        <v>0.3686394</v>
+        <v>0.3866077</v>
       </c>
     </row>
     <row r="286" spans="1:4">
@@ -4416,7 +4416,7 @@
         <v>101</v>
       </c>
       <c r="D286">
-        <v>0.3634664</v>
+        <v>0.3832111</v>
       </c>
     </row>
     <row r="287" spans="1:4">
@@ -4430,7 +4430,7 @@
         <v>102</v>
       </c>
       <c r="D287">
-        <v>0.3580927</v>
+        <v>0.3797266</v>
       </c>
     </row>
     <row r="288" spans="1:4">
@@ -4444,7 +4444,7 @@
         <v>103</v>
       </c>
       <c r="D288">
-        <v>0.3525208</v>
+        <v>0.3761545</v>
       </c>
     </row>
     <row r="289" spans="1:4">
@@ -4458,7 +4458,7 @@
         <v>104</v>
       </c>
       <c r="D289">
-        <v>0.3467553</v>
+        <v>0.3724951</v>
       </c>
     </row>
     <row r="290" spans="1:4">
@@ -4472,7 +4472,7 @@
         <v>105</v>
       </c>
       <c r="D290">
-        <v>0.3408028</v>
+        <v>0.3687491</v>
       </c>
     </row>
     <row r="291" spans="1:4">
@@ -4486,7 +4486,7 @@
         <v>106</v>
       </c>
       <c r="D291">
-        <v>0.334672</v>
+        <v>0.3649171</v>
       </c>
     </row>
     <row r="292" spans="1:4">
@@ -4500,7 +4500,7 @@
         <v>107</v>
       </c>
       <c r="D292">
-        <v>0.3283735</v>
+        <v>0.3609997</v>
       </c>
     </row>
     <row r="293" spans="1:4">
@@ -4514,7 +4514,7 @@
         <v>108</v>
       </c>
       <c r="D293">
-        <v>0.3219205</v>
+        <v>0.3569978</v>
       </c>
     </row>
     <row r="294" spans="1:4">
@@ -4528,7 +4528,7 @@
         <v>109</v>
       </c>
       <c r="D294">
-        <v>0.315328</v>
+        <v>0.3529125</v>
       </c>
     </row>
     <row r="295" spans="1:4">
@@ -4542,7 +4542,7 @@
         <v>110</v>
       </c>
       <c r="D295">
-        <v>0.3086133</v>
+        <v>0.3487448</v>
       </c>
     </row>
     <row r="296" spans="1:4">
@@ -4556,7 +4556,7 @@
         <v>111</v>
       </c>
       <c r="D296">
-        <v>0.3017956</v>
+        <v>0.3444962</v>
       </c>
     </row>
     <row r="297" spans="1:4">
@@ -4570,7 +4570,7 @@
         <v>112</v>
       </c>
       <c r="D297">
-        <v>0.294896</v>
+        <v>0.340168</v>
       </c>
     </row>
     <row r="298" spans="1:4">
@@ -4584,7 +4584,7 @@
         <v>113</v>
       </c>
       <c r="D298">
-        <v>0.2879367</v>
+        <v>0.3357618</v>
       </c>
     </row>
     <row r="299" spans="1:4">
@@ -4598,7 +4598,7 @@
         <v>114</v>
       </c>
       <c r="D299">
-        <v>0.2809415</v>
+        <v>0.3312795</v>
       </c>
     </row>
     <row r="300" spans="1:4">
@@ -4612,7 +4612,7 @@
         <v>115</v>
       </c>
       <c r="D300">
-        <v>0.2739348</v>
+        <v>0.3267231</v>
       </c>
     </row>
     <row r="301" spans="1:4">
@@ -4626,7 +4626,7 @@
         <v>116</v>
       </c>
       <c r="D301">
-        <v>0.2669416</v>
+        <v>0.3220947</v>
       </c>
     </row>
     <row r="302" spans="1:4">
@@ -4640,7 +4640,7 @@
         <v>117</v>
       </c>
       <c r="D302">
-        <v>0.2599867</v>
+        <v>0.3173969</v>
       </c>
     </row>
     <row r="303" spans="1:4">
@@ -4654,7 +4654,7 @@
         <v>118</v>
       </c>
       <c r="D303">
-        <v>0.2530949</v>
+        <v>0.3126322</v>
       </c>
     </row>
     <row r="304" spans="1:4">
@@ -4668,7 +4668,7 @@
         <v>119</v>
       </c>
       <c r="D304">
-        <v>0.2462898</v>
+        <v>0.3078037</v>
       </c>
     </row>
     <row r="305" spans="1:4">
@@ -4682,7 +4682,7 @@
         <v>120</v>
       </c>
       <c r="D305">
-        <v>0.2395943</v>
+        <v>0.3029145</v>
       </c>
     </row>
     <row r="306" spans="1:4">
@@ -4696,7 +4696,7 @@
         <v>121</v>
       </c>
       <c r="D306">
-        <v>0.2330295</v>
+        <v>0.2979681</v>
       </c>
     </row>
     <row r="307" spans="1:4">
@@ -4710,7 +4710,7 @@
         <v>122</v>
       </c>
       <c r="D307">
-        <v>0.226615</v>
+        <v>0.2929683</v>
       </c>
     </row>
     <row r="308" spans="1:4">
@@ -4724,7 +4724,7 @@
         <v>123</v>
       </c>
       <c r="D308">
-        <v>0.2203683</v>
+        <v>0.2879194</v>
       </c>
     </row>
     <row r="309" spans="1:4">
@@ -4738,7 +4738,7 @@
         <v>124</v>
       </c>
       <c r="D309">
-        <v>0.2143046</v>
+        <v>0.2828257</v>
       </c>
     </row>
     <row r="310" spans="1:4">
@@ -4752,7 +4752,7 @@
         <v>125</v>
       </c>
       <c r="D310">
-        <v>0.208437</v>
+        <v>0.2776922</v>
       </c>
     </row>
     <row r="311" spans="1:4">
@@ -4766,7 +4766,7 @@
         <v>126</v>
       </c>
       <c r="D311">
-        <v>0.2027763</v>
+        <v>0.272524</v>
       </c>
     </row>
     <row r="312" spans="1:4">
@@ -4780,7 +4780,7 @@
         <v>127</v>
       </c>
       <c r="D312">
-        <v>0.1973308</v>
+        <v>0.2673268</v>
       </c>
     </row>
     <row r="313" spans="1:4">
@@ -4794,7 +4794,7 @@
         <v>128</v>
       </c>
       <c r="D313">
-        <v>0.1921068</v>
+        <v>0.2621064</v>
       </c>
     </row>
     <row r="314" spans="1:4">
@@ -4808,7 +4808,7 @@
         <v>129</v>
       </c>
       <c r="D314">
-        <v>0.1871081</v>
+        <v>0.2568692</v>
       </c>
     </row>
     <row r="315" spans="1:4">
@@ -4822,7 +4822,7 @@
         <v>130</v>
       </c>
       <c r="D315">
-        <v>0.1823367</v>
+        <v>0.251622</v>
       </c>
     </row>
     <row r="316" spans="1:4">
@@ -4836,7 +4836,7 @@
         <v>131</v>
       </c>
       <c r="D316">
-        <v>0.1777926</v>
+        <v>0.2463716</v>
       </c>
     </row>
     <row r="317" spans="1:4">
@@ -4850,7 +4850,7 @@
         <v>132</v>
       </c>
       <c r="D317">
-        <v>0.1734744</v>
+        <v>0.2411255</v>
       </c>
     </row>
     <row r="318" spans="1:4">
@@ -4864,7 +4864,7 @@
         <v>133</v>
       </c>
       <c r="D318">
-        <v>0.1693788</v>
+        <v>0.2358913</v>
       </c>
     </row>
     <row r="319" spans="1:4">
@@ -4878,7 +4878,7 @@
         <v>134</v>
       </c>
       <c r="D319">
-        <v>0.1655014</v>
+        <v>0.2306768</v>
       </c>
     </row>
     <row r="320" spans="1:4">
@@ -4892,7 +4892,7 @@
         <v>135</v>
       </c>
       <c r="D320">
-        <v>0.1618368</v>
+        <v>0.2254902</v>
       </c>
     </row>
     <row r="321" spans="1:4">
@@ -4906,7 +4906,7 @@
         <v>136</v>
       </c>
       <c r="D321">
-        <v>0.1583787</v>
+        <v>0.2203396</v>
       </c>
     </row>
     <row r="322" spans="1:4">
@@ -4920,7 +4920,7 @@
         <v>137</v>
       </c>
       <c r="D322">
-        <v>0.1551198</v>
+        <v>0.2152333</v>
       </c>
     </row>
     <row r="323" spans="1:4">
@@ -4934,7 +4934,7 @@
         <v>138</v>
       </c>
       <c r="D323">
-        <v>0.1520526</v>
+        <v>0.2101797</v>
       </c>
     </row>
     <row r="324" spans="1:4">
@@ -4948,7 +4948,7 @@
         <v>139</v>
       </c>
       <c r="D324">
-        <v>0.1491689</v>
+        <v>0.2051871</v>
       </c>
     </row>
     <row r="325" spans="1:4">
@@ -4962,7 +4962,7 @@
         <v>140</v>
       </c>
       <c r="D325">
-        <v>0.1464606</v>
+        <v>0.2002635</v>
       </c>
     </row>
     <row r="326" spans="1:4">
@@ -4976,7 +4976,7 @@
         <v>141</v>
       </c>
       <c r="D326">
-        <v>0.143919</v>
+        <v>0.1954169</v>
       </c>
     </row>
     <row r="327" spans="1:4">
@@ -4990,7 +4990,7 @@
         <v>142</v>
       </c>
       <c r="D327">
-        <v>0.1415359</v>
+        <v>0.1906549</v>
       </c>
     </row>
     <row r="328" spans="1:4">
@@ -5004,7 +5004,7 @@
         <v>143</v>
       </c>
       <c r="D328">
-        <v>0.1393027</v>
+        <v>0.185985</v>
       </c>
     </row>
     <row r="329" spans="1:4">
@@ -5018,7 +5018,7 @@
         <v>144</v>
       </c>
       <c r="D329">
-        <v>0.1372111</v>
+        <v>0.181414</v>
       </c>
     </row>
     <row r="330" spans="1:4">
@@ -5032,7 +5032,7 @@
         <v>145</v>
       </c>
       <c r="D330">
-        <v>0.135253</v>
+        <v>0.1769483</v>
       </c>
     </row>
     <row r="331" spans="1:4">
@@ -5046,7 +5046,7 @@
         <v>146</v>
       </c>
       <c r="D331">
-        <v>0.1334205</v>
+        <v>0.1725939</v>
       </c>
     </row>
     <row r="332" spans="1:4">
@@ -5060,7 +5060,7 @@
         <v>147</v>
       </c>
       <c r="D332">
-        <v>0.1317062</v>
+        <v>0.1683561</v>
       </c>
     </row>
     <row r="333" spans="1:4">
@@ -5074,7 +5074,7 @@
         <v>148</v>
       </c>
       <c r="D333">
-        <v>0.1301025</v>
+        <v>0.1642397</v>
       </c>
     </row>
     <row r="334" spans="1:4">
@@ -5088,7 +5088,7 @@
         <v>149</v>
       </c>
       <c r="D334">
-        <v>0.1286027</v>
+        <v>0.1602486</v>
       </c>
     </row>
     <row r="335" spans="1:4">
@@ -5102,7 +5102,7 @@
         <v>150</v>
       </c>
       <c r="D335">
-        <v>0.1271999</v>
+        <v>0.1563864</v>
       </c>
     </row>
     <row r="336" spans="1:4">
@@ -5116,7 +5116,7 @@
         <v>151</v>
       </c>
       <c r="D336">
-        <v>0.125888</v>
+        <v>0.1526557</v>
       </c>
     </row>
     <row r="337" spans="1:4">
@@ -5130,7 +5130,7 @@
         <v>152</v>
       </c>
       <c r="D337">
-        <v>0.124661</v>
+        <v>0.1490586</v>
       </c>
     </row>
     <row r="338" spans="1:4">
@@ -5144,7 +5144,7 @@
         <v>153</v>
       </c>
       <c r="D338">
-        <v>0.1235132</v>
+        <v>0.1455965</v>
       </c>
     </row>
     <row r="339" spans="1:4">
@@ -5158,7 +5158,7 @@
         <v>154</v>
       </c>
       <c r="D339">
-        <v>0.1224393</v>
+        <v>0.1422702</v>
       </c>
     </row>
     <row r="340" spans="1:4">
@@ -5172,7 +5172,7 @@
         <v>155</v>
       </c>
       <c r="D340">
-        <v>0.1214343</v>
+        <v>0.1390798</v>
       </c>
     </row>
     <row r="341" spans="1:4">
@@ -5186,7 +5186,7 @@
         <v>156</v>
       </c>
       <c r="D341">
-        <v>0.1204937</v>
+        <v>0.1360248</v>
       </c>
     </row>
     <row r="342" spans="1:4">
@@ -5200,7 +5200,7 @@
         <v>157</v>
       </c>
       <c r="D342">
-        <v>0.1196129</v>
+        <v>0.1331042</v>
       </c>
     </row>
     <row r="343" spans="1:4">
@@ -5214,7 +5214,7 @@
         <v>158</v>
       </c>
       <c r="D343">
-        <v>0.118788</v>
+        <v>0.1303165</v>
       </c>
     </row>
     <row r="344" spans="1:4">
@@ -5228,7 +5228,7 @@
         <v>159</v>
       </c>
       <c r="D344">
-        <v>0.1180151</v>
+        <v>0.1276596</v>
       </c>
     </row>
     <row r="345" spans="1:4">
@@ -5242,7 +5242,7 @@
         <v>160</v>
       </c>
       <c r="D345">
-        <v>0.1172906</v>
+        <v>0.1251313</v>
       </c>
     </row>
     <row r="346" spans="1:4">
@@ -5256,7 +5256,7 @@
         <v>161</v>
       </c>
       <c r="D346">
-        <v>0.1166113</v>
+        <v>0.1227286</v>
       </c>
     </row>
     <row r="347" spans="1:4">
@@ -5270,7 +5270,7 @@
         <v>162</v>
       </c>
       <c r="D347">
-        <v>0.115974</v>
+        <v>0.1204485</v>
       </c>
     </row>
     <row r="348" spans="1:4">
@@ -5284,7 +5284,7 @@
         <v>163</v>
       </c>
       <c r="D348">
-        <v>0.1153759</v>
+        <v>0.1182875</v>
       </c>
     </row>
     <row r="349" spans="1:4">
@@ -5298,7 +5298,7 @@
         <v>164</v>
       </c>
       <c r="D349">
-        <v>0.1148143</v>
+        <v>0.1162422</v>
       </c>
     </row>
     <row r="350" spans="1:4">
@@ -5312,7 +5312,7 @@
         <v>165</v>
       </c>
       <c r="D350">
-        <v>0.1142868</v>
+        <v>0.1143086</v>
       </c>
     </row>
     <row r="351" spans="1:4">
@@ -5326,7 +5326,7 @@
         <v>166</v>
       </c>
       <c r="D351">
-        <v>0.113791</v>
+        <v>0.1124828</v>
       </c>
     </row>
     <row r="352" spans="1:4">
@@ -5340,7 +5340,7 @@
         <v>167</v>
       </c>
       <c r="D352">
-        <v>0.1133247</v>
+        <v>0.1107608</v>
       </c>
     </row>
     <row r="353" spans="1:4">
@@ -5354,7 +5354,7 @@
         <v>168</v>
       </c>
       <c r="D353">
-        <v>0.1128861</v>
+        <v>0.1091385</v>
       </c>
     </row>
     <row r="354" spans="1:4">
@@ -5368,7 +5368,7 @@
         <v>169</v>
       </c>
       <c r="D354">
-        <v>0.1124732</v>
+        <v>0.1076117</v>
       </c>
     </row>
     <row r="355" spans="1:4">
@@ -5382,7 +5382,7 @@
         <v>170</v>
       </c>
       <c r="D355">
-        <v>0.1120844</v>
+        <v>0.1061762</v>
       </c>
     </row>
     <row r="356" spans="1:4">
@@ -5396,7 +5396,7 @@
         <v>171</v>
       </c>
       <c r="D356">
-        <v>0.111718</v>
+        <v>0.104828</v>
       </c>
     </row>
     <row r="357" spans="1:4">
@@ -5410,7 +5410,7 @@
         <v>172</v>
       </c>
       <c r="D357">
-        <v>0.1113726</v>
+        <v>0.1035628</v>
       </c>
     </row>
     <row r="358" spans="1:4">
@@ -5424,7 +5424,7 @@
         <v>173</v>
       </c>
       <c r="D358">
-        <v>0.1110467</v>
+        <v>0.1023768</v>
       </c>
     </row>
     <row r="359" spans="1:4">
@@ -5438,7 +5438,7 @@
         <v>174</v>
       </c>
       <c r="D359">
-        <v>0.1107392</v>
+        <v>0.1012658</v>
       </c>
     </row>
     <row r="360" spans="1:4">
@@ -5452,7 +5452,7 @@
         <v>175</v>
       </c>
       <c r="D360">
-        <v>0.1104489</v>
+        <v>0.1002261</v>
       </c>
     </row>
     <row r="361" spans="1:4">
@@ -5466,7 +5466,7 @@
         <v>176</v>
       </c>
       <c r="D361">
-        <v>0.1101745</v>
+        <v>0.099254</v>
       </c>
     </row>
     <row r="362" spans="1:4">
@@ -5480,7 +5480,7 @@
         <v>177</v>
       </c>
       <c r="D362">
-        <v>0.1099152</v>
+        <v>0.09834569999999999</v>
       </c>
     </row>
     <row r="363" spans="1:4">
@@ -5494,7 +5494,7 @@
         <v>178</v>
       </c>
       <c r="D363">
-        <v>0.10967</v>
+        <v>0.09749770000000001</v>
       </c>
     </row>
     <row r="364" spans="1:4">
@@ -5508,7 +5508,7 @@
         <v>179</v>
       </c>
       <c r="D364">
-        <v>0.109438</v>
+        <v>0.09670670000000001</v>
       </c>
     </row>
     <row r="365" spans="1:4">
@@ -5522,7 +5522,7 @@
         <v>180</v>
       </c>
       <c r="D365">
-        <v>0.1092183</v>
+        <v>0.0959694</v>
       </c>
     </row>
     <row r="366" spans="1:4">
@@ -5536,7 +5536,7 @@
         <v>181</v>
       </c>
       <c r="D366">
-        <v>0.1090103</v>
+        <v>0.0952827</v>
       </c>
     </row>
     <row r="367" spans="1:4">
@@ -5550,7 +5550,7 @@
         <v>182</v>
       </c>
       <c r="D367">
-        <v>0.1088131</v>
+        <v>0.09464350000000001</v>
       </c>
     </row>
   </sheetData>
@@ -5997,7 +5997,7 @@
         <v>3</v>
       </c>
       <c r="D31">
-        <v>0.4540282</v>
+        <v>0.4540283</v>
       </c>
     </row>
     <row r="32" spans="1:4">
@@ -6011,7 +6011,7 @@
         <v>4</v>
       </c>
       <c r="D32">
-        <v>0.4558202</v>
+        <v>0.4558204</v>
       </c>
     </row>
     <row r="33" spans="1:4">
@@ -6025,7 +6025,7 @@
         <v>5</v>
       </c>
       <c r="D33">
-        <v>0.4571062</v>
+        <v>0.4571071</v>
       </c>
     </row>
     <row r="34" spans="1:4">
@@ -6039,7 +6039,7 @@
         <v>6</v>
       </c>
       <c r="D34">
-        <v>0.4578825</v>
+        <v>0.4578865</v>
       </c>
     </row>
     <row r="35" spans="1:4">
@@ -6053,7 +6053,7 @@
         <v>7</v>
       </c>
       <c r="D35">
-        <v>0.4578512</v>
+        <v>0.4578663</v>
       </c>
     </row>
     <row r="36" spans="1:4">
@@ -6067,7 +6067,7 @@
         <v>8</v>
       </c>
       <c r="D36">
-        <v>0.4564597</v>
+        <v>0.4565129</v>
       </c>
     </row>
     <row r="37" spans="1:4">
@@ -6081,7 +6081,7 @@
         <v>9</v>
       </c>
       <c r="D37">
-        <v>0.452982</v>
+        <v>0.4531566</v>
       </c>
     </row>
     <row r="38" spans="1:4">
@@ -6095,7 +6095,7 @@
         <v>10</v>
       </c>
       <c r="D38">
-        <v>0.4465912</v>
+        <v>0.4471211</v>
       </c>
     </row>
     <row r="39" spans="1:4">
@@ -6109,7 +6109,7 @@
         <v>11</v>
       </c>
       <c r="D39">
-        <v>0.4363407</v>
+        <v>0.4378224</v>
       </c>
     </row>
     <row r="40" spans="1:4">
@@ -6123,7 +6123,7 @@
         <v>12</v>
       </c>
       <c r="D40">
-        <v>0.4210124</v>
+        <v>0.4248062</v>
       </c>
     </row>
     <row r="41" spans="1:4">
@@ -6137,7 +6137,7 @@
         <v>13</v>
       </c>
       <c r="D41">
-        <v>0.3989418</v>
+        <v>0.4077434</v>
       </c>
     </row>
     <row r="42" spans="1:4">
@@ -6151,7 +6151,7 @@
         <v>14</v>
       </c>
       <c r="D42">
-        <v>0.368237</v>
+        <v>0.3864316</v>
       </c>
     </row>
     <row r="43" spans="1:4">
@@ -6165,7 +6165,7 @@
         <v>15</v>
       </c>
       <c r="D43">
-        <v>0.3280665</v>
+        <v>0.3608309</v>
       </c>
     </row>
     <row r="44" spans="1:4">
@@ -6179,7 +6179,7 @@
         <v>16</v>
       </c>
       <c r="D44">
-        <v>0.280919</v>
+        <v>0.3311315</v>
       </c>
     </row>
     <row r="45" spans="1:4">
@@ -6193,7 +6193,7 @@
         <v>17</v>
       </c>
       <c r="D45">
-        <v>0.2333281</v>
+        <v>0.2978617</v>
       </c>
     </row>
     <row r="46" spans="1:4">
@@ -6207,7 +6207,7 @@
         <v>18</v>
       </c>
       <c r="D46">
-        <v>0.1925555</v>
+        <v>0.2620732</v>
       </c>
     </row>
     <row r="47" spans="1:4">
@@ -6221,7 +6221,7 @@
         <v>19</v>
       </c>
       <c r="D47">
-        <v>0.1622489</v>
+        <v>0.2255623</v>
       </c>
     </row>
     <row r="48" spans="1:4">
@@ -6235,7 +6235,7 @@
         <v>20</v>
       </c>
       <c r="D48">
-        <v>0.1418359</v>
+        <v>0.1908385</v>
       </c>
     </row>
     <row r="49" spans="1:4">
@@ -6249,7 +6249,7 @@
         <v>21</v>
       </c>
       <c r="D49">
-        <v>0.1287973</v>
+        <v>0.1605056</v>
       </c>
     </row>
     <row r="50" spans="1:4">
@@ -6263,7 +6263,7 @@
         <v>22</v>
       </c>
       <c r="D50">
-        <v>0.1206138</v>
+        <v>0.1362931</v>
       </c>
     </row>
     <row r="51" spans="1:4">
@@ -6277,7 +6277,7 @@
         <v>23</v>
       </c>
       <c r="D51">
-        <v>0.1154491</v>
+        <v>0.1185185</v>
       </c>
     </row>
     <row r="52" spans="1:4">
@@ -6291,7 +6291,7 @@
         <v>24</v>
       </c>
       <c r="D52">
-        <v>0.1121294</v>
+        <v>0.1063507</v>
       </c>
     </row>
     <row r="53" spans="1:4">
@@ -6305,7 +6305,7 @@
         <v>25</v>
       </c>
       <c r="D53">
-        <v>0.1099434</v>
+        <v>0.0984665</v>
       </c>
     </row>
   </sheetData>
@@ -6346,7 +6346,7 @@
         <v>7</v>
       </c>
       <c r="D2">
-        <v>0.1103389</v>
+        <v>0.1098961</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -6444,7 +6444,7 @@
         <v>2</v>
       </c>
       <c r="D9">
-        <v>0.4573791</v>
+        <v>0.4573919</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -6458,7 +6458,7 @@
         <v>3</v>
       </c>
       <c r="D10">
-        <v>0.4393333</v>
+        <v>0.4408844</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -6472,7 +6472,7 @@
         <v>4</v>
       </c>
       <c r="D11">
-        <v>0.3320819</v>
+        <v>0.3636858</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -6486,7 +6486,7 @@
         <v>5</v>
       </c>
       <c r="D12">
-        <v>0.1660555</v>
+        <v>0.2221123</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -6500,7 +6500,7 @@
         <v>6</v>
       </c>
       <c r="D13">
-        <v>0.1146874</v>
+        <v>0.1153914</v>
       </c>
     </row>
   </sheetData>

</xml_diff>